<commit_message>
Had typo on cable number for hv gui guide
</commit_message>
<xml_diff>
--- a/Cables and Labels/CableMapping.xlsx
+++ b/Cables and Labels/CableMapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/spaubt/Desktop/CDet/Cables and Labels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{919FC3BE-C782-DD47-8AD4-BA819E48E05E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D4601D2-2887-A64E-A571-4D9D94052AE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="820" windowWidth="29080" windowHeight="16920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9600" yWindow="740" windowWidth="19800" windowHeight="16680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cdet TDC Cable Map" sheetId="4" r:id="rId1"/>
@@ -922,7 +922,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -945,19 +945,6 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -966,6 +953,23 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -977,24 +981,19 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1213,2999 +1212,2999 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C267A411-0DF7-B748-9579-92A194184DBE}">
   <dimension ref="A2:W54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="I3" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.5" style="19" customWidth="1"/>
-    <col min="2" max="3" width="13.6640625" style="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5" style="19" customWidth="1"/>
-    <col min="5" max="5" width="19.5" style="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.5" style="19" customWidth="1"/>
-    <col min="7" max="7" width="15.83203125" style="19" customWidth="1"/>
-    <col min="8" max="8" width="16.33203125" style="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.33203125" style="19" customWidth="1"/>
-    <col min="10" max="10" width="19.5" style="19" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.5" style="19" customWidth="1"/>
-    <col min="12" max="12" width="6.83203125" style="19" customWidth="1"/>
-    <col min="13" max="13" width="4.5" style="19" customWidth="1"/>
-    <col min="14" max="14" width="15.83203125" style="19" customWidth="1"/>
-    <col min="15" max="15" width="13.5" style="19" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.5" style="19" customWidth="1"/>
-    <col min="17" max="18" width="19.5" style="19" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.83203125" style="19" customWidth="1"/>
-    <col min="20" max="20" width="13.5" style="19" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.5" style="19" customWidth="1"/>
-    <col min="22" max="22" width="19.5" style="19" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.5" style="19" customWidth="1"/>
-    <col min="24" max="16384" width="10.83203125" style="19"/>
+    <col min="1" max="1" width="4.5" style="14" customWidth="1"/>
+    <col min="2" max="3" width="13.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5" style="14" customWidth="1"/>
+    <col min="5" max="5" width="19.5" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5" style="14" customWidth="1"/>
+    <col min="7" max="7" width="15.83203125" style="14" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" style="14" customWidth="1"/>
+    <col min="10" max="10" width="19.5" style="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.5" style="14" customWidth="1"/>
+    <col min="12" max="12" width="6.83203125" style="14" customWidth="1"/>
+    <col min="13" max="13" width="4.5" style="14" customWidth="1"/>
+    <col min="14" max="14" width="15.83203125" style="14" customWidth="1"/>
+    <col min="15" max="15" width="13.5" style="14" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.5" style="14" customWidth="1"/>
+    <col min="17" max="18" width="19.5" style="14" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.83203125" style="14" customWidth="1"/>
+    <col min="20" max="20" width="13.5" style="14" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5" style="14" customWidth="1"/>
+    <col min="22" max="22" width="19.5" style="14" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.5" style="14" customWidth="1"/>
+    <col min="24" max="16384" width="10.83203125" style="14"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="16" t="s">
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="16" t="s">
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="N2" s="16"/>
-      <c r="O2" s="16"/>
-      <c r="P2" s="16"/>
-      <c r="Q2" s="16"/>
-      <c r="R2" s="17"/>
-      <c r="S2" s="16" t="s">
+      <c r="N2" s="26"/>
+      <c r="O2" s="26"/>
+      <c r="P2" s="26"/>
+      <c r="Q2" s="26"/>
+      <c r="R2" s="12"/>
+      <c r="S2" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="T2" s="16"/>
-      <c r="U2" s="16"/>
-      <c r="V2" s="16"/>
-      <c r="W2" s="16"/>
+      <c r="T2" s="26"/>
+      <c r="U2" s="26"/>
+      <c r="V2" s="26"/>
+      <c r="W2" s="26"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="16" t="s">
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="N3" s="16"/>
-      <c r="O3" s="16"/>
-      <c r="P3" s="16"/>
-      <c r="Q3" s="16"/>
-      <c r="R3" s="16"/>
-      <c r="S3" s="16"/>
-      <c r="T3" s="16"/>
-      <c r="U3" s="16"/>
-      <c r="V3" s="16"/>
-      <c r="W3" s="16"/>
+      <c r="N3" s="26"/>
+      <c r="O3" s="26"/>
+      <c r="P3" s="26"/>
+      <c r="Q3" s="26"/>
+      <c r="R3" s="26"/>
+      <c r="S3" s="26"/>
+      <c r="T3" s="26"/>
+      <c r="U3" s="26"/>
+      <c r="V3" s="26"/>
+      <c r="W3" s="26"/>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A4" s="20"/>
-      <c r="B4" s="27" t="s">
+      <c r="A4" s="15"/>
+      <c r="B4" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="29" t="s">
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="G4" s="21" t="s">
+      <c r="G4" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="20"/>
-      <c r="N4" s="21" t="s">
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="O4" s="22"/>
-      <c r="P4" s="22"/>
-      <c r="Q4" s="23"/>
-      <c r="R4" s="30" t="s">
+      <c r="O4" s="24"/>
+      <c r="P4" s="24"/>
+      <c r="Q4" s="25"/>
+      <c r="R4" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="S4" s="21" t="s">
+      <c r="S4" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="T4" s="22"/>
-      <c r="U4" s="22"/>
-      <c r="V4" s="23"/>
-      <c r="W4" s="20"/>
+      <c r="T4" s="24"/>
+      <c r="U4" s="24"/>
+      <c r="V4" s="25"/>
+      <c r="W4" s="15"/>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A5" s="20"/>
-      <c r="B5" s="26" t="s">
+      <c r="A5" s="15"/>
+      <c r="B5" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="E5" s="25" t="s">
+      <c r="E5" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="F5" s="20"/>
-      <c r="G5" s="26" t="s">
+      <c r="F5" s="15"/>
+      <c r="G5" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="25" t="s">
+      <c r="H5" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="I5" s="25" t="s">
+      <c r="I5" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="J5" s="25" t="s">
+      <c r="J5" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="K5" s="20"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="20"/>
-      <c r="N5" s="26" t="s">
+      <c r="K5" s="15"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="O5" s="25" t="s">
+      <c r="O5" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="P5" s="25" t="s">
+      <c r="P5" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="Q5" s="25" t="s">
+      <c r="Q5" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="R5" s="31"/>
-      <c r="S5" s="26" t="s">
+      <c r="R5" s="20"/>
+      <c r="S5" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="T5" s="25" t="s">
+      <c r="T5" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="U5" s="25" t="s">
+      <c r="U5" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="V5" s="25" t="s">
+      <c r="V5" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="W5" s="20"/>
+      <c r="W5" s="15"/>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A6" s="20"/>
-      <c r="B6" s="26">
+      <c r="A6" s="15"/>
+      <c r="B6" s="18">
         <f t="shared" ref="B6:B17" si="0">B7+1</f>
         <v>41</v>
       </c>
-      <c r="C6" s="26">
+      <c r="C6" s="18">
         <v>14</v>
       </c>
-      <c r="D6" s="26">
+      <c r="D6" s="18">
         <v>1</v>
       </c>
-      <c r="E6" s="26" t="s">
+      <c r="E6" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="F6" s="20"/>
-      <c r="G6" s="26">
+      <c r="F6" s="15"/>
+      <c r="G6" s="18">
         <f t="shared" ref="G6:G17" si="1">G7+1</f>
         <v>83</v>
       </c>
-      <c r="H6" s="26">
+      <c r="H6" s="18">
         <v>14</v>
       </c>
-      <c r="I6" s="26">
+      <c r="I6" s="18">
         <v>1</v>
       </c>
-      <c r="J6" s="26" t="s">
+      <c r="J6" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="K6" s="20"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="20"/>
-      <c r="N6" s="26">
+      <c r="K6" s="15"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="18">
         <f t="shared" ref="N6:N17" si="2">N7+1</f>
         <v>125</v>
       </c>
-      <c r="O6" s="26">
+      <c r="O6" s="18">
         <v>14</v>
       </c>
-      <c r="P6" s="26">
+      <c r="P6" s="18">
         <v>1</v>
       </c>
-      <c r="Q6" s="26" t="s">
+      <c r="Q6" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="R6" s="31"/>
-      <c r="S6" s="26">
+      <c r="R6" s="20"/>
+      <c r="S6" s="18">
         <f t="shared" ref="S6:S17" si="3">S7+1</f>
         <v>167</v>
       </c>
-      <c r="T6" s="26">
+      <c r="T6" s="18">
         <v>14</v>
       </c>
-      <c r="U6" s="26">
+      <c r="U6" s="18">
         <v>1</v>
       </c>
-      <c r="V6" s="26" t="s">
+      <c r="V6" s="18" t="s">
         <v>193</v>
       </c>
-      <c r="W6" s="20"/>
+      <c r="W6" s="15"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A7" s="20"/>
-      <c r="B7" s="26">
+      <c r="A7" s="15"/>
+      <c r="B7" s="18">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="C7" s="26">
+      <c r="C7" s="18">
         <v>13</v>
       </c>
-      <c r="D7" s="26">
+      <c r="D7" s="18">
         <v>2</v>
       </c>
-      <c r="E7" s="26" t="s">
+      <c r="E7" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="F7" s="20"/>
-      <c r="G7" s="26">
+      <c r="F7" s="15"/>
+      <c r="G7" s="18">
         <f t="shared" si="1"/>
         <v>82</v>
       </c>
-      <c r="H7" s="26">
+      <c r="H7" s="18">
         <v>13</v>
       </c>
-      <c r="I7" s="26">
+      <c r="I7" s="18">
         <v>2</v>
       </c>
-      <c r="J7" s="26" t="s">
+      <c r="J7" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="K7" s="20"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="20"/>
-      <c r="N7" s="26">
+      <c r="K7" s="15"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="18">
         <f t="shared" si="2"/>
         <v>124</v>
       </c>
-      <c r="O7" s="26">
+      <c r="O7" s="18">
         <v>13</v>
       </c>
-      <c r="P7" s="26">
+      <c r="P7" s="18">
         <v>2</v>
       </c>
-      <c r="Q7" s="26" t="s">
+      <c r="Q7" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="R7" s="31"/>
-      <c r="S7" s="26">
+      <c r="R7" s="20"/>
+      <c r="S7" s="18">
         <f t="shared" si="3"/>
         <v>166</v>
       </c>
-      <c r="T7" s="26">
+      <c r="T7" s="18">
         <v>13</v>
       </c>
-      <c r="U7" s="26">
+      <c r="U7" s="18">
         <v>2</v>
       </c>
-      <c r="V7" s="26" t="s">
+      <c r="V7" s="18" t="s">
         <v>206</v>
       </c>
-      <c r="W7" s="20"/>
+      <c r="W7" s="15"/>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A8" s="20"/>
-      <c r="B8" s="26">
+      <c r="A8" s="15"/>
+      <c r="B8" s="18">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="C8" s="26">
+      <c r="C8" s="18">
         <v>12</v>
       </c>
-      <c r="D8" s="26">
+      <c r="D8" s="18">
         <v>3</v>
       </c>
-      <c r="E8" s="26" t="s">
+      <c r="E8" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="F8" s="20"/>
-      <c r="G8" s="26">
+      <c r="F8" s="15"/>
+      <c r="G8" s="18">
         <f t="shared" si="1"/>
         <v>81</v>
       </c>
-      <c r="H8" s="26">
+      <c r="H8" s="18">
         <v>12</v>
       </c>
-      <c r="I8" s="26">
+      <c r="I8" s="18">
         <v>3</v>
       </c>
-      <c r="J8" s="26" t="s">
+      <c r="J8" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="K8" s="20"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="20"/>
-      <c r="N8" s="26">
+      <c r="K8" s="15"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="18">
         <f t="shared" si="2"/>
         <v>123</v>
       </c>
-      <c r="O8" s="26">
+      <c r="O8" s="18">
         <v>12</v>
       </c>
-      <c r="P8" s="26">
+      <c r="P8" s="18">
         <v>3</v>
       </c>
-      <c r="Q8" s="26" t="s">
+      <c r="Q8" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="R8" s="31"/>
-      <c r="S8" s="26">
+      <c r="R8" s="20"/>
+      <c r="S8" s="18">
         <f t="shared" si="3"/>
         <v>165</v>
       </c>
-      <c r="T8" s="26">
+      <c r="T8" s="18">
         <v>12</v>
       </c>
-      <c r="U8" s="26">
+      <c r="U8" s="18">
         <v>3</v>
       </c>
-      <c r="V8" s="26" t="s">
+      <c r="V8" s="18" t="s">
         <v>180</v>
       </c>
-      <c r="W8" s="20"/>
+      <c r="W8" s="15"/>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A9" s="20"/>
-      <c r="B9" s="26">
+      <c r="A9" s="15"/>
+      <c r="B9" s="18">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="C9" s="26">
+      <c r="C9" s="18">
         <v>11</v>
       </c>
-      <c r="D9" s="26">
+      <c r="D9" s="18">
         <v>4</v>
       </c>
-      <c r="E9" s="26" t="s">
+      <c r="E9" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="F9" s="20"/>
-      <c r="G9" s="26">
+      <c r="F9" s="15"/>
+      <c r="G9" s="18">
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
-      <c r="H9" s="26">
+      <c r="H9" s="18">
         <v>11</v>
       </c>
-      <c r="I9" s="26">
+      <c r="I9" s="18">
         <v>4</v>
       </c>
-      <c r="J9" s="26" t="s">
+      <c r="J9" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="K9" s="20"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="20"/>
-      <c r="N9" s="26">
+      <c r="K9" s="15"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="18">
         <f t="shared" si="2"/>
         <v>122</v>
       </c>
-      <c r="O9" s="26">
+      <c r="O9" s="18">
         <v>11</v>
       </c>
-      <c r="P9" s="26">
+      <c r="P9" s="18">
         <v>4</v>
       </c>
-      <c r="Q9" s="26" t="s">
+      <c r="Q9" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="R9" s="31"/>
-      <c r="S9" s="26">
+      <c r="R9" s="20"/>
+      <c r="S9" s="18">
         <f t="shared" si="3"/>
         <v>164</v>
       </c>
-      <c r="T9" s="26">
+      <c r="T9" s="18">
         <v>11</v>
       </c>
-      <c r="U9" s="26">
+      <c r="U9" s="18">
         <v>4</v>
       </c>
-      <c r="V9" s="26" t="s">
+      <c r="V9" s="18" t="s">
         <v>167</v>
       </c>
-      <c r="W9" s="20"/>
+      <c r="W9" s="15"/>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A10" s="20"/>
-      <c r="B10" s="26">
+      <c r="A10" s="15"/>
+      <c r="B10" s="18">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="C10" s="26">
+      <c r="C10" s="18">
         <v>10</v>
       </c>
-      <c r="D10" s="26">
+      <c r="D10" s="18">
         <v>5</v>
       </c>
-      <c r="E10" s="26" t="s">
+      <c r="E10" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="F10" s="20"/>
-      <c r="G10" s="26">
+      <c r="F10" s="15"/>
+      <c r="G10" s="18">
         <f t="shared" si="1"/>
         <v>79</v>
       </c>
-      <c r="H10" s="26">
+      <c r="H10" s="18">
         <v>10</v>
       </c>
-      <c r="I10" s="26">
+      <c r="I10" s="18">
         <v>5</v>
       </c>
-      <c r="J10" s="26" t="s">
+      <c r="J10" s="18" t="s">
         <v>194</v>
       </c>
-      <c r="K10" s="20"/>
-      <c r="L10" s="18"/>
-      <c r="M10" s="20"/>
-      <c r="N10" s="26">
+      <c r="K10" s="15"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="18">
         <f t="shared" si="2"/>
         <v>121</v>
       </c>
-      <c r="O10" s="26">
+      <c r="O10" s="18">
         <v>10</v>
       </c>
-      <c r="P10" s="26">
+      <c r="P10" s="18">
         <v>5</v>
       </c>
-      <c r="Q10" s="26" t="s">
+      <c r="Q10" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="R10" s="31"/>
-      <c r="S10" s="26">
+      <c r="R10" s="20"/>
+      <c r="S10" s="18">
         <f t="shared" si="3"/>
         <v>163</v>
       </c>
-      <c r="T10" s="26">
+      <c r="T10" s="18">
         <v>10</v>
       </c>
-      <c r="U10" s="26">
+      <c r="U10" s="18">
         <v>5</v>
       </c>
-      <c r="V10" s="26" t="s">
+      <c r="V10" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="W10" s="20"/>
+      <c r="W10" s="15"/>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A11" s="20"/>
-      <c r="B11" s="26">
+      <c r="A11" s="15"/>
+      <c r="B11" s="18">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="C11" s="26">
+      <c r="C11" s="18">
         <v>9</v>
       </c>
-      <c r="D11" s="26">
+      <c r="D11" s="18">
         <v>6</v>
       </c>
-      <c r="E11" s="26" t="s">
+      <c r="E11" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="F11" s="20"/>
-      <c r="G11" s="26">
+      <c r="F11" s="15"/>
+      <c r="G11" s="18">
         <f t="shared" si="1"/>
         <v>78</v>
       </c>
-      <c r="H11" s="26">
+      <c r="H11" s="18">
         <v>9</v>
       </c>
-      <c r="I11" s="26">
+      <c r="I11" s="18">
         <v>6</v>
       </c>
-      <c r="J11" s="26" t="s">
+      <c r="J11" s="18" t="s">
         <v>207</v>
       </c>
-      <c r="K11" s="20"/>
-      <c r="L11" s="18"/>
-      <c r="M11" s="20"/>
-      <c r="N11" s="26">
+      <c r="K11" s="15"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="18">
         <f t="shared" si="2"/>
         <v>120</v>
       </c>
-      <c r="O11" s="26">
+      <c r="O11" s="18">
         <v>9</v>
       </c>
-      <c r="P11" s="26">
+      <c r="P11" s="18">
         <v>6</v>
       </c>
-      <c r="Q11" s="26" t="s">
+      <c r="Q11" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="R11" s="31"/>
-      <c r="S11" s="26">
+      <c r="R11" s="20"/>
+      <c r="S11" s="18">
         <f t="shared" si="3"/>
         <v>162</v>
       </c>
-      <c r="T11" s="26">
+      <c r="T11" s="18">
         <v>9</v>
       </c>
-      <c r="U11" s="26">
+      <c r="U11" s="18">
         <v>6</v>
       </c>
-      <c r="V11" s="26" t="s">
+      <c r="V11" s="18" t="s">
         <v>153</v>
       </c>
-      <c r="W11" s="20"/>
+      <c r="W11" s="15"/>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A12" s="20"/>
-      <c r="B12" s="26">
+      <c r="A12" s="15"/>
+      <c r="B12" s="18">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="C12" s="26">
+      <c r="C12" s="18">
         <v>8</v>
       </c>
-      <c r="D12" s="26">
+      <c r="D12" s="18">
         <v>7</v>
       </c>
-      <c r="E12" s="26" t="s">
+      <c r="E12" s="18" t="s">
         <v>195</v>
       </c>
-      <c r="F12" s="20"/>
-      <c r="G12" s="26">
+      <c r="F12" s="15"/>
+      <c r="G12" s="18">
         <f t="shared" si="1"/>
         <v>77</v>
       </c>
-      <c r="H12" s="26">
+      <c r="H12" s="18">
         <v>8</v>
       </c>
-      <c r="I12" s="26">
+      <c r="I12" s="18">
         <v>7</v>
       </c>
-      <c r="J12" s="26" t="s">
+      <c r="J12" s="18" t="s">
         <v>181</v>
       </c>
-      <c r="K12" s="20"/>
-      <c r="L12" s="18"/>
-      <c r="M12" s="20"/>
-      <c r="N12" s="26">
+      <c r="K12" s="15"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="18">
         <f t="shared" si="2"/>
         <v>119</v>
       </c>
-      <c r="O12" s="26">
+      <c r="O12" s="18">
         <v>8</v>
       </c>
-      <c r="P12" s="26">
+      <c r="P12" s="18">
         <v>7</v>
       </c>
-      <c r="Q12" s="26" t="s">
+      <c r="Q12" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="R12" s="31"/>
-      <c r="S12" s="26">
+      <c r="R12" s="20"/>
+      <c r="S12" s="18">
         <f t="shared" si="3"/>
         <v>161</v>
       </c>
-      <c r="T12" s="26">
+      <c r="T12" s="18">
         <v>8</v>
       </c>
-      <c r="U12" s="26">
+      <c r="U12" s="18">
         <v>7</v>
       </c>
-      <c r="V12" s="26" t="s">
+      <c r="V12" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="W12" s="20"/>
+      <c r="W12" s="15"/>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A13" s="20"/>
-      <c r="B13" s="26">
+      <c r="A13" s="15"/>
+      <c r="B13" s="18">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="C13" s="26">
+      <c r="C13" s="18">
         <v>7</v>
       </c>
-      <c r="D13" s="26">
+      <c r="D13" s="18">
         <v>8</v>
       </c>
-      <c r="E13" s="26" t="s">
+      <c r="E13" s="18" t="s">
         <v>208</v>
       </c>
-      <c r="F13" s="20"/>
-      <c r="G13" s="26">
+      <c r="F13" s="15"/>
+      <c r="G13" s="18">
         <f t="shared" si="1"/>
         <v>76</v>
       </c>
-      <c r="H13" s="26">
+      <c r="H13" s="18">
         <v>7</v>
       </c>
-      <c r="I13" s="26">
+      <c r="I13" s="18">
         <v>8</v>
       </c>
-      <c r="J13" s="26" t="s">
+      <c r="J13" s="18" t="s">
         <v>168</v>
       </c>
-      <c r="K13" s="20"/>
-      <c r="L13" s="18"/>
-      <c r="M13" s="20"/>
-      <c r="N13" s="26">
+      <c r="K13" s="15"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="18">
         <f t="shared" si="2"/>
         <v>118</v>
       </c>
-      <c r="O13" s="26">
+      <c r="O13" s="18">
         <v>7</v>
       </c>
-      <c r="P13" s="26">
+      <c r="P13" s="18">
         <v>8</v>
       </c>
-      <c r="Q13" s="26" t="s">
+      <c r="Q13" s="18" t="s">
         <v>154</v>
       </c>
-      <c r="R13" s="31"/>
-      <c r="S13" s="26">
+      <c r="R13" s="20"/>
+      <c r="S13" s="18">
         <f t="shared" si="3"/>
         <v>160</v>
       </c>
-      <c r="T13" s="26">
+      <c r="T13" s="18">
         <v>7</v>
       </c>
-      <c r="U13" s="26">
+      <c r="U13" s="18">
         <v>8</v>
       </c>
-      <c r="V13" s="26" t="s">
+      <c r="V13" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="W13" s="20"/>
+      <c r="W13" s="15"/>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A14" s="20"/>
-      <c r="B14" s="26">
+      <c r="A14" s="15"/>
+      <c r="B14" s="18">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="C14" s="26">
+      <c r="C14" s="18">
         <v>6</v>
       </c>
-      <c r="D14" s="26">
+      <c r="D14" s="18">
         <v>9</v>
       </c>
-      <c r="E14" s="26" t="s">
+      <c r="E14" s="18" t="s">
         <v>182</v>
       </c>
-      <c r="F14" s="20"/>
-      <c r="G14" s="26">
+      <c r="F14" s="15"/>
+      <c r="G14" s="18">
         <f t="shared" si="1"/>
         <v>75</v>
       </c>
-      <c r="H14" s="26">
+      <c r="H14" s="18">
         <v>6</v>
       </c>
-      <c r="I14" s="26">
+      <c r="I14" s="18">
         <v>9</v>
       </c>
-      <c r="J14" s="26" t="s">
+      <c r="J14" s="18" t="s">
         <v>141</v>
       </c>
-      <c r="K14" s="20"/>
-      <c r="L14" s="18"/>
-      <c r="M14" s="20"/>
-      <c r="N14" s="26">
+      <c r="K14" s="15"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="18">
         <f t="shared" si="2"/>
         <v>117</v>
       </c>
-      <c r="O14" s="26">
+      <c r="O14" s="18">
         <v>6</v>
       </c>
-      <c r="P14" s="26">
+      <c r="P14" s="18">
         <v>9</v>
       </c>
-      <c r="Q14" s="26" t="s">
+      <c r="Q14" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="R14" s="31"/>
-      <c r="S14" s="26">
+      <c r="R14" s="20"/>
+      <c r="S14" s="18">
         <f t="shared" si="3"/>
         <v>159</v>
       </c>
-      <c r="T14" s="26">
+      <c r="T14" s="18">
         <v>6</v>
       </c>
-      <c r="U14" s="26">
+      <c r="U14" s="18">
         <v>9</v>
       </c>
-      <c r="V14" s="26" t="s">
+      <c r="V14" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="W14" s="20"/>
+      <c r="W14" s="15"/>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A15" s="20"/>
-      <c r="B15" s="26">
+      <c r="A15" s="15"/>
+      <c r="B15" s="18">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="C15" s="26">
+      <c r="C15" s="18">
         <v>5</v>
       </c>
-      <c r="D15" s="26">
+      <c r="D15" s="18">
         <v>10</v>
       </c>
-      <c r="E15" s="26" t="s">
+      <c r="E15" s="18" t="s">
         <v>169</v>
       </c>
-      <c r="F15" s="20"/>
-      <c r="G15" s="26">
+      <c r="F15" s="15"/>
+      <c r="G15" s="18">
         <f t="shared" si="1"/>
         <v>74</v>
       </c>
-      <c r="H15" s="26">
+      <c r="H15" s="18">
         <v>5</v>
       </c>
-      <c r="I15" s="26">
+      <c r="I15" s="18">
         <v>10</v>
       </c>
-      <c r="J15" s="26" t="s">
+      <c r="J15" s="18" t="s">
         <v>155</v>
       </c>
-      <c r="K15" s="20"/>
-      <c r="L15" s="18"/>
-      <c r="M15" s="20"/>
-      <c r="N15" s="26">
+      <c r="K15" s="15"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="15"/>
+      <c r="N15" s="18">
         <f t="shared" si="2"/>
         <v>116</v>
       </c>
-      <c r="O15" s="26">
+      <c r="O15" s="18">
         <v>5</v>
       </c>
-      <c r="P15" s="26">
+      <c r="P15" s="18">
         <v>10</v>
       </c>
-      <c r="Q15" s="26" t="s">
+      <c r="Q15" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="R15" s="31"/>
-      <c r="S15" s="26">
+      <c r="R15" s="20"/>
+      <c r="S15" s="18">
         <f t="shared" si="3"/>
         <v>158</v>
       </c>
-      <c r="T15" s="26">
+      <c r="T15" s="18">
         <v>5</v>
       </c>
-      <c r="U15" s="26">
+      <c r="U15" s="18">
         <v>10</v>
       </c>
-      <c r="V15" s="26" t="s">
+      <c r="V15" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="W15" s="20"/>
+      <c r="W15" s="15"/>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A16" s="20"/>
-      <c r="B16" s="26">
+      <c r="A16" s="15"/>
+      <c r="B16" s="18">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="C16" s="26">
+      <c r="C16" s="18">
         <v>4</v>
       </c>
-      <c r="D16" s="26">
+      <c r="D16" s="18">
         <v>11</v>
       </c>
-      <c r="E16" s="26" t="s">
+      <c r="E16" s="18" t="s">
         <v>142</v>
       </c>
-      <c r="F16" s="20"/>
-      <c r="G16" s="26">
+      <c r="F16" s="15"/>
+      <c r="G16" s="18">
         <f t="shared" si="1"/>
         <v>73</v>
       </c>
-      <c r="H16" s="26">
+      <c r="H16" s="18">
         <v>4</v>
       </c>
-      <c r="I16" s="26">
+      <c r="I16" s="18">
         <v>11</v>
       </c>
-      <c r="J16" s="26" t="s">
+      <c r="J16" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="K16" s="20"/>
-      <c r="L16" s="18"/>
-      <c r="M16" s="20"/>
-      <c r="N16" s="26">
+      <c r="K16" s="15"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="15"/>
+      <c r="N16" s="18">
         <f t="shared" si="2"/>
         <v>115</v>
       </c>
-      <c r="O16" s="26">
+      <c r="O16" s="18">
         <v>4</v>
       </c>
-      <c r="P16" s="26">
+      <c r="P16" s="18">
         <v>11</v>
       </c>
-      <c r="Q16" s="26" t="s">
+      <c r="Q16" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="R16" s="31"/>
-      <c r="S16" s="26">
+      <c r="R16" s="20"/>
+      <c r="S16" s="18">
         <f t="shared" si="3"/>
         <v>157</v>
       </c>
-      <c r="T16" s="26">
+      <c r="T16" s="18">
         <v>4</v>
       </c>
-      <c r="U16" s="26">
+      <c r="U16" s="18">
         <v>11</v>
       </c>
-      <c r="V16" s="26" t="s">
+      <c r="V16" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="W16" s="20"/>
+      <c r="W16" s="15"/>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A17" s="20"/>
-      <c r="B17" s="26">
+      <c r="A17" s="15"/>
+      <c r="B17" s="18">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="C17" s="26">
+      <c r="C17" s="18">
         <v>3</v>
       </c>
-      <c r="D17" s="26">
+      <c r="D17" s="18">
         <v>12</v>
       </c>
-      <c r="E17" s="26" t="s">
+      <c r="E17" s="18" t="s">
         <v>156</v>
       </c>
-      <c r="F17" s="20"/>
-      <c r="G17" s="26">
+      <c r="F17" s="15"/>
+      <c r="G17" s="18">
         <f t="shared" si="1"/>
         <v>72</v>
       </c>
-      <c r="H17" s="26">
+      <c r="H17" s="18">
         <v>3</v>
       </c>
-      <c r="I17" s="26">
+      <c r="I17" s="18">
         <v>12</v>
       </c>
-      <c r="J17" s="26" t="s">
+      <c r="J17" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="K17" s="20"/>
-      <c r="L17" s="18"/>
-      <c r="M17" s="20"/>
-      <c r="N17" s="26">
+      <c r="K17" s="15"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="15"/>
+      <c r="N17" s="18">
         <f t="shared" si="2"/>
         <v>114</v>
       </c>
-      <c r="O17" s="26">
+      <c r="O17" s="18">
         <v>3</v>
       </c>
-      <c r="P17" s="26">
+      <c r="P17" s="18">
         <v>12</v>
       </c>
-      <c r="Q17" s="26" t="s">
+      <c r="Q17" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="R17" s="31"/>
-      <c r="S17" s="26">
+      <c r="R17" s="20"/>
+      <c r="S17" s="18">
         <f t="shared" si="3"/>
         <v>156</v>
       </c>
-      <c r="T17" s="26">
+      <c r="T17" s="18">
         <v>3</v>
       </c>
-      <c r="U17" s="26">
+      <c r="U17" s="18">
         <v>12</v>
       </c>
-      <c r="V17" s="26" t="s">
+      <c r="V17" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="W17" s="20"/>
+      <c r="W17" s="15"/>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A18" s="20"/>
-      <c r="B18" s="26">
+      <c r="A18" s="15"/>
+      <c r="B18" s="18">
         <f>B19+1</f>
         <v>29</v>
       </c>
-      <c r="C18" s="26">
+      <c r="C18" s="18">
         <v>2</v>
       </c>
-      <c r="D18" s="26">
+      <c r="D18" s="18">
         <v>13</v>
       </c>
-      <c r="E18" s="26" t="s">
+      <c r="E18" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="F18" s="20"/>
-      <c r="G18" s="26">
+      <c r="F18" s="15"/>
+      <c r="G18" s="18">
         <f>G19+1</f>
         <v>71</v>
       </c>
-      <c r="H18" s="26">
+      <c r="H18" s="18">
         <v>2</v>
       </c>
-      <c r="I18" s="26">
+      <c r="I18" s="18">
         <v>13</v>
       </c>
-      <c r="J18" s="26" t="s">
+      <c r="J18" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="K18" s="20"/>
-      <c r="L18" s="18"/>
-      <c r="M18" s="20"/>
-      <c r="N18" s="26">
+      <c r="K18" s="15"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="15"/>
+      <c r="N18" s="18">
         <f>N19+1</f>
         <v>113</v>
       </c>
-      <c r="O18" s="26">
+      <c r="O18" s="18">
         <v>2</v>
       </c>
-      <c r="P18" s="26">
+      <c r="P18" s="18">
         <v>13</v>
       </c>
-      <c r="Q18" s="26" t="s">
+      <c r="Q18" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="R18" s="31"/>
-      <c r="S18" s="26">
+      <c r="R18" s="20"/>
+      <c r="S18" s="18">
         <f>S19+1</f>
         <v>155</v>
       </c>
-      <c r="T18" s="26">
+      <c r="T18" s="18">
         <v>2</v>
       </c>
-      <c r="U18" s="26">
+      <c r="U18" s="18">
         <v>13</v>
       </c>
-      <c r="V18" s="26" t="s">
+      <c r="V18" s="18" t="s">
         <v>196</v>
       </c>
-      <c r="W18" s="20"/>
+      <c r="W18" s="15"/>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A19" s="20"/>
-      <c r="B19" s="26">
+      <c r="A19" s="15"/>
+      <c r="B19" s="18">
         <f>B23+1</f>
         <v>28</v>
       </c>
-      <c r="C19" s="26">
+      <c r="C19" s="18">
         <v>1</v>
       </c>
-      <c r="D19" s="26">
+      <c r="D19" s="18">
         <v>14</v>
       </c>
-      <c r="E19" s="26" t="s">
+      <c r="E19" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="F19" s="20"/>
-      <c r="G19" s="26">
+      <c r="F19" s="15"/>
+      <c r="G19" s="18">
         <f>G23+1</f>
         <v>70</v>
       </c>
-      <c r="H19" s="26">
+      <c r="H19" s="18">
         <v>1</v>
       </c>
-      <c r="I19" s="26">
+      <c r="I19" s="18">
         <v>14</v>
       </c>
-      <c r="J19" s="26" t="s">
+      <c r="J19" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="K19" s="20"/>
-      <c r="L19" s="18"/>
-      <c r="M19" s="20"/>
-      <c r="N19" s="26">
+      <c r="K19" s="15"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="15"/>
+      <c r="N19" s="18">
         <f>N23+1</f>
         <v>112</v>
       </c>
-      <c r="O19" s="26">
+      <c r="O19" s="18">
         <v>1</v>
       </c>
-      <c r="P19" s="26">
+      <c r="P19" s="18">
         <v>14</v>
       </c>
-      <c r="Q19" s="26" t="s">
+      <c r="Q19" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="R19" s="31"/>
-      <c r="S19" s="26">
+      <c r="R19" s="20"/>
+      <c r="S19" s="18">
         <f>S23+1</f>
         <v>154</v>
       </c>
-      <c r="T19" s="26">
+      <c r="T19" s="18">
         <v>1</v>
       </c>
-      <c r="U19" s="26">
+      <c r="U19" s="18">
         <v>14</v>
       </c>
-      <c r="V19" s="26" t="s">
+      <c r="V19" s="18" t="s">
         <v>209</v>
       </c>
-      <c r="W19" s="20"/>
+      <c r="W19" s="15"/>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A20" s="20"/>
-      <c r="B20" s="20"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="20"/>
-      <c r="J20" s="20"/>
-      <c r="K20" s="20"/>
-      <c r="L20" s="18"/>
-      <c r="M20" s="20"/>
-      <c r="N20" s="20"/>
-      <c r="O20" s="20"/>
-      <c r="P20" s="20"/>
-      <c r="Q20" s="20"/>
-      <c r="R20" s="31"/>
-      <c r="S20" s="20"/>
-      <c r="T20" s="20"/>
-      <c r="U20" s="20"/>
-      <c r="V20" s="20"/>
-      <c r="W20" s="20"/>
+      <c r="A20" s="15"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="15"/>
+      <c r="N20" s="15"/>
+      <c r="O20" s="15"/>
+      <c r="P20" s="15"/>
+      <c r="Q20" s="15"/>
+      <c r="R20" s="20"/>
+      <c r="S20" s="15"/>
+      <c r="T20" s="15"/>
+      <c r="U20" s="15"/>
+      <c r="V20" s="15"/>
+      <c r="W20" s="15"/>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A21" s="20"/>
-      <c r="B21" s="24"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="29" t="s">
+      <c r="A21" s="15"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="G21" s="24"/>
-      <c r="H21" s="24"/>
-      <c r="I21" s="24"/>
-      <c r="J21" s="24"/>
-      <c r="K21" s="20"/>
-      <c r="L21" s="18"/>
-      <c r="M21" s="20"/>
-      <c r="N21" s="24"/>
-      <c r="O21" s="24"/>
-      <c r="P21" s="24"/>
-      <c r="Q21" s="24"/>
-      <c r="R21" s="30" t="s">
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="15"/>
+      <c r="N21" s="16"/>
+      <c r="O21" s="16"/>
+      <c r="P21" s="16"/>
+      <c r="Q21" s="16"/>
+      <c r="R21" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="S21" s="24"/>
-      <c r="T21" s="24"/>
-      <c r="U21" s="24"/>
-      <c r="V21" s="24"/>
-      <c r="W21" s="20"/>
+      <c r="S21" s="16"/>
+      <c r="T21" s="16"/>
+      <c r="U21" s="16"/>
+      <c r="V21" s="16"/>
+      <c r="W21" s="15"/>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A22" s="20"/>
-      <c r="B22" s="26" t="s">
+      <c r="A22" s="15"/>
+      <c r="B22" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="25" t="s">
+      <c r="C22" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="D22" s="25" t="s">
+      <c r="D22" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="E22" s="25" t="s">
+      <c r="E22" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="F22" s="20"/>
-      <c r="G22" s="26" t="s">
+      <c r="F22" s="15"/>
+      <c r="G22" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="H22" s="25" t="s">
+      <c r="H22" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="I22" s="25" t="s">
+      <c r="I22" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="J22" s="25" t="s">
+      <c r="J22" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="K22" s="20"/>
-      <c r="L22" s="18"/>
-      <c r="M22" s="20"/>
-      <c r="N22" s="26" t="s">
+      <c r="K22" s="15"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="15"/>
+      <c r="N22" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="O22" s="25" t="s">
+      <c r="O22" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="P22" s="25" t="s">
+      <c r="P22" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="Q22" s="25" t="s">
+      <c r="Q22" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="R22" s="31"/>
-      <c r="S22" s="26" t="s">
+      <c r="R22" s="20"/>
+      <c r="S22" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="T22" s="25" t="s">
+      <c r="T22" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="U22" s="25" t="s">
+      <c r="U22" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="V22" s="25" t="s">
+      <c r="V22" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="W22" s="20"/>
+      <c r="W22" s="15"/>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A23" s="20"/>
-      <c r="B23" s="26">
+      <c r="A23" s="15"/>
+      <c r="B23" s="18">
         <f t="shared" ref="B23:B34" si="4">B24+1</f>
         <v>27</v>
       </c>
-      <c r="C23" s="26">
+      <c r="C23" s="18">
         <v>14</v>
       </c>
-      <c r="D23" s="26">
+      <c r="D23" s="18">
         <v>1</v>
       </c>
-      <c r="E23" s="26" t="s">
+      <c r="E23" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="F23" s="20"/>
-      <c r="G23" s="26">
+      <c r="F23" s="15"/>
+      <c r="G23" s="18">
         <f t="shared" ref="G23:G34" si="5">G24+1</f>
         <v>69</v>
       </c>
-      <c r="H23" s="26">
+      <c r="H23" s="18">
         <v>14</v>
       </c>
-      <c r="I23" s="26">
+      <c r="I23" s="18">
         <v>1</v>
       </c>
-      <c r="J23" s="26" t="s">
+      <c r="J23" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="K23" s="20"/>
-      <c r="L23" s="18"/>
-      <c r="M23" s="20"/>
-      <c r="N23" s="26">
+      <c r="K23" s="15"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="15"/>
+      <c r="N23" s="18">
         <f t="shared" ref="N23:N34" si="6">N24+1</f>
         <v>111</v>
       </c>
-      <c r="O23" s="26">
+      <c r="O23" s="18">
         <v>14</v>
       </c>
-      <c r="P23" s="26">
+      <c r="P23" s="18">
         <v>1</v>
       </c>
-      <c r="Q23" s="26" t="s">
+      <c r="Q23" s="18" t="s">
         <v>197</v>
       </c>
-      <c r="R23" s="31"/>
-      <c r="S23" s="26">
+      <c r="R23" s="20"/>
+      <c r="S23" s="18">
         <f t="shared" ref="S23:S34" si="7">S24+1</f>
         <v>153</v>
       </c>
-      <c r="T23" s="26">
+      <c r="T23" s="18">
         <v>14</v>
       </c>
-      <c r="U23" s="26">
+      <c r="U23" s="18">
         <v>1</v>
       </c>
-      <c r="V23" s="26" t="s">
+      <c r="V23" s="18" t="s">
         <v>183</v>
       </c>
-      <c r="W23" s="20"/>
+      <c r="W23" s="15"/>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A24" s="20"/>
-      <c r="B24" s="26">
+      <c r="A24" s="15"/>
+      <c r="B24" s="18">
         <f t="shared" si="4"/>
         <v>26</v>
       </c>
-      <c r="C24" s="26">
+      <c r="C24" s="18">
         <v>13</v>
       </c>
-      <c r="D24" s="26">
+      <c r="D24" s="18">
         <v>2</v>
       </c>
-      <c r="E24" s="26" t="s">
+      <c r="E24" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="F24" s="20"/>
-      <c r="G24" s="26">
+      <c r="F24" s="15"/>
+      <c r="G24" s="18">
         <f t="shared" si="5"/>
         <v>68</v>
       </c>
-      <c r="H24" s="26">
+      <c r="H24" s="18">
         <v>13</v>
       </c>
-      <c r="I24" s="26">
+      <c r="I24" s="18">
         <v>2</v>
       </c>
-      <c r="J24" s="26" t="s">
+      <c r="J24" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="K24" s="20"/>
-      <c r="L24" s="18"/>
-      <c r="M24" s="20"/>
-      <c r="N24" s="26">
+      <c r="K24" s="15"/>
+      <c r="L24" s="13"/>
+      <c r="M24" s="15"/>
+      <c r="N24" s="18">
         <f t="shared" si="6"/>
         <v>110</v>
       </c>
-      <c r="O24" s="26">
+      <c r="O24" s="18">
         <v>13</v>
       </c>
-      <c r="P24" s="26">
+      <c r="P24" s="18">
         <v>2</v>
       </c>
-      <c r="Q24" s="26" t="s">
+      <c r="Q24" s="18" t="s">
         <v>210</v>
       </c>
-      <c r="R24" s="31"/>
-      <c r="S24" s="26">
+      <c r="R24" s="20"/>
+      <c r="S24" s="18">
         <f t="shared" si="7"/>
         <v>152</v>
       </c>
-      <c r="T24" s="26">
+      <c r="T24" s="18">
         <v>13</v>
       </c>
-      <c r="U24" s="26">
+      <c r="U24" s="18">
         <v>2</v>
       </c>
-      <c r="V24" s="26" t="s">
+      <c r="V24" s="18" t="s">
         <v>170</v>
       </c>
-      <c r="W24" s="20"/>
+      <c r="W24" s="15"/>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A25" s="20"/>
-      <c r="B25" s="26">
+      <c r="A25" s="15"/>
+      <c r="B25" s="18">
         <f t="shared" si="4"/>
         <v>25</v>
       </c>
-      <c r="C25" s="26">
+      <c r="C25" s="18">
         <v>12</v>
       </c>
-      <c r="D25" s="26">
+      <c r="D25" s="18">
         <v>3</v>
       </c>
-      <c r="E25" s="26" t="s">
+      <c r="E25" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="F25" s="20"/>
-      <c r="G25" s="26">
+      <c r="F25" s="15"/>
+      <c r="G25" s="18">
         <f t="shared" si="5"/>
         <v>67</v>
       </c>
-      <c r="H25" s="26">
+      <c r="H25" s="18">
         <v>12</v>
       </c>
-      <c r="I25" s="26">
+      <c r="I25" s="18">
         <v>3</v>
       </c>
-      <c r="J25" s="26" t="s">
+      <c r="J25" s="18" t="s">
         <v>198</v>
       </c>
-      <c r="K25" s="20"/>
-      <c r="L25" s="18"/>
-      <c r="M25" s="20"/>
-      <c r="N25" s="26">
+      <c r="K25" s="15"/>
+      <c r="L25" s="13"/>
+      <c r="M25" s="15"/>
+      <c r="N25" s="18">
         <f t="shared" si="6"/>
         <v>109</v>
       </c>
-      <c r="O25" s="26">
+      <c r="O25" s="18">
         <v>12</v>
       </c>
-      <c r="P25" s="26">
+      <c r="P25" s="18">
         <v>3</v>
       </c>
-      <c r="Q25" s="26" t="s">
+      <c r="Q25" s="18" t="s">
         <v>184</v>
       </c>
-      <c r="R25" s="31"/>
-      <c r="S25" s="26">
+      <c r="R25" s="20"/>
+      <c r="S25" s="18">
         <f t="shared" si="7"/>
         <v>151</v>
       </c>
-      <c r="T25" s="26">
+      <c r="T25" s="18">
         <v>12</v>
       </c>
-      <c r="U25" s="26">
+      <c r="U25" s="18">
         <v>3</v>
       </c>
-      <c r="V25" s="26" t="s">
+      <c r="V25" s="18" t="s">
         <v>143</v>
       </c>
-      <c r="W25" s="20"/>
+      <c r="W25" s="15"/>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A26" s="20"/>
-      <c r="B26" s="26">
+      <c r="A26" s="15"/>
+      <c r="B26" s="18">
         <f t="shared" si="4"/>
         <v>24</v>
       </c>
-      <c r="C26" s="26">
+      <c r="C26" s="18">
         <v>11</v>
       </c>
-      <c r="D26" s="26">
+      <c r="D26" s="18">
         <v>4</v>
       </c>
-      <c r="E26" s="26" t="s">
+      <c r="E26" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="F26" s="20"/>
-      <c r="G26" s="26">
+      <c r="F26" s="15"/>
+      <c r="G26" s="18">
         <f t="shared" si="5"/>
         <v>66</v>
       </c>
-      <c r="H26" s="26">
+      <c r="H26" s="18">
         <v>11</v>
       </c>
-      <c r="I26" s="26">
+      <c r="I26" s="18">
         <v>4</v>
       </c>
-      <c r="J26" s="26" t="s">
+      <c r="J26" s="18" t="s">
         <v>211</v>
       </c>
-      <c r="K26" s="20"/>
-      <c r="L26" s="18"/>
-      <c r="M26" s="20"/>
-      <c r="N26" s="26">
+      <c r="K26" s="15"/>
+      <c r="L26" s="13"/>
+      <c r="M26" s="15"/>
+      <c r="N26" s="18">
         <f t="shared" si="6"/>
         <v>108</v>
       </c>
-      <c r="O26" s="26">
+      <c r="O26" s="18">
         <v>11</v>
       </c>
-      <c r="P26" s="26">
+      <c r="P26" s="18">
         <v>4</v>
       </c>
-      <c r="Q26" s="26" t="s">
+      <c r="Q26" s="18" t="s">
         <v>171</v>
       </c>
-      <c r="R26" s="31"/>
-      <c r="S26" s="26">
+      <c r="R26" s="20"/>
+      <c r="S26" s="18">
         <f t="shared" si="7"/>
         <v>150</v>
       </c>
-      <c r="T26" s="26">
+      <c r="T26" s="18">
         <v>11</v>
       </c>
-      <c r="U26" s="26">
+      <c r="U26" s="18">
         <v>4</v>
       </c>
-      <c r="V26" s="26" t="s">
+      <c r="V26" s="18" t="s">
         <v>157</v>
       </c>
-      <c r="W26" s="20"/>
+      <c r="W26" s="15"/>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A27" s="20"/>
-      <c r="B27" s="26">
+      <c r="A27" s="15"/>
+      <c r="B27" s="18">
         <f t="shared" si="4"/>
         <v>23</v>
       </c>
-      <c r="C27" s="26">
+      <c r="C27" s="18">
         <v>10</v>
       </c>
-      <c r="D27" s="26">
+      <c r="D27" s="18">
         <v>5</v>
       </c>
-      <c r="E27" s="26" t="s">
+      <c r="E27" s="18" t="s">
         <v>199</v>
       </c>
-      <c r="F27" s="20"/>
-      <c r="G27" s="26">
+      <c r="F27" s="15"/>
+      <c r="G27" s="18">
         <f t="shared" si="5"/>
         <v>65</v>
       </c>
-      <c r="H27" s="26">
+      <c r="H27" s="18">
         <v>10</v>
       </c>
-      <c r="I27" s="26">
+      <c r="I27" s="18">
         <v>5</v>
       </c>
-      <c r="J27" s="26" t="s">
+      <c r="J27" s="18" t="s">
         <v>185</v>
       </c>
-      <c r="K27" s="20"/>
-      <c r="L27" s="18"/>
-      <c r="M27" s="20"/>
-      <c r="N27" s="26">
+      <c r="K27" s="15"/>
+      <c r="L27" s="13"/>
+      <c r="M27" s="15"/>
+      <c r="N27" s="18">
         <f t="shared" si="6"/>
         <v>107</v>
       </c>
-      <c r="O27" s="26">
+      <c r="O27" s="18">
         <v>10</v>
       </c>
-      <c r="P27" s="26">
+      <c r="P27" s="18">
         <v>5</v>
       </c>
-      <c r="Q27" s="26" t="s">
+      <c r="Q27" s="18" t="s">
         <v>144</v>
       </c>
-      <c r="R27" s="31"/>
-      <c r="S27" s="26">
+      <c r="R27" s="20"/>
+      <c r="S27" s="18">
         <f t="shared" si="7"/>
         <v>149</v>
       </c>
-      <c r="T27" s="26">
+      <c r="T27" s="18">
         <v>10</v>
       </c>
-      <c r="U27" s="26">
+      <c r="U27" s="18">
         <v>5</v>
       </c>
-      <c r="V27" s="26" t="s">
+      <c r="V27" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="W27" s="20"/>
+      <c r="W27" s="15"/>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A28" s="20"/>
-      <c r="B28" s="26">
+      <c r="A28" s="15"/>
+      <c r="B28" s="18">
         <f t="shared" si="4"/>
         <v>22</v>
       </c>
-      <c r="C28" s="26">
+      <c r="C28" s="18">
         <v>9</v>
       </c>
-      <c r="D28" s="26">
+      <c r="D28" s="18">
         <v>6</v>
       </c>
-      <c r="E28" s="26" t="s">
+      <c r="E28" s="18" t="s">
         <v>212</v>
       </c>
-      <c r="F28" s="20"/>
-      <c r="G28" s="26">
+      <c r="F28" s="15"/>
+      <c r="G28" s="18">
         <f t="shared" si="5"/>
         <v>64</v>
       </c>
-      <c r="H28" s="26">
+      <c r="H28" s="18">
         <v>9</v>
       </c>
-      <c r="I28" s="26">
+      <c r="I28" s="18">
         <v>6</v>
       </c>
-      <c r="J28" s="26" t="s">
+      <c r="J28" s="18" t="s">
         <v>172</v>
       </c>
-      <c r="K28" s="20"/>
-      <c r="L28" s="18"/>
-      <c r="M28" s="20"/>
-      <c r="N28" s="26">
+      <c r="K28" s="15"/>
+      <c r="L28" s="13"/>
+      <c r="M28" s="15"/>
+      <c r="N28" s="18">
         <f t="shared" si="6"/>
         <v>106</v>
       </c>
-      <c r="O28" s="26">
+      <c r="O28" s="18">
         <v>9</v>
       </c>
-      <c r="P28" s="26">
+      <c r="P28" s="18">
         <v>6</v>
       </c>
-      <c r="Q28" s="26" t="s">
+      <c r="Q28" s="18" t="s">
         <v>158</v>
       </c>
-      <c r="R28" s="31"/>
-      <c r="S28" s="26">
+      <c r="R28" s="20"/>
+      <c r="S28" s="18">
         <f t="shared" si="7"/>
         <v>148</v>
       </c>
-      <c r="T28" s="26">
+      <c r="T28" s="18">
         <v>9</v>
       </c>
-      <c r="U28" s="26">
+      <c r="U28" s="18">
         <v>6</v>
       </c>
-      <c r="V28" s="26" t="s">
+      <c r="V28" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="W28" s="20"/>
+      <c r="W28" s="15"/>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A29" s="20"/>
-      <c r="B29" s="26">
+      <c r="A29" s="15"/>
+      <c r="B29" s="18">
         <f t="shared" si="4"/>
         <v>21</v>
       </c>
-      <c r="C29" s="26">
+      <c r="C29" s="18">
         <v>8</v>
       </c>
-      <c r="D29" s="26">
+      <c r="D29" s="18">
         <v>7</v>
       </c>
-      <c r="E29" s="26" t="s">
+      <c r="E29" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="F29" s="20"/>
-      <c r="G29" s="26">
+      <c r="F29" s="15"/>
+      <c r="G29" s="18">
         <f t="shared" si="5"/>
         <v>63</v>
       </c>
-      <c r="H29" s="26">
+      <c r="H29" s="18">
         <v>8</v>
       </c>
-      <c r="I29" s="26">
+      <c r="I29" s="18">
         <v>7</v>
       </c>
-      <c r="J29" s="26" t="s">
+      <c r="J29" s="18" t="s">
         <v>145</v>
       </c>
-      <c r="K29" s="20"/>
-      <c r="L29" s="18"/>
-      <c r="M29" s="20"/>
-      <c r="N29" s="26">
+      <c r="K29" s="15"/>
+      <c r="L29" s="13"/>
+      <c r="M29" s="15"/>
+      <c r="N29" s="18">
         <f t="shared" si="6"/>
         <v>105</v>
       </c>
-      <c r="O29" s="26">
+      <c r="O29" s="18">
         <v>8</v>
       </c>
-      <c r="P29" s="26">
+      <c r="P29" s="18">
         <v>7</v>
       </c>
-      <c r="Q29" s="26" t="s">
+      <c r="Q29" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="R29" s="31"/>
-      <c r="S29" s="26">
+      <c r="R29" s="20"/>
+      <c r="S29" s="18">
         <f t="shared" si="7"/>
         <v>147</v>
       </c>
-      <c r="T29" s="26">
+      <c r="T29" s="18">
         <v>8</v>
       </c>
-      <c r="U29" s="26">
+      <c r="U29" s="18">
         <v>7</v>
       </c>
-      <c r="V29" s="26" t="s">
+      <c r="V29" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="W29" s="20"/>
+      <c r="W29" s="15"/>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A30" s="20"/>
-      <c r="B30" s="26">
+      <c r="A30" s="15"/>
+      <c r="B30" s="18">
         <f t="shared" si="4"/>
         <v>20</v>
       </c>
-      <c r="C30" s="26">
+      <c r="C30" s="18">
         <v>7</v>
       </c>
-      <c r="D30" s="26">
+      <c r="D30" s="18">
         <v>8</v>
       </c>
-      <c r="E30" s="26" t="s">
+      <c r="E30" s="18" t="s">
         <v>173</v>
       </c>
-      <c r="F30" s="20"/>
-      <c r="G30" s="26">
+      <c r="F30" s="15"/>
+      <c r="G30" s="18">
         <f t="shared" si="5"/>
         <v>62</v>
       </c>
-      <c r="H30" s="26">
+      <c r="H30" s="18">
         <v>7</v>
       </c>
-      <c r="I30" s="26">
+      <c r="I30" s="18">
         <v>8</v>
       </c>
-      <c r="J30" s="26" t="s">
+      <c r="J30" s="18" t="s">
         <v>159</v>
       </c>
-      <c r="K30" s="20"/>
-      <c r="L30" s="18"/>
-      <c r="M30" s="20"/>
-      <c r="N30" s="26">
+      <c r="K30" s="15"/>
+      <c r="L30" s="13"/>
+      <c r="M30" s="15"/>
+      <c r="N30" s="18">
         <f t="shared" si="6"/>
         <v>104</v>
       </c>
-      <c r="O30" s="26">
+      <c r="O30" s="18">
         <v>7</v>
       </c>
-      <c r="P30" s="26">
+      <c r="P30" s="18">
         <v>8</v>
       </c>
-      <c r="Q30" s="26" t="s">
+      <c r="Q30" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="R30" s="31"/>
-      <c r="S30" s="26">
+      <c r="R30" s="20"/>
+      <c r="S30" s="18">
         <f t="shared" si="7"/>
         <v>146</v>
       </c>
-      <c r="T30" s="26">
+      <c r="T30" s="18">
         <v>7</v>
       </c>
-      <c r="U30" s="26">
+      <c r="U30" s="18">
         <v>8</v>
       </c>
-      <c r="V30" s="26" t="s">
+      <c r="V30" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="W30" s="20"/>
+      <c r="W30" s="15"/>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A31" s="20"/>
-      <c r="B31" s="26">
+      <c r="A31" s="15"/>
+      <c r="B31" s="18">
         <f t="shared" si="4"/>
         <v>19</v>
       </c>
-      <c r="C31" s="26">
+      <c r="C31" s="18">
         <v>6</v>
       </c>
-      <c r="D31" s="26">
+      <c r="D31" s="18">
         <v>9</v>
       </c>
-      <c r="E31" s="26" t="s">
+      <c r="E31" s="18" t="s">
         <v>146</v>
       </c>
-      <c r="F31" s="20"/>
-      <c r="G31" s="26">
+      <c r="F31" s="15"/>
+      <c r="G31" s="18">
         <f t="shared" si="5"/>
         <v>61</v>
       </c>
-      <c r="H31" s="26">
+      <c r="H31" s="18">
         <v>6</v>
       </c>
-      <c r="I31" s="26">
+      <c r="I31" s="18">
         <v>9</v>
       </c>
-      <c r="J31" s="26" t="s">
+      <c r="J31" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="K31" s="20"/>
-      <c r="L31" s="18"/>
-      <c r="M31" s="20"/>
-      <c r="N31" s="26">
+      <c r="K31" s="15"/>
+      <c r="L31" s="13"/>
+      <c r="M31" s="15"/>
+      <c r="N31" s="18">
         <f t="shared" si="6"/>
         <v>103</v>
       </c>
-      <c r="O31" s="26">
+      <c r="O31" s="18">
         <v>6</v>
       </c>
-      <c r="P31" s="26">
+      <c r="P31" s="18">
         <v>9</v>
       </c>
-      <c r="Q31" s="26" t="s">
+      <c r="Q31" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="R31" s="31"/>
-      <c r="S31" s="26">
+      <c r="R31" s="20"/>
+      <c r="S31" s="18">
         <f t="shared" si="7"/>
         <v>145</v>
       </c>
-      <c r="T31" s="26">
+      <c r="T31" s="18">
         <v>6</v>
       </c>
-      <c r="U31" s="26">
+      <c r="U31" s="18">
         <v>9</v>
       </c>
-      <c r="V31" s="26" t="s">
+      <c r="V31" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="W31" s="20"/>
+      <c r="W31" s="15"/>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A32" s="20"/>
-      <c r="B32" s="26">
+      <c r="A32" s="15"/>
+      <c r="B32" s="18">
         <f t="shared" si="4"/>
         <v>18</v>
       </c>
-      <c r="C32" s="26">
+      <c r="C32" s="18">
         <v>5</v>
       </c>
-      <c r="D32" s="26">
+      <c r="D32" s="18">
         <v>10</v>
       </c>
-      <c r="E32" s="26" t="s">
+      <c r="E32" s="18" t="s">
         <v>160</v>
       </c>
-      <c r="F32" s="20"/>
-      <c r="G32" s="26">
+      <c r="F32" s="15"/>
+      <c r="G32" s="18">
         <f t="shared" si="5"/>
         <v>60</v>
       </c>
-      <c r="H32" s="26">
+      <c r="H32" s="18">
         <v>5</v>
       </c>
-      <c r="I32" s="26">
+      <c r="I32" s="18">
         <v>10</v>
       </c>
-      <c r="J32" s="26" t="s">
+      <c r="J32" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="K32" s="20"/>
-      <c r="L32" s="18"/>
-      <c r="M32" s="20"/>
-      <c r="N32" s="26">
+      <c r="K32" s="15"/>
+      <c r="L32" s="13"/>
+      <c r="M32" s="15"/>
+      <c r="N32" s="18">
         <f t="shared" si="6"/>
         <v>102</v>
       </c>
-      <c r="O32" s="26">
+      <c r="O32" s="18">
         <v>5</v>
       </c>
-      <c r="P32" s="26">
+      <c r="P32" s="18">
         <v>10</v>
       </c>
-      <c r="Q32" s="26" t="s">
+      <c r="Q32" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="R32" s="31"/>
-      <c r="S32" s="26">
+      <c r="R32" s="20"/>
+      <c r="S32" s="18">
         <f t="shared" si="7"/>
         <v>144</v>
       </c>
-      <c r="T32" s="26">
+      <c r="T32" s="18">
         <v>5</v>
       </c>
-      <c r="U32" s="26">
+      <c r="U32" s="18">
         <v>10</v>
       </c>
-      <c r="V32" s="26" t="s">
+      <c r="V32" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="W32" s="20"/>
+      <c r="W32" s="15"/>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A33" s="20"/>
-      <c r="B33" s="26">
+      <c r="A33" s="15"/>
+      <c r="B33" s="18">
         <f t="shared" si="4"/>
         <v>17</v>
       </c>
-      <c r="C33" s="26">
+      <c r="C33" s="18">
         <v>4</v>
       </c>
-      <c r="D33" s="26">
+      <c r="D33" s="18">
         <v>11</v>
       </c>
-      <c r="E33" s="26" t="s">
+      <c r="E33" s="18" t="s">
         <v>134</v>
       </c>
-      <c r="F33" s="20"/>
-      <c r="G33" s="26">
+      <c r="F33" s="15"/>
+      <c r="G33" s="18">
         <f t="shared" si="5"/>
         <v>59</v>
       </c>
-      <c r="H33" s="26">
+      <c r="H33" s="18">
         <v>4</v>
       </c>
-      <c r="I33" s="26">
+      <c r="I33" s="18">
         <v>11</v>
       </c>
-      <c r="J33" s="26" t="s">
+      <c r="J33" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="K33" s="20"/>
-      <c r="L33" s="18"/>
-      <c r="M33" s="20"/>
-      <c r="N33" s="26">
+      <c r="K33" s="15"/>
+      <c r="L33" s="13"/>
+      <c r="M33" s="15"/>
+      <c r="N33" s="18">
         <f t="shared" si="6"/>
         <v>101</v>
       </c>
-      <c r="O33" s="26">
+      <c r="O33" s="18">
         <v>4</v>
       </c>
-      <c r="P33" s="26">
+      <c r="P33" s="18">
         <v>11</v>
       </c>
-      <c r="Q33" s="26" t="s">
+      <c r="Q33" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="R33" s="31"/>
-      <c r="S33" s="26">
+      <c r="R33" s="20"/>
+      <c r="S33" s="18">
         <f t="shared" si="7"/>
         <v>143</v>
       </c>
-      <c r="T33" s="26">
+      <c r="T33" s="18">
         <v>4</v>
       </c>
-      <c r="U33" s="26">
+      <c r="U33" s="18">
         <v>11</v>
       </c>
-      <c r="V33" s="26" t="s">
+      <c r="V33" s="18" t="s">
         <v>200</v>
       </c>
-      <c r="W33" s="20"/>
+      <c r="W33" s="15"/>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A34" s="20"/>
-      <c r="B34" s="26">
+      <c r="A34" s="15"/>
+      <c r="B34" s="18">
         <f t="shared" si="4"/>
         <v>16</v>
       </c>
-      <c r="C34" s="26">
+      <c r="C34" s="18">
         <v>3</v>
       </c>
-      <c r="D34" s="26">
+      <c r="D34" s="18">
         <v>12</v>
       </c>
-      <c r="E34" s="26" t="s">
+      <c r="E34" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="F34" s="20"/>
-      <c r="G34" s="26">
+      <c r="F34" s="15"/>
+      <c r="G34" s="18">
         <f t="shared" si="5"/>
         <v>58</v>
       </c>
-      <c r="H34" s="26">
+      <c r="H34" s="18">
         <v>3</v>
       </c>
-      <c r="I34" s="26">
+      <c r="I34" s="18">
         <v>12</v>
       </c>
-      <c r="J34" s="26" t="s">
+      <c r="J34" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="K34" s="20"/>
-      <c r="L34" s="18"/>
-      <c r="M34" s="20"/>
-      <c r="N34" s="26">
+      <c r="K34" s="15"/>
+      <c r="L34" s="13"/>
+      <c r="M34" s="15"/>
+      <c r="N34" s="18">
         <f t="shared" si="6"/>
         <v>100</v>
       </c>
-      <c r="O34" s="26">
+      <c r="O34" s="18">
         <v>3</v>
       </c>
-      <c r="P34" s="26">
+      <c r="P34" s="18">
         <v>12</v>
       </c>
-      <c r="Q34" s="26" t="s">
+      <c r="Q34" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="R34" s="31"/>
-      <c r="S34" s="26">
+      <c r="R34" s="20"/>
+      <c r="S34" s="18">
         <f t="shared" si="7"/>
         <v>142</v>
       </c>
-      <c r="T34" s="26">
+      <c r="T34" s="18">
         <v>3</v>
       </c>
-      <c r="U34" s="26">
+      <c r="U34" s="18">
         <v>12</v>
       </c>
-      <c r="V34" s="26" t="s">
+      <c r="V34" s="18" t="s">
         <v>213</v>
       </c>
-      <c r="W34" s="20"/>
+      <c r="W34" s="15"/>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A35" s="20"/>
-      <c r="B35" s="26">
+      <c r="A35" s="15"/>
+      <c r="B35" s="18">
         <f>B36+1</f>
         <v>15</v>
       </c>
-      <c r="C35" s="26">
+      <c r="C35" s="18">
         <v>2</v>
       </c>
-      <c r="D35" s="26">
+      <c r="D35" s="18">
         <v>13</v>
       </c>
-      <c r="E35" s="26" t="s">
+      <c r="E35" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="F35" s="20"/>
-      <c r="G35" s="26">
+      <c r="F35" s="15"/>
+      <c r="G35" s="18">
         <f>G36+1</f>
         <v>57</v>
       </c>
-      <c r="H35" s="26">
+      <c r="H35" s="18">
         <v>2</v>
       </c>
-      <c r="I35" s="26">
+      <c r="I35" s="18">
         <v>13</v>
       </c>
-      <c r="J35" s="26" t="s">
+      <c r="J35" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="K35" s="20"/>
-      <c r="L35" s="18"/>
-      <c r="M35" s="20"/>
-      <c r="N35" s="26">
+      <c r="K35" s="15"/>
+      <c r="L35" s="13"/>
+      <c r="M35" s="15"/>
+      <c r="N35" s="18">
         <f>N36+1</f>
         <v>99</v>
       </c>
-      <c r="O35" s="26">
+      <c r="O35" s="18">
         <v>2</v>
       </c>
-      <c r="P35" s="26">
+      <c r="P35" s="18">
         <v>13</v>
       </c>
-      <c r="Q35" s="26" t="s">
+      <c r="Q35" s="18" t="s">
         <v>201</v>
       </c>
-      <c r="R35" s="31"/>
-      <c r="S35" s="26">
+      <c r="R35" s="20"/>
+      <c r="S35" s="18">
         <f>S36+1</f>
         <v>141</v>
       </c>
-      <c r="T35" s="26">
+      <c r="T35" s="18">
         <v>2</v>
       </c>
-      <c r="U35" s="26">
+      <c r="U35" s="18">
         <v>13</v>
       </c>
-      <c r="V35" s="26" t="s">
+      <c r="V35" s="18" t="s">
         <v>187</v>
       </c>
-      <c r="W35" s="20"/>
+      <c r="W35" s="15"/>
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A36" s="20"/>
-      <c r="B36" s="26">
+      <c r="A36" s="15"/>
+      <c r="B36" s="18">
         <f>B40+1</f>
         <v>14</v>
       </c>
-      <c r="C36" s="26">
+      <c r="C36" s="18">
         <v>1</v>
       </c>
-      <c r="D36" s="26">
+      <c r="D36" s="18">
         <v>14</v>
       </c>
-      <c r="E36" s="26" t="s">
+      <c r="E36" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="F36" s="20"/>
-      <c r="G36" s="26">
+      <c r="F36" s="15"/>
+      <c r="G36" s="18">
         <f>G40+1</f>
         <v>56</v>
       </c>
-      <c r="H36" s="26">
+      <c r="H36" s="18">
         <v>1</v>
       </c>
-      <c r="I36" s="26">
+      <c r="I36" s="18">
         <v>14</v>
       </c>
-      <c r="J36" s="26" t="s">
+      <c r="J36" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="K36" s="20"/>
-      <c r="L36" s="18"/>
-      <c r="M36" s="20"/>
-      <c r="N36" s="26">
+      <c r="K36" s="15"/>
+      <c r="L36" s="13"/>
+      <c r="M36" s="15"/>
+      <c r="N36" s="18">
         <f>N40+1</f>
         <v>98</v>
       </c>
-      <c r="O36" s="26">
+      <c r="O36" s="18">
         <v>1</v>
       </c>
-      <c r="P36" s="26">
+      <c r="P36" s="18">
         <v>14</v>
       </c>
-      <c r="Q36" s="26" t="s">
+      <c r="Q36" s="18" t="s">
         <v>214</v>
       </c>
-      <c r="R36" s="31"/>
-      <c r="S36" s="26">
+      <c r="R36" s="20"/>
+      <c r="S36" s="18">
         <f>S40+1</f>
         <v>140</v>
       </c>
-      <c r="T36" s="26">
+      <c r="T36" s="18">
         <v>1</v>
       </c>
-      <c r="U36" s="26">
+      <c r="U36" s="18">
         <v>14</v>
       </c>
-      <c r="V36" s="26" t="s">
+      <c r="V36" s="18" t="s">
         <v>174</v>
       </c>
-      <c r="W36" s="20"/>
+      <c r="W36" s="15"/>
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A37" s="20"/>
-      <c r="B37" s="20"/>
-      <c r="C37" s="20"/>
-      <c r="D37" s="20"/>
-      <c r="E37" s="20"/>
-      <c r="F37" s="20"/>
-      <c r="G37" s="20"/>
-      <c r="H37" s="20"/>
-      <c r="I37" s="20"/>
-      <c r="J37" s="20"/>
-      <c r="K37" s="20"/>
-      <c r="L37" s="18"/>
-      <c r="M37" s="20"/>
-      <c r="N37" s="20"/>
-      <c r="O37" s="20"/>
-      <c r="P37" s="20"/>
-      <c r="Q37" s="20"/>
-      <c r="R37" s="31"/>
-      <c r="S37" s="20"/>
-      <c r="T37" s="20"/>
-      <c r="U37" s="20"/>
-      <c r="V37" s="20"/>
-      <c r="W37" s="20"/>
+      <c r="A37" s="15"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="15"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="15"/>
+      <c r="J37" s="15"/>
+      <c r="K37" s="15"/>
+      <c r="L37" s="13"/>
+      <c r="M37" s="15"/>
+      <c r="N37" s="15"/>
+      <c r="O37" s="15"/>
+      <c r="P37" s="15"/>
+      <c r="Q37" s="15"/>
+      <c r="R37" s="20"/>
+      <c r="S37" s="15"/>
+      <c r="T37" s="15"/>
+      <c r="U37" s="15"/>
+      <c r="V37" s="15"/>
+      <c r="W37" s="15"/>
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A38" s="20"/>
-      <c r="B38" s="24"/>
-      <c r="C38" s="24"/>
-      <c r="D38" s="24"/>
-      <c r="E38" s="24"/>
-      <c r="F38" s="29" t="s">
+      <c r="A38" s="15"/>
+      <c r="B38" s="16"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="G38" s="24"/>
-      <c r="H38" s="24"/>
-      <c r="I38" s="24"/>
-      <c r="J38" s="24"/>
-      <c r="K38" s="20"/>
-      <c r="L38" s="18"/>
-      <c r="M38" s="20"/>
-      <c r="N38" s="24"/>
-      <c r="O38" s="24"/>
-      <c r="P38" s="24"/>
-      <c r="Q38" s="24"/>
-      <c r="R38" s="30" t="s">
+      <c r="G38" s="16"/>
+      <c r="H38" s="16"/>
+      <c r="I38" s="16"/>
+      <c r="J38" s="16"/>
+      <c r="K38" s="15"/>
+      <c r="L38" s="13"/>
+      <c r="M38" s="15"/>
+      <c r="N38" s="16"/>
+      <c r="O38" s="16"/>
+      <c r="P38" s="16"/>
+      <c r="Q38" s="16"/>
+      <c r="R38" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="S38" s="24"/>
-      <c r="T38" s="24"/>
-      <c r="U38" s="24"/>
-      <c r="V38" s="24"/>
-      <c r="W38" s="20"/>
+      <c r="S38" s="16"/>
+      <c r="T38" s="16"/>
+      <c r="U38" s="16"/>
+      <c r="V38" s="16"/>
+      <c r="W38" s="15"/>
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A39" s="20"/>
-      <c r="B39" s="26" t="s">
+      <c r="A39" s="15"/>
+      <c r="B39" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C39" s="25" t="s">
+      <c r="C39" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="D39" s="25" t="s">
+      <c r="D39" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="E39" s="25" t="s">
+      <c r="E39" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="F39" s="20"/>
-      <c r="G39" s="26" t="s">
+      <c r="F39" s="15"/>
+      <c r="G39" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="H39" s="25" t="s">
+      <c r="H39" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="I39" s="25" t="s">
+      <c r="I39" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="J39" s="25" t="s">
+      <c r="J39" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="K39" s="20"/>
-      <c r="L39" s="18"/>
-      <c r="M39" s="20"/>
-      <c r="N39" s="26" t="s">
+      <c r="K39" s="15"/>
+      <c r="L39" s="13"/>
+      <c r="M39" s="15"/>
+      <c r="N39" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="O39" s="25" t="s">
+      <c r="O39" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="P39" s="25" t="s">
+      <c r="P39" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="Q39" s="25" t="s">
+      <c r="Q39" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="R39" s="20"/>
-      <c r="S39" s="26" t="s">
+      <c r="R39" s="15"/>
+      <c r="S39" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="T39" s="25" t="s">
+      <c r="T39" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="U39" s="25" t="s">
+      <c r="U39" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="V39" s="25" t="s">
+      <c r="V39" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="W39" s="20"/>
+      <c r="W39" s="15"/>
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A40" s="20"/>
-      <c r="B40" s="26">
+      <c r="A40" s="15"/>
+      <c r="B40" s="18">
         <f t="shared" ref="B40:B51" si="8">B41+1</f>
         <v>13</v>
       </c>
-      <c r="C40" s="26">
+      <c r="C40" s="18">
         <v>14</v>
       </c>
-      <c r="D40" s="26">
+      <c r="D40" s="18">
         <v>1</v>
       </c>
-      <c r="E40" s="26" t="s">
+      <c r="E40" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="F40" s="20"/>
-      <c r="G40" s="26">
+      <c r="F40" s="15"/>
+      <c r="G40" s="18">
         <f t="shared" ref="G40:G51" si="9">G41+1</f>
         <v>55</v>
       </c>
-      <c r="H40" s="26">
+      <c r="H40" s="18">
         <v>14</v>
       </c>
-      <c r="I40" s="26">
+      <c r="I40" s="18">
         <v>1</v>
       </c>
-      <c r="J40" s="26" t="s">
+      <c r="J40" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="K40" s="20"/>
-      <c r="L40" s="18"/>
-      <c r="M40" s="20"/>
-      <c r="N40" s="26">
+      <c r="K40" s="15"/>
+      <c r="L40" s="13"/>
+      <c r="M40" s="15"/>
+      <c r="N40" s="18">
         <f t="shared" ref="N40:N51" si="10">N41+1</f>
         <v>97</v>
       </c>
-      <c r="O40" s="26">
+      <c r="O40" s="18">
         <v>14</v>
       </c>
-      <c r="P40" s="26">
+      <c r="P40" s="18">
         <v>1</v>
       </c>
-      <c r="Q40" s="26" t="s">
+      <c r="Q40" s="18" t="s">
         <v>188</v>
       </c>
-      <c r="R40" s="20"/>
-      <c r="S40" s="26">
+      <c r="R40" s="15"/>
+      <c r="S40" s="18">
         <f t="shared" ref="S40:S51" si="11">S41+1</f>
         <v>139</v>
       </c>
-      <c r="T40" s="26">
+      <c r="T40" s="18">
         <v>14</v>
       </c>
-      <c r="U40" s="26">
+      <c r="U40" s="18">
         <v>1</v>
       </c>
-      <c r="V40" s="26" t="s">
+      <c r="V40" s="18" t="s">
         <v>148</v>
       </c>
-      <c r="W40" s="20"/>
+      <c r="W40" s="15"/>
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A41" s="20"/>
-      <c r="B41" s="26">
+      <c r="A41" s="15"/>
+      <c r="B41" s="18">
         <f t="shared" si="8"/>
         <v>12</v>
       </c>
-      <c r="C41" s="26">
+      <c r="C41" s="18">
         <v>13</v>
       </c>
-      <c r="D41" s="26">
+      <c r="D41" s="18">
         <v>2</v>
       </c>
-      <c r="E41" s="26" t="s">
+      <c r="E41" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="F41" s="20"/>
-      <c r="G41" s="26">
+      <c r="F41" s="15"/>
+      <c r="G41" s="18">
         <f t="shared" si="9"/>
         <v>54</v>
       </c>
-      <c r="H41" s="26">
+      <c r="H41" s="18">
         <v>13</v>
       </c>
-      <c r="I41" s="26">
+      <c r="I41" s="18">
         <v>2</v>
       </c>
-      <c r="J41" s="26" t="s">
+      <c r="J41" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="K41" s="20"/>
-      <c r="L41" s="18"/>
-      <c r="M41" s="20"/>
-      <c r="N41" s="26">
+      <c r="K41" s="15"/>
+      <c r="L41" s="13"/>
+      <c r="M41" s="15"/>
+      <c r="N41" s="18">
         <f t="shared" si="10"/>
         <v>96</v>
       </c>
-      <c r="O41" s="26">
+      <c r="O41" s="18">
         <v>13</v>
       </c>
-      <c r="P41" s="26">
+      <c r="P41" s="18">
         <v>2</v>
       </c>
-      <c r="Q41" s="26" t="s">
+      <c r="Q41" s="18" t="s">
         <v>175</v>
       </c>
-      <c r="R41" s="20"/>
-      <c r="S41" s="26">
+      <c r="R41" s="15"/>
+      <c r="S41" s="18">
         <f t="shared" si="11"/>
         <v>138</v>
       </c>
-      <c r="T41" s="26">
+      <c r="T41" s="18">
         <v>13</v>
       </c>
-      <c r="U41" s="26">
+      <c r="U41" s="18">
         <v>2</v>
       </c>
-      <c r="V41" s="26" t="s">
+      <c r="V41" s="18" t="s">
         <v>162</v>
       </c>
-      <c r="W41" s="20"/>
+      <c r="W41" s="15"/>
     </row>
     <row r="42" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A42" s="20"/>
-      <c r="B42" s="26">
+      <c r="A42" s="15"/>
+      <c r="B42" s="18">
         <f t="shared" si="8"/>
         <v>11</v>
       </c>
-      <c r="C42" s="26">
+      <c r="C42" s="18">
         <v>12</v>
       </c>
-      <c r="D42" s="26">
+      <c r="D42" s="18">
         <v>3</v>
       </c>
-      <c r="E42" s="26" t="s">
+      <c r="E42" s="18" t="s">
         <v>202</v>
       </c>
-      <c r="F42" s="20"/>
-      <c r="G42" s="26">
+      <c r="F42" s="15"/>
+      <c r="G42" s="18">
         <f t="shared" si="9"/>
         <v>53</v>
       </c>
-      <c r="H42" s="26">
+      <c r="H42" s="18">
         <v>12</v>
       </c>
-      <c r="I42" s="26">
+      <c r="I42" s="18">
         <v>3</v>
       </c>
-      <c r="J42" s="26" t="s">
+      <c r="J42" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="K42" s="20"/>
-      <c r="L42" s="18"/>
-      <c r="M42" s="20"/>
-      <c r="N42" s="26">
+      <c r="K42" s="15"/>
+      <c r="L42" s="13"/>
+      <c r="M42" s="15"/>
+      <c r="N42" s="18">
         <f t="shared" si="10"/>
         <v>95</v>
       </c>
-      <c r="O42" s="26">
+      <c r="O42" s="18">
         <v>12</v>
       </c>
-      <c r="P42" s="26">
+      <c r="P42" s="18">
         <v>3</v>
       </c>
-      <c r="Q42" s="26" t="s">
+      <c r="Q42" s="18" t="s">
         <v>149</v>
       </c>
-      <c r="R42" s="20"/>
-      <c r="S42" s="26">
+      <c r="R42" s="15"/>
+      <c r="S42" s="18">
         <f t="shared" si="11"/>
         <v>137</v>
       </c>
-      <c r="T42" s="26">
+      <c r="T42" s="18">
         <v>12</v>
       </c>
-      <c r="U42" s="26">
+      <c r="U42" s="18">
         <v>3</v>
       </c>
-      <c r="V42" s="26" t="s">
+      <c r="V42" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="W42" s="20"/>
+      <c r="W42" s="15"/>
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A43" s="20"/>
-      <c r="B43" s="26">
+      <c r="A43" s="15"/>
+      <c r="B43" s="18">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
-      <c r="C43" s="26">
+      <c r="C43" s="18">
         <v>11</v>
       </c>
-      <c r="D43" s="26">
+      <c r="D43" s="18">
         <v>4</v>
       </c>
-      <c r="E43" s="26" t="s">
+      <c r="E43" s="18" t="s">
         <v>215</v>
       </c>
-      <c r="F43" s="20"/>
-      <c r="G43" s="26">
+      <c r="F43" s="15"/>
+      <c r="G43" s="18">
         <f t="shared" si="9"/>
         <v>52</v>
       </c>
-      <c r="H43" s="26">
+      <c r="H43" s="18">
         <v>11</v>
       </c>
-      <c r="I43" s="26">
+      <c r="I43" s="18">
         <v>4</v>
       </c>
-      <c r="J43" s="26" t="s">
+      <c r="J43" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="K43" s="20"/>
-      <c r="L43" s="18"/>
-      <c r="M43" s="20"/>
-      <c r="N43" s="26">
+      <c r="K43" s="15"/>
+      <c r="L43" s="13"/>
+      <c r="M43" s="15"/>
+      <c r="N43" s="18">
         <f t="shared" si="10"/>
         <v>94</v>
       </c>
-      <c r="O43" s="26">
+      <c r="O43" s="18">
         <v>11</v>
       </c>
-      <c r="P43" s="26">
+      <c r="P43" s="18">
         <v>4</v>
       </c>
-      <c r="Q43" s="26" t="s">
+      <c r="Q43" s="18" t="s">
         <v>163</v>
       </c>
-      <c r="R43" s="20"/>
-      <c r="S43" s="26">
+      <c r="R43" s="15"/>
+      <c r="S43" s="18">
         <f t="shared" si="11"/>
         <v>136</v>
       </c>
-      <c r="T43" s="26">
+      <c r="T43" s="18">
         <v>11</v>
       </c>
-      <c r="U43" s="26">
+      <c r="U43" s="18">
         <v>4</v>
       </c>
-      <c r="V43" s="26" t="s">
+      <c r="V43" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="W43" s="20"/>
+      <c r="W43" s="15"/>
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A44" s="20"/>
-      <c r="B44" s="26">
+      <c r="A44" s="15"/>
+      <c r="B44" s="18">
         <f t="shared" si="8"/>
         <v>9</v>
       </c>
-      <c r="C44" s="26">
+      <c r="C44" s="18">
         <v>10</v>
       </c>
-      <c r="D44" s="26">
+      <c r="D44" s="18">
         <v>5</v>
       </c>
-      <c r="E44" s="26" t="s">
+      <c r="E44" s="18" t="s">
         <v>189</v>
       </c>
-      <c r="F44" s="20"/>
-      <c r="G44" s="26">
+      <c r="F44" s="15"/>
+      <c r="G44" s="18">
         <f t="shared" si="9"/>
         <v>51</v>
       </c>
-      <c r="H44" s="26">
+      <c r="H44" s="18">
         <v>10</v>
       </c>
-      <c r="I44" s="26">
+      <c r="I44" s="18">
         <v>5</v>
       </c>
-      <c r="J44" s="26" t="s">
+      <c r="J44" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="K44" s="20"/>
-      <c r="L44" s="18"/>
-      <c r="M44" s="20"/>
-      <c r="N44" s="26">
+      <c r="K44" s="15"/>
+      <c r="L44" s="13"/>
+      <c r="M44" s="15"/>
+      <c r="N44" s="18">
         <f t="shared" si="10"/>
         <v>93</v>
       </c>
-      <c r="O44" s="26">
+      <c r="O44" s="18">
         <v>10</v>
       </c>
-      <c r="P44" s="26">
+      <c r="P44" s="18">
         <v>5</v>
       </c>
-      <c r="Q44" s="26" t="s">
+      <c r="Q44" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="R44" s="20"/>
-      <c r="S44" s="26">
+      <c r="R44" s="15"/>
+      <c r="S44" s="18">
         <f t="shared" si="11"/>
         <v>135</v>
       </c>
-      <c r="T44" s="26">
+      <c r="T44" s="18">
         <v>10</v>
       </c>
-      <c r="U44" s="26">
+      <c r="U44" s="18">
         <v>5</v>
       </c>
-      <c r="V44" s="26" t="s">
+      <c r="V44" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="W44" s="20"/>
+      <c r="W44" s="15"/>
     </row>
     <row r="45" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A45" s="20"/>
-      <c r="B45" s="26">
+      <c r="A45" s="15"/>
+      <c r="B45" s="18">
         <f t="shared" si="8"/>
         <v>8</v>
       </c>
-      <c r="C45" s="26">
+      <c r="C45" s="18">
         <v>9</v>
       </c>
-      <c r="D45" s="26">
+      <c r="D45" s="18">
         <v>6</v>
       </c>
-      <c r="E45" s="26" t="s">
+      <c r="E45" s="18" t="s">
         <v>176</v>
       </c>
-      <c r="F45" s="20"/>
-      <c r="G45" s="26">
+      <c r="F45" s="15"/>
+      <c r="G45" s="18">
         <f t="shared" si="9"/>
         <v>50</v>
       </c>
-      <c r="H45" s="26">
+      <c r="H45" s="18">
         <v>9</v>
       </c>
-      <c r="I45" s="26">
+      <c r="I45" s="18">
         <v>6</v>
       </c>
-      <c r="J45" s="26" t="s">
+      <c r="J45" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="K45" s="20"/>
-      <c r="L45" s="18"/>
-      <c r="M45" s="20"/>
-      <c r="N45" s="26">
+      <c r="K45" s="15"/>
+      <c r="L45" s="13"/>
+      <c r="M45" s="15"/>
+      <c r="N45" s="18">
         <f t="shared" si="10"/>
         <v>92</v>
       </c>
-      <c r="O45" s="26">
+      <c r="O45" s="18">
         <v>9</v>
       </c>
-      <c r="P45" s="26">
+      <c r="P45" s="18">
         <v>6</v>
       </c>
-      <c r="Q45" s="26" t="s">
+      <c r="Q45" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="R45" s="20"/>
-      <c r="S45" s="26">
+      <c r="R45" s="15"/>
+      <c r="S45" s="18">
         <f t="shared" si="11"/>
         <v>134</v>
       </c>
-      <c r="T45" s="26">
+      <c r="T45" s="18">
         <v>9</v>
       </c>
-      <c r="U45" s="26">
+      <c r="U45" s="18">
         <v>6</v>
       </c>
-      <c r="V45" s="26" t="s">
+      <c r="V45" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="W45" s="20"/>
+      <c r="W45" s="15"/>
     </row>
     <row r="46" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A46" s="20"/>
-      <c r="B46" s="26">
+      <c r="A46" s="15"/>
+      <c r="B46" s="18">
         <f t="shared" si="8"/>
         <v>7</v>
       </c>
-      <c r="C46" s="26">
+      <c r="C46" s="18">
         <v>8</v>
       </c>
-      <c r="D46" s="26">
+      <c r="D46" s="18">
         <v>7</v>
       </c>
-      <c r="E46" s="26" t="s">
+      <c r="E46" s="18" t="s">
         <v>150</v>
       </c>
-      <c r="F46" s="20"/>
-      <c r="G46" s="26">
+      <c r="F46" s="15"/>
+      <c r="G46" s="18">
         <f t="shared" si="9"/>
         <v>49</v>
       </c>
-      <c r="H46" s="26">
+      <c r="H46" s="18">
         <v>8</v>
       </c>
-      <c r="I46" s="26">
+      <c r="I46" s="18">
         <v>7</v>
       </c>
-      <c r="J46" s="26" t="s">
+      <c r="J46" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="K46" s="20"/>
-      <c r="L46" s="18"/>
-      <c r="M46" s="20"/>
-      <c r="N46" s="26">
+      <c r="K46" s="15"/>
+      <c r="L46" s="13"/>
+      <c r="M46" s="15"/>
+      <c r="N46" s="18">
         <f t="shared" si="10"/>
         <v>91</v>
       </c>
-      <c r="O46" s="26">
+      <c r="O46" s="18">
         <v>8</v>
       </c>
-      <c r="P46" s="26">
+      <c r="P46" s="18">
         <v>7</v>
       </c>
-      <c r="Q46" s="26" t="s">
+      <c r="Q46" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="R46" s="20"/>
-      <c r="S46" s="26">
+      <c r="R46" s="15"/>
+      <c r="S46" s="18">
         <f t="shared" si="11"/>
         <v>133</v>
       </c>
-      <c r="T46" s="26">
+      <c r="T46" s="18">
         <v>8</v>
       </c>
-      <c r="U46" s="26">
+      <c r="U46" s="18">
         <v>7</v>
       </c>
-      <c r="V46" s="26" t="s">
+      <c r="V46" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="W46" s="20"/>
+      <c r="W46" s="15"/>
     </row>
     <row r="47" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A47" s="20"/>
-      <c r="B47" s="26">
+      <c r="A47" s="15"/>
+      <c r="B47" s="18">
         <f t="shared" si="8"/>
         <v>6</v>
       </c>
-      <c r="C47" s="26">
+      <c r="C47" s="18">
         <v>7</v>
       </c>
-      <c r="D47" s="26">
+      <c r="D47" s="18">
         <v>8</v>
       </c>
-      <c r="E47" s="26" t="s">
+      <c r="E47" s="18" t="s">
         <v>164</v>
       </c>
-      <c r="F47" s="20"/>
-      <c r="G47" s="26">
+      <c r="F47" s="15"/>
+      <c r="G47" s="18">
         <f t="shared" si="9"/>
         <v>48</v>
       </c>
-      <c r="H47" s="26">
+      <c r="H47" s="18">
         <v>7</v>
       </c>
-      <c r="I47" s="26">
+      <c r="I47" s="18">
         <v>8</v>
       </c>
-      <c r="J47" s="26" t="s">
+      <c r="J47" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="K47" s="20"/>
-      <c r="L47" s="18"/>
-      <c r="M47" s="20"/>
-      <c r="N47" s="26">
+      <c r="K47" s="15"/>
+      <c r="L47" s="13"/>
+      <c r="M47" s="15"/>
+      <c r="N47" s="18">
         <f t="shared" si="10"/>
         <v>90</v>
       </c>
-      <c r="O47" s="26">
+      <c r="O47" s="18">
         <v>7</v>
       </c>
-      <c r="P47" s="26">
+      <c r="P47" s="18">
         <v>8</v>
       </c>
-      <c r="Q47" s="26" t="s">
+      <c r="Q47" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="R47" s="20"/>
-      <c r="S47" s="26">
+      <c r="R47" s="15"/>
+      <c r="S47" s="18">
         <f t="shared" si="11"/>
         <v>132</v>
       </c>
-      <c r="T47" s="26">
+      <c r="T47" s="18">
         <v>7</v>
       </c>
-      <c r="U47" s="26">
+      <c r="U47" s="18">
         <v>8</v>
       </c>
-      <c r="V47" s="26" t="s">
+      <c r="V47" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="W47" s="20"/>
+      <c r="W47" s="15"/>
     </row>
     <row r="48" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A48" s="20"/>
-      <c r="B48" s="26">
+      <c r="A48" s="15"/>
+      <c r="B48" s="18">
         <f t="shared" si="8"/>
         <v>5</v>
       </c>
-      <c r="C48" s="26">
+      <c r="C48" s="18">
         <v>6</v>
       </c>
-      <c r="D48" s="26">
+      <c r="D48" s="18">
         <v>9</v>
       </c>
-      <c r="E48" s="26" t="s">
+      <c r="E48" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="F48" s="20"/>
-      <c r="G48" s="26">
+      <c r="F48" s="15"/>
+      <c r="G48" s="18">
         <f t="shared" si="9"/>
         <v>47</v>
       </c>
-      <c r="H48" s="26">
+      <c r="H48" s="18">
         <v>6</v>
       </c>
-      <c r="I48" s="26">
+      <c r="I48" s="18">
         <v>9</v>
       </c>
-      <c r="J48" s="26" t="s">
+      <c r="J48" s="18" t="s">
         <v>203</v>
       </c>
-      <c r="K48" s="20"/>
-      <c r="L48" s="18"/>
-      <c r="M48" s="20"/>
-      <c r="N48" s="26">
+      <c r="K48" s="15"/>
+      <c r="L48" s="13"/>
+      <c r="M48" s="15"/>
+      <c r="N48" s="18">
         <f t="shared" si="10"/>
         <v>89</v>
       </c>
-      <c r="O48" s="26">
+      <c r="O48" s="18">
         <v>6</v>
       </c>
-      <c r="P48" s="26">
+      <c r="P48" s="18">
         <v>9</v>
       </c>
-      <c r="Q48" s="26" t="s">
+      <c r="Q48" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="R48" s="20"/>
-      <c r="S48" s="26">
+      <c r="R48" s="15"/>
+      <c r="S48" s="18">
         <f t="shared" si="11"/>
         <v>131</v>
       </c>
-      <c r="T48" s="26">
+      <c r="T48" s="18">
         <v>6</v>
       </c>
-      <c r="U48" s="26">
+      <c r="U48" s="18">
         <v>9</v>
       </c>
-      <c r="V48" s="26" t="s">
+      <c r="V48" s="18" t="s">
         <v>204</v>
       </c>
-      <c r="W48" s="20"/>
+      <c r="W48" s="15"/>
     </row>
     <row r="49" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A49" s="20"/>
-      <c r="B49" s="26">
+      <c r="A49" s="15"/>
+      <c r="B49" s="18">
         <f t="shared" si="8"/>
         <v>4</v>
       </c>
-      <c r="C49" s="26">
+      <c r="C49" s="18">
         <v>5</v>
       </c>
-      <c r="D49" s="26">
+      <c r="D49" s="18">
         <v>10</v>
       </c>
-      <c r="E49" s="26" t="s">
+      <c r="E49" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="F49" s="20"/>
-      <c r="G49" s="26">
+      <c r="F49" s="15"/>
+      <c r="G49" s="18">
         <f t="shared" si="9"/>
         <v>46</v>
       </c>
-      <c r="H49" s="26">
+      <c r="H49" s="18">
         <v>5</v>
       </c>
-      <c r="I49" s="26">
+      <c r="I49" s="18">
         <v>10</v>
       </c>
-      <c r="J49" s="26" t="s">
+      <c r="J49" s="18" t="s">
         <v>216</v>
       </c>
-      <c r="K49" s="20"/>
-      <c r="L49" s="18"/>
-      <c r="M49" s="20"/>
-      <c r="N49" s="26">
+      <c r="K49" s="15"/>
+      <c r="L49" s="13"/>
+      <c r="M49" s="15"/>
+      <c r="N49" s="18">
         <f t="shared" si="10"/>
         <v>88</v>
       </c>
-      <c r="O49" s="26">
+      <c r="O49" s="18">
         <v>5</v>
       </c>
-      <c r="P49" s="26">
+      <c r="P49" s="18">
         <v>10</v>
       </c>
-      <c r="Q49" s="26" t="s">
+      <c r="Q49" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="R49" s="20"/>
-      <c r="S49" s="26">
+      <c r="R49" s="15"/>
+      <c r="S49" s="18">
         <f t="shared" si="11"/>
         <v>130</v>
       </c>
-      <c r="T49" s="26">
+      <c r="T49" s="18">
         <v>5</v>
       </c>
-      <c r="U49" s="26">
+      <c r="U49" s="18">
         <v>10</v>
       </c>
-      <c r="V49" s="26" t="s">
+      <c r="V49" s="18" t="s">
         <v>217</v>
       </c>
-      <c r="W49" s="20"/>
+      <c r="W49" s="15"/>
     </row>
     <row r="50" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A50" s="20"/>
-      <c r="B50" s="26">
+      <c r="A50" s="15"/>
+      <c r="B50" s="18">
         <f t="shared" si="8"/>
         <v>3</v>
       </c>
-      <c r="C50" s="26">
+      <c r="C50" s="18">
         <v>4</v>
       </c>
-      <c r="D50" s="26">
+      <c r="D50" s="18">
         <v>11</v>
       </c>
-      <c r="E50" s="26" t="s">
+      <c r="E50" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="F50" s="20"/>
-      <c r="G50" s="26">
+      <c r="F50" s="15"/>
+      <c r="G50" s="18">
         <f t="shared" si="9"/>
         <v>45</v>
       </c>
-      <c r="H50" s="26">
+      <c r="H50" s="18">
         <v>4</v>
       </c>
-      <c r="I50" s="26">
+      <c r="I50" s="18">
         <v>11</v>
       </c>
-      <c r="J50" s="26" t="s">
+      <c r="J50" s="18" t="s">
         <v>190</v>
       </c>
-      <c r="K50" s="20"/>
-      <c r="L50" s="18"/>
-      <c r="M50" s="20"/>
-      <c r="N50" s="26">
+      <c r="K50" s="15"/>
+      <c r="L50" s="13"/>
+      <c r="M50" s="15"/>
+      <c r="N50" s="18">
         <f t="shared" si="10"/>
         <v>87</v>
       </c>
-      <c r="O50" s="26">
+      <c r="O50" s="18">
         <v>4</v>
       </c>
-      <c r="P50" s="26">
+      <c r="P50" s="18">
         <v>11</v>
       </c>
-      <c r="Q50" s="26" t="s">
+      <c r="Q50" s="18" t="s">
         <v>205</v>
       </c>
-      <c r="R50" s="20"/>
-      <c r="S50" s="26">
+      <c r="R50" s="15"/>
+      <c r="S50" s="18">
         <f t="shared" si="11"/>
         <v>129</v>
       </c>
-      <c r="T50" s="26">
+      <c r="T50" s="18">
         <v>4</v>
       </c>
-      <c r="U50" s="26">
+      <c r="U50" s="18">
         <v>11</v>
       </c>
-      <c r="V50" s="26" t="s">
+      <c r="V50" s="18" t="s">
         <v>191</v>
       </c>
-      <c r="W50" s="20"/>
+      <c r="W50" s="15"/>
     </row>
     <row r="51" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A51" s="20"/>
-      <c r="B51" s="26">
+      <c r="A51" s="15"/>
+      <c r="B51" s="18">
         <f t="shared" si="8"/>
         <v>2</v>
       </c>
-      <c r="C51" s="26">
+      <c r="C51" s="18">
         <v>3</v>
       </c>
-      <c r="D51" s="26">
+      <c r="D51" s="18">
         <v>12</v>
       </c>
-      <c r="E51" s="26" t="s">
+      <c r="E51" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="F51" s="20"/>
-      <c r="G51" s="26">
+      <c r="F51" s="15"/>
+      <c r="G51" s="18">
         <f t="shared" si="9"/>
         <v>44</v>
       </c>
-      <c r="H51" s="26">
+      <c r="H51" s="18">
         <v>3</v>
       </c>
-      <c r="I51" s="26">
+      <c r="I51" s="18">
         <v>12</v>
       </c>
-      <c r="J51" s="26" t="s">
+      <c r="J51" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="K51" s="20"/>
-      <c r="L51" s="18"/>
-      <c r="M51" s="20"/>
-      <c r="N51" s="26">
+      <c r="K51" s="15"/>
+      <c r="L51" s="13"/>
+      <c r="M51" s="15"/>
+      <c r="N51" s="18">
         <f t="shared" si="10"/>
         <v>86</v>
       </c>
-      <c r="O51" s="26">
+      <c r="O51" s="18">
         <v>3</v>
       </c>
-      <c r="P51" s="26">
+      <c r="P51" s="18">
         <v>12</v>
       </c>
-      <c r="Q51" s="26" t="s">
+      <c r="Q51" s="18" t="s">
         <v>218</v>
       </c>
-      <c r="R51" s="20"/>
-      <c r="S51" s="26">
+      <c r="R51" s="15"/>
+      <c r="S51" s="18">
         <f t="shared" si="11"/>
         <v>128</v>
       </c>
-      <c r="T51" s="26">
+      <c r="T51" s="18">
         <v>3</v>
       </c>
-      <c r="U51" s="26">
+      <c r="U51" s="18">
         <v>12</v>
       </c>
-      <c r="V51" s="26" t="s">
+      <c r="V51" s="18" t="s">
         <v>178</v>
       </c>
-      <c r="W51" s="20"/>
+      <c r="W51" s="15"/>
     </row>
     <row r="52" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A52" s="20"/>
-      <c r="B52" s="26">
+      <c r="A52" s="15"/>
+      <c r="B52" s="18">
         <f>B53+1</f>
         <v>1</v>
       </c>
-      <c r="C52" s="26">
+      <c r="C52" s="18">
         <v>2</v>
       </c>
-      <c r="D52" s="26">
+      <c r="D52" s="18">
         <v>13</v>
       </c>
-      <c r="E52" s="26" t="s">
+      <c r="E52" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="F52" s="20"/>
-      <c r="G52" s="26">
+      <c r="F52" s="15"/>
+      <c r="G52" s="18">
         <f>G53+1</f>
         <v>43</v>
       </c>
-      <c r="H52" s="26">
+      <c r="H52" s="18">
         <v>2</v>
       </c>
-      <c r="I52" s="26">
+      <c r="I52" s="18">
         <v>13</v>
       </c>
-      <c r="J52" s="26" t="s">
+      <c r="J52" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="K52" s="20"/>
-      <c r="L52" s="18"/>
-      <c r="M52" s="20"/>
-      <c r="N52" s="26">
+      <c r="K52" s="15"/>
+      <c r="L52" s="13"/>
+      <c r="M52" s="15"/>
+      <c r="N52" s="18">
         <f>N53+1</f>
         <v>85</v>
       </c>
-      <c r="O52" s="26">
+      <c r="O52" s="18">
         <v>2</v>
       </c>
-      <c r="P52" s="26">
+      <c r="P52" s="18">
         <v>13</v>
       </c>
-      <c r="Q52" s="26" t="s">
+      <c r="Q52" s="18" t="s">
         <v>192</v>
       </c>
-      <c r="R52" s="20"/>
-      <c r="S52" s="26">
+      <c r="R52" s="15"/>
+      <c r="S52" s="18">
         <f>S53+1</f>
         <v>127</v>
       </c>
-      <c r="T52" s="26">
+      <c r="T52" s="18">
         <v>2</v>
       </c>
-      <c r="U52" s="26">
+      <c r="U52" s="18">
         <v>13</v>
       </c>
-      <c r="V52" s="26" t="s">
+      <c r="V52" s="18" t="s">
         <v>152</v>
       </c>
-      <c r="W52" s="20"/>
+      <c r="W52" s="15"/>
     </row>
     <row r="53" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A53" s="20"/>
-      <c r="B53" s="26">
+      <c r="A53" s="15"/>
+      <c r="B53" s="18">
         <v>0</v>
       </c>
-      <c r="C53" s="26">
+      <c r="C53" s="18">
         <v>1</v>
       </c>
-      <c r="D53" s="26">
+      <c r="D53" s="18">
         <v>14</v>
       </c>
-      <c r="E53" s="26" t="s">
+      <c r="E53" s="18" t="s">
         <v>219</v>
       </c>
-      <c r="F53" s="20"/>
-      <c r="G53" s="26">
+      <c r="F53" s="15"/>
+      <c r="G53" s="18">
         <f>B6+1</f>
         <v>42</v>
       </c>
-      <c r="H53" s="26">
+      <c r="H53" s="18">
         <v>1</v>
       </c>
-      <c r="I53" s="26">
+      <c r="I53" s="18">
         <v>14</v>
       </c>
-      <c r="J53" s="26" t="s">
+      <c r="J53" s="18" t="s">
         <v>165</v>
       </c>
-      <c r="K53" s="20"/>
-      <c r="L53" s="18"/>
-      <c r="M53" s="20"/>
-      <c r="N53" s="26">
+      <c r="K53" s="15"/>
+      <c r="L53" s="13"/>
+      <c r="M53" s="15"/>
+      <c r="N53" s="18">
         <f>G6+1</f>
         <v>84</v>
       </c>
-      <c r="O53" s="26">
+      <c r="O53" s="18">
         <v>1</v>
       </c>
-      <c r="P53" s="26">
+      <c r="P53" s="18">
         <v>14</v>
       </c>
-      <c r="Q53" s="26" t="s">
+      <c r="Q53" s="18" t="s">
         <v>179</v>
       </c>
-      <c r="R53" s="20"/>
-      <c r="S53" s="26">
+      <c r="R53" s="15"/>
+      <c r="S53" s="18">
         <f>N6+1</f>
         <v>126</v>
       </c>
-      <c r="T53" s="26">
+      <c r="T53" s="18">
         <v>1</v>
       </c>
-      <c r="U53" s="26">
+      <c r="U53" s="18">
         <v>14</v>
       </c>
-      <c r="V53" s="26" t="s">
+      <c r="V53" s="18" t="s">
         <v>166</v>
       </c>
-      <c r="W53" s="20"/>
+      <c r="W53" s="15"/>
     </row>
     <row r="54" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A54" s="20"/>
-      <c r="B54" s="20"/>
-      <c r="C54" s="20"/>
-      <c r="D54" s="20"/>
-      <c r="E54" s="20"/>
-      <c r="F54" s="20"/>
-      <c r="G54" s="20"/>
-      <c r="H54" s="20"/>
-      <c r="I54" s="20"/>
-      <c r="J54" s="20"/>
-      <c r="K54" s="20"/>
-      <c r="L54" s="18"/>
-      <c r="M54" s="20"/>
-      <c r="N54" s="20"/>
-      <c r="O54" s="20"/>
-      <c r="P54" s="20"/>
-      <c r="Q54" s="20"/>
-      <c r="R54" s="20"/>
-      <c r="S54" s="20"/>
-      <c r="T54" s="20"/>
-      <c r="U54" s="20"/>
-      <c r="V54" s="20"/>
-      <c r="W54" s="20"/>
+      <c r="A54" s="15"/>
+      <c r="B54" s="15"/>
+      <c r="C54" s="15"/>
+      <c r="D54" s="15"/>
+      <c r="E54" s="15"/>
+      <c r="F54" s="15"/>
+      <c r="G54" s="15"/>
+      <c r="H54" s="15"/>
+      <c r="I54" s="15"/>
+      <c r="J54" s="15"/>
+      <c r="K54" s="15"/>
+      <c r="L54" s="13"/>
+      <c r="M54" s="15"/>
+      <c r="N54" s="15"/>
+      <c r="O54" s="15"/>
+      <c r="P54" s="15"/>
+      <c r="Q54" s="15"/>
+      <c r="R54" s="15"/>
+      <c r="S54" s="15"/>
+      <c r="T54" s="15"/>
+      <c r="U54" s="15"/>
+      <c r="V54" s="15"/>
+      <c r="W54" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -4243,35 +4242,35 @@
   <sheetData>
     <row r="1" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
       <c r="E1" s="2"/>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
       <c r="I1" s="2"/>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
       <c r="M1" s="2"/>
-      <c r="N1" s="14" t="s">
+      <c r="N1" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
       <c r="Q1" s="2"/>
-      <c r="R1" s="12" t="s">
+      <c r="R1" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
       <c r="U1" s="2"/>
     </row>
     <row r="2" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4854,35 +4853,35 @@
     </row>
     <row r="16" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1"/>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="12" t="s">
+      <c r="F16" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="28"/>
       <c r="I16" s="2"/>
-      <c r="J16" s="12" t="s">
+      <c r="J16" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
+      <c r="K16" s="28"/>
+      <c r="L16" s="28"/>
       <c r="M16" s="2"/>
-      <c r="N16" s="14" t="s">
+      <c r="N16" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="O16" s="13"/>
-      <c r="P16" s="13"/>
+      <c r="O16" s="28"/>
+      <c r="P16" s="28"/>
       <c r="Q16" s="2"/>
-      <c r="R16" s="12" t="s">
+      <c r="R16" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="S16" s="13"/>
-      <c r="T16" s="13"/>
+      <c r="S16" s="28"/>
+      <c r="T16" s="28"/>
       <c r="U16" s="2"/>
     </row>
     <row r="17" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -5483,35 +5482,35 @@
     </row>
     <row r="31" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="2"/>
-      <c r="B31" s="12" t="s">
+      <c r="B31" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
+      <c r="C31" s="28"/>
+      <c r="D31" s="28"/>
       <c r="E31" s="2"/>
-      <c r="F31" s="12" t="s">
+      <c r="F31" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="G31" s="13"/>
-      <c r="H31" s="13"/>
+      <c r="G31" s="28"/>
+      <c r="H31" s="28"/>
       <c r="I31" s="2"/>
-      <c r="J31" s="14" t="s">
+      <c r="J31" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="K31" s="13"/>
-      <c r="L31" s="13"/>
+      <c r="K31" s="28"/>
+      <c r="L31" s="28"/>
       <c r="M31" s="2"/>
-      <c r="N31" s="12" t="s">
+      <c r="N31" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="O31" s="13"/>
-      <c r="P31" s="13"/>
+      <c r="O31" s="28"/>
+      <c r="P31" s="28"/>
       <c r="Q31" s="2"/>
-      <c r="R31" s="12" t="s">
+      <c r="R31" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="S31" s="13"/>
-      <c r="T31" s="13"/>
+      <c r="S31" s="28"/>
+      <c r="T31" s="28"/>
       <c r="U31" s="2"/>
       <c r="V31" s="7"/>
     </row>

</xml_diff>

<commit_message>
updated tdc cable map
</commit_message>
<xml_diff>
--- a/Cables and Labels/CableMapping.xlsx
+++ b/Cables and Labels/CableMapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/spaubt/Desktop/CDet/Cables and Labels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{655D13E3-B776-624D-B679-ADE613963D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9765643D-E4F5-164E-BEF4-AB0BC65C2A83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="740" windowWidth="26300" windowHeight="16680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-960" yWindow="800" windowWidth="26000" windowHeight="16680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cdet TDC Cable Map" sheetId="4" r:id="rId1"/>
@@ -176,480 +176,6 @@
     <t>DAQ Slot</t>
   </si>
   <si>
-    <t>10 A-L</t>
-  </si>
-  <si>
-    <t>6 A-L</t>
-  </si>
-  <si>
-    <t>16 A-L</t>
-  </si>
-  <si>
-    <t>19 A-L</t>
-  </si>
-  <si>
-    <t>15 A-L</t>
-  </si>
-  <si>
-    <t>9 A-L</t>
-  </si>
-  <si>
-    <t>5 A-L</t>
-  </si>
-  <si>
-    <t>18 A-L</t>
-  </si>
-  <si>
-    <t>8 A-L</t>
-  </si>
-  <si>
-    <t>4 A-L</t>
-  </si>
-  <si>
-    <t>7 A-L</t>
-  </si>
-  <si>
-    <t>17 A-L</t>
-  </si>
-  <si>
-    <t>10 A-R</t>
-  </si>
-  <si>
-    <t>6 A-R</t>
-  </si>
-  <si>
-    <t>16 A-R</t>
-  </si>
-  <si>
-    <t>19 A-R</t>
-  </si>
-  <si>
-    <t>15 A-R</t>
-  </si>
-  <si>
-    <t>9 A-R</t>
-  </si>
-  <si>
-    <t>5 A-R</t>
-  </si>
-  <si>
-    <t>18 A-R</t>
-  </si>
-  <si>
-    <t>8 A-R</t>
-  </si>
-  <si>
-    <t>4 A-R</t>
-  </si>
-  <si>
-    <t>7 A-R</t>
-  </si>
-  <si>
-    <t>17 A-R</t>
-  </si>
-  <si>
-    <t>3 A-R</t>
-  </si>
-  <si>
-    <t>10 B-R</t>
-  </si>
-  <si>
-    <t>6 B-R</t>
-  </si>
-  <si>
-    <t>16 B-R</t>
-  </si>
-  <si>
-    <t>19 B-R</t>
-  </si>
-  <si>
-    <t>15 B-R</t>
-  </si>
-  <si>
-    <t>9 B-R</t>
-  </si>
-  <si>
-    <t>5 B-R</t>
-  </si>
-  <si>
-    <t>18 B-R</t>
-  </si>
-  <si>
-    <t>14 B-R</t>
-  </si>
-  <si>
-    <t>8 B-R</t>
-  </si>
-  <si>
-    <t>4 B-R</t>
-  </si>
-  <si>
-    <t>7 B-R</t>
-  </si>
-  <si>
-    <t>17 B-R</t>
-  </si>
-  <si>
-    <t>3 B-R</t>
-  </si>
-  <si>
-    <t>10 B-L</t>
-  </si>
-  <si>
-    <t>6 B-L</t>
-  </si>
-  <si>
-    <t>16 B-L</t>
-  </si>
-  <si>
-    <t>19 B-L</t>
-  </si>
-  <si>
-    <t>15 B-L</t>
-  </si>
-  <si>
-    <t>9 B-L</t>
-  </si>
-  <si>
-    <t>5 B-L</t>
-  </si>
-  <si>
-    <t>18 B-L</t>
-  </si>
-  <si>
-    <t>14 B-L</t>
-  </si>
-  <si>
-    <t>8 B-L</t>
-  </si>
-  <si>
-    <t>4 B-L</t>
-  </si>
-  <si>
-    <t>7 B-L</t>
-  </si>
-  <si>
-    <t>17 B-L</t>
-  </si>
-  <si>
-    <t>3 B-L</t>
-  </si>
-  <si>
-    <t>6 C-L</t>
-  </si>
-  <si>
-    <t>16 C-L</t>
-  </si>
-  <si>
-    <t>19 C-L</t>
-  </si>
-  <si>
-    <t>15 C-L</t>
-  </si>
-  <si>
-    <t>9 C-L</t>
-  </si>
-  <si>
-    <t>5 C-L</t>
-  </si>
-  <si>
-    <t>18 C-L</t>
-  </si>
-  <si>
-    <t>14 C-L</t>
-  </si>
-  <si>
-    <t>8 C-L</t>
-  </si>
-  <si>
-    <t>4 C-L</t>
-  </si>
-  <si>
-    <t>7 C-L</t>
-  </si>
-  <si>
-    <t>17 C-L</t>
-  </si>
-  <si>
-    <t>3 C-L</t>
-  </si>
-  <si>
-    <t>6 C-R</t>
-  </si>
-  <si>
-    <t>16 C-R</t>
-  </si>
-  <si>
-    <t>19 C-R</t>
-  </si>
-  <si>
-    <t>15 C-R</t>
-  </si>
-  <si>
-    <t>9 C-R</t>
-  </si>
-  <si>
-    <t>5 C-R</t>
-  </si>
-  <si>
-    <t>18 C-R</t>
-  </si>
-  <si>
-    <t>14 C-R</t>
-  </si>
-  <si>
-    <t>8 C-R</t>
-  </si>
-  <si>
-    <t>4 C-R</t>
-  </si>
-  <si>
-    <t>7 C-R</t>
-  </si>
-  <si>
-    <t>17 C-R</t>
-  </si>
-  <si>
-    <t>3 C-R</t>
-  </si>
-  <si>
-    <t>19 D-R</t>
-  </si>
-  <si>
-    <t>15 D-R</t>
-  </si>
-  <si>
-    <t>9 D-R</t>
-  </si>
-  <si>
-    <t>5 D-R</t>
-  </si>
-  <si>
-    <t>18 D-R</t>
-  </si>
-  <si>
-    <t>14 D-R</t>
-  </si>
-  <si>
-    <t>8 D-R</t>
-  </si>
-  <si>
-    <t>4 D-R</t>
-  </si>
-  <si>
-    <t>7 D-R</t>
-  </si>
-  <si>
-    <t>17 D-R</t>
-  </si>
-  <si>
-    <t>3 D-R</t>
-  </si>
-  <si>
-    <t>6 D-R</t>
-  </si>
-  <si>
-    <t>16 D-R</t>
-  </si>
-  <si>
-    <t>19 D-L</t>
-  </si>
-  <si>
-    <t>15 D-L</t>
-  </si>
-  <si>
-    <t>9 D-L</t>
-  </si>
-  <si>
-    <t>5 D-L</t>
-  </si>
-  <si>
-    <t>18 D-L</t>
-  </si>
-  <si>
-    <t>14 D-L</t>
-  </si>
-  <si>
-    <t>8 D-L</t>
-  </si>
-  <si>
-    <t>4 D-L</t>
-  </si>
-  <si>
-    <t>7 D-L</t>
-  </si>
-  <si>
-    <t>17 D-L</t>
-  </si>
-  <si>
-    <t>3 D-L</t>
-  </si>
-  <si>
-    <t>6 D-L</t>
-  </si>
-  <si>
-    <t>16 D-L</t>
-  </si>
-  <si>
-    <t>19 F-L</t>
-  </si>
-  <si>
-    <t>9 F-L</t>
-  </si>
-  <si>
-    <t>5 F-L</t>
-  </si>
-  <si>
-    <t>18 F-L</t>
-  </si>
-  <si>
-    <t>14 F-L</t>
-  </si>
-  <si>
-    <t>8 F-L</t>
-  </si>
-  <si>
-    <t>4 F-L</t>
-  </si>
-  <si>
-    <t>17 F-L</t>
-  </si>
-  <si>
-    <t>13 F-L</t>
-  </si>
-  <si>
-    <t>3 F-L</t>
-  </si>
-  <si>
-    <t>6 F-L</t>
-  </si>
-  <si>
-    <t>16 F-L</t>
-  </si>
-  <si>
-    <t>10 F-L</t>
-  </si>
-  <si>
-    <t>19 F-R</t>
-  </si>
-  <si>
-    <t>9 F-R</t>
-  </si>
-  <si>
-    <t>5 F-R</t>
-  </si>
-  <si>
-    <t>18 F-R</t>
-  </si>
-  <si>
-    <t>14 F-R</t>
-  </si>
-  <si>
-    <t>8 F-R</t>
-  </si>
-  <si>
-    <t>4 F-R</t>
-  </si>
-  <si>
-    <t>17 F-R</t>
-  </si>
-  <si>
-    <t>13 F-R</t>
-  </si>
-  <si>
-    <t>3 F-R</t>
-  </si>
-  <si>
-    <t>6 F-R</t>
-  </si>
-  <si>
-    <t>16 F-R</t>
-  </si>
-  <si>
-    <t>10 F-R</t>
-  </si>
-  <si>
-    <t>19 G-R</t>
-  </si>
-  <si>
-    <t>9 G-R</t>
-  </si>
-  <si>
-    <t>5 G-R</t>
-  </si>
-  <si>
-    <t>18 G-R</t>
-  </si>
-  <si>
-    <t>14 G-R</t>
-  </si>
-  <si>
-    <t>8 G-R</t>
-  </si>
-  <si>
-    <t>4 G-R</t>
-  </si>
-  <si>
-    <t>17 G-R</t>
-  </si>
-  <si>
-    <t>13 G-R</t>
-  </si>
-  <si>
-    <t>3 G-R</t>
-  </si>
-  <si>
-    <t>6 G-R</t>
-  </si>
-  <si>
-    <t>16 G-R</t>
-  </si>
-  <si>
-    <t>10 G-R</t>
-  </si>
-  <si>
-    <t>19 G-L</t>
-  </si>
-  <si>
-    <t>9 G-L</t>
-  </si>
-  <si>
-    <t>5 G-L</t>
-  </si>
-  <si>
-    <t>18 G-L</t>
-  </si>
-  <si>
-    <t>14 G-L</t>
-  </si>
-  <si>
-    <t>8 G-L</t>
-  </si>
-  <si>
-    <t>4 G-L</t>
-  </si>
-  <si>
-    <t>17 G-L</t>
-  </si>
-  <si>
-    <t>13 G-L</t>
-  </si>
-  <si>
-    <t>3 G-L</t>
-  </si>
-  <si>
-    <t>6 G-L</t>
-  </si>
-  <si>
-    <t>16 G-L</t>
-  </si>
-  <si>
-    <t>10 G-L</t>
-  </si>
-  <si>
-    <t>3 A-L</t>
-  </si>
-  <si>
     <t>GUI Label</t>
   </si>
   <si>
@@ -1163,45 +689,526 @@
     <t>&lt;- UNUSED</t>
   </si>
   <si>
-    <t>20 D-R</t>
-  </si>
-  <si>
-    <t>20 D-L</t>
-  </si>
-  <si>
-    <t>20 C-R</t>
-  </si>
-  <si>
-    <t>20 C-L</t>
-  </si>
-  <si>
-    <t>20 B-R</t>
-  </si>
-  <si>
-    <t>20 B-L</t>
-  </si>
-  <si>
-    <t>20 A-R</t>
-  </si>
-  <si>
-    <t>20 A-L</t>
-  </si>
-  <si>
-    <t>10 D-L</t>
-  </si>
-  <si>
-    <t>10 D-R</t>
+    <t>10, 48-63</t>
+  </si>
+  <si>
+    <t>10, 32-47</t>
+  </si>
+  <si>
+    <t>10, 16-31</t>
+  </si>
+  <si>
+    <t>10, 0-15</t>
+  </si>
+  <si>
+    <t>6, 0-15</t>
+  </si>
+  <si>
+    <t>17, 0-15</t>
+  </si>
+  <si>
+    <t>20, 0-15</t>
+  </si>
+  <si>
+    <t>16, 0-15</t>
+  </si>
+  <si>
+    <t>9, 0-15</t>
+  </si>
+  <si>
+    <t>5, 0-15</t>
+  </si>
+  <si>
+    <t>19, 0-15</t>
+  </si>
+  <si>
+    <t>15, 0-15</t>
+  </si>
+  <si>
+    <t>8, 0-15</t>
+  </si>
+  <si>
+    <t>4, 0-15</t>
+  </si>
+  <si>
+    <t>7, 0-15</t>
+  </si>
+  <si>
+    <t>18, 0-15</t>
+  </si>
+  <si>
+    <t>3, 0-15</t>
+  </si>
+  <si>
+    <t>6, 16-31</t>
+  </si>
+  <si>
+    <t>17, 16-31</t>
+  </si>
+  <si>
+    <t>20, 16-31</t>
+  </si>
+  <si>
+    <t>16, 16-31</t>
+  </si>
+  <si>
+    <t>9, 16-31</t>
+  </si>
+  <si>
+    <t>5, 16-31</t>
+  </si>
+  <si>
+    <t>19, 16-31</t>
+  </si>
+  <si>
+    <t>15, 16-31</t>
+  </si>
+  <si>
+    <t>8, 16-31</t>
+  </si>
+  <si>
+    <t>4, 16-31</t>
+  </si>
+  <si>
+    <t>7, 16-31</t>
+  </si>
+  <si>
+    <t>18, 16-31</t>
+  </si>
+  <si>
+    <t>3, 16-31</t>
+  </si>
+  <si>
+    <t>6, 32-47</t>
+  </si>
+  <si>
+    <t>17, 32-47</t>
+  </si>
+  <si>
+    <t>20, 32-47</t>
+  </si>
+  <si>
+    <t>16, 32-47</t>
+  </si>
+  <si>
+    <t>9, 32-47</t>
+  </si>
+  <si>
+    <t>5, 32-47</t>
+  </si>
+  <si>
+    <t>19, 32-47</t>
+  </si>
+  <si>
+    <t>15, 32-47</t>
+  </si>
+  <si>
+    <t>8, 32-47</t>
+  </si>
+  <si>
+    <t>4, 32-47</t>
+  </si>
+  <si>
+    <t>7, 32-47</t>
+  </si>
+  <si>
+    <t>18, 32-47</t>
+  </si>
+  <si>
+    <t>14, 32-47</t>
+  </si>
+  <si>
+    <t>3, 32-47</t>
+  </si>
+  <si>
+    <t>6, 48-63</t>
+  </si>
+  <si>
+    <t>17, 48-63</t>
+  </si>
+  <si>
+    <t>20, 48-63</t>
+  </si>
+  <si>
+    <t>16, 48-63</t>
+  </si>
+  <si>
+    <t>9, 48-63</t>
+  </si>
+  <si>
+    <t>5, 48-63</t>
+  </si>
+  <si>
+    <t>19, 48-63</t>
+  </si>
+  <si>
+    <t>15, 48-63</t>
+  </si>
+  <si>
+    <t>8, 48-63</t>
+  </si>
+  <si>
+    <t>4, 48-63</t>
+  </si>
+  <si>
+    <t>7, 48-63</t>
+  </si>
+  <si>
+    <t>18, 48-63</t>
+  </si>
+  <si>
+    <t>14, 48-63</t>
+  </si>
+  <si>
+    <t>3, 48-63</t>
+  </si>
+  <si>
+    <t>6, 64-79</t>
+  </si>
+  <si>
+    <t>17, 64-79</t>
+  </si>
+  <si>
+    <t>20, 64-79</t>
+  </si>
+  <si>
+    <t>16, 64-79</t>
+  </si>
+  <si>
+    <t>9, 64-79</t>
+  </si>
+  <si>
+    <t>5, 64-79</t>
+  </si>
+  <si>
+    <t>19, 64-79</t>
+  </si>
+  <si>
+    <t>15, 64-79</t>
+  </si>
+  <si>
+    <t>8, 64-79</t>
+  </si>
+  <si>
+    <t>4, 64-79</t>
+  </si>
+  <si>
+    <t>7, 64-79</t>
+  </si>
+  <si>
+    <t>18, 64-79</t>
+  </si>
+  <si>
+    <t>14, 64-79</t>
+  </si>
+  <si>
+    <t>3, 64-79</t>
+  </si>
+  <si>
+    <t>6, 80-95</t>
+  </si>
+  <si>
+    <t>17, 80-95</t>
+  </si>
+  <si>
+    <t>20, 80-95</t>
+  </si>
+  <si>
+    <t>16, 80-95</t>
+  </si>
+  <si>
+    <t>9, 80-95</t>
+  </si>
+  <si>
+    <t>5, 80-95</t>
+  </si>
+  <si>
+    <t>19, 80-95</t>
+  </si>
+  <si>
+    <t>15, 80-95</t>
+  </si>
+  <si>
+    <t>8, 80-95</t>
+  </si>
+  <si>
+    <t>4, 80-95</t>
+  </si>
+  <si>
+    <t>7, 80-95</t>
+  </si>
+  <si>
+    <t>18, 80-95</t>
+  </si>
+  <si>
+    <t>14, 80-95</t>
+  </si>
+  <si>
+    <t>3, 80-95</t>
+  </si>
+  <si>
+    <t>20, 96-111</t>
+  </si>
+  <si>
+    <t>16, 96-111</t>
+  </si>
+  <si>
+    <t>9, 96-111</t>
+  </si>
+  <si>
+    <t>5, 96-111</t>
+  </si>
+  <si>
+    <t>19, 96-111</t>
+  </si>
+  <si>
+    <t>15, 96-111</t>
+  </si>
+  <si>
+    <t>8, 96-111</t>
+  </si>
+  <si>
+    <t>4, 96-111</t>
+  </si>
+  <si>
+    <t>7, 96-111</t>
+  </si>
+  <si>
+    <t>18, 96-111</t>
+  </si>
+  <si>
+    <t>14, 96-111</t>
+  </si>
+  <si>
+    <t>3, 96-111</t>
+  </si>
+  <si>
+    <t>10, 96-111</t>
+  </si>
+  <si>
+    <t>6, 96-111</t>
+  </si>
+  <si>
+    <t>17, 96-111</t>
+  </si>
+  <si>
+    <t>20, 112-127</t>
+  </si>
+  <si>
+    <t>16, 112-127</t>
+  </si>
+  <si>
+    <t>9, 112-127</t>
+  </si>
+  <si>
+    <t>5, 112-127</t>
+  </si>
+  <si>
+    <t>19, 112-127</t>
+  </si>
+  <si>
+    <t>15, 112-127</t>
+  </si>
+  <si>
+    <t>8, 112-127</t>
+  </si>
+  <si>
+    <t>4, 112-127</t>
+  </si>
+  <si>
+    <t>7, 112-127</t>
+  </si>
+  <si>
+    <t>18, 112-127</t>
+  </si>
+  <si>
+    <t>14, 112-127</t>
+  </si>
+  <si>
+    <t>3, 112-127</t>
+  </si>
+  <si>
+    <t>10, 112-127</t>
+  </si>
+  <si>
+    <t>6, 112-127</t>
+  </si>
+  <si>
+    <t>17, 112-127</t>
+  </si>
+  <si>
+    <t>19, 128-143</t>
+  </si>
+  <si>
+    <t>9, 128-143</t>
+  </si>
+  <si>
+    <t>5, 128-143</t>
+  </si>
+  <si>
+    <t>18, 128-143</t>
+  </si>
+  <si>
+    <t>14, 128-143</t>
+  </si>
+  <si>
+    <t>8, 128-143</t>
+  </si>
+  <si>
+    <t>4, 128-143</t>
+  </si>
+  <si>
+    <t>17, 128-143</t>
+  </si>
+  <si>
+    <t>13, 128-143</t>
+  </si>
+  <si>
+    <t>3, 128-143</t>
+  </si>
+  <si>
+    <t>6, 128-143</t>
+  </si>
+  <si>
+    <t>16, 128-143</t>
+  </si>
+  <si>
+    <t>10, 128-143</t>
+  </si>
+  <si>
+    <t>19, 144-159</t>
+  </si>
+  <si>
+    <t>9, 144-159</t>
+  </si>
+  <si>
+    <t>5, 144-159</t>
+  </si>
+  <si>
+    <t>18, 144-159</t>
+  </si>
+  <si>
+    <t>14, 144-159</t>
+  </si>
+  <si>
+    <t>8, 144-159</t>
+  </si>
+  <si>
+    <t>4, 144-159</t>
+  </si>
+  <si>
+    <t>17, 144-159</t>
+  </si>
+  <si>
+    <t>13, 144-159</t>
+  </si>
+  <si>
+    <t>3, 144-159</t>
+  </si>
+  <si>
+    <t>6, 144-159</t>
+  </si>
+  <si>
+    <t>16, 144-159</t>
+  </si>
+  <si>
+    <t>10, 144-159</t>
+  </si>
+  <si>
+    <t>19, 160-175</t>
+  </si>
+  <si>
+    <t>9, 160-175</t>
+  </si>
+  <si>
+    <t>5, 160-175</t>
+  </si>
+  <si>
+    <t>18, 160-175</t>
+  </si>
+  <si>
+    <t>14, 160-175</t>
+  </si>
+  <si>
+    <t>8, 160-175</t>
+  </si>
+  <si>
+    <t>4, 160-175</t>
+  </si>
+  <si>
+    <t>17, 160-175</t>
+  </si>
+  <si>
+    <t>13, 160-175</t>
+  </si>
+  <si>
+    <t>3, 160-175</t>
+  </si>
+  <si>
+    <t>6, 160-175</t>
+  </si>
+  <si>
+    <t>16, 160-175</t>
+  </si>
+  <si>
+    <t>10, 160-175</t>
+  </si>
+  <si>
+    <t>19, 176-191</t>
+  </si>
+  <si>
+    <t>9, 176-191</t>
+  </si>
+  <si>
+    <t>5, 176-191</t>
+  </si>
+  <si>
+    <t>18, 176-191</t>
+  </si>
+  <si>
+    <t>14, 176-191</t>
+  </si>
+  <si>
+    <t>8, 176-191</t>
+  </si>
+  <si>
+    <t>4, 176-191</t>
+  </si>
+  <si>
+    <t>17, 176-191</t>
+  </si>
+  <si>
+    <t>13, 176-191</t>
+  </si>
+  <si>
+    <t>3, 176-191</t>
+  </si>
+  <si>
+    <t>6, 176-191</t>
+  </si>
+  <si>
+    <t>16, 176-191</t>
+  </si>
+  <si>
+    <t>10, 176-191</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1437,97 +1444,98 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1751,8 +1759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C267A411-0DF7-B748-9579-92A194184DBE}">
   <dimension ref="A2:W54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="O44" sqref="O44"/>
+    <sheetView tabSelected="1" topLeftCell="H17" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="Q48" sqref="Q48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1782,102 +1790,102 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
-      <c r="H2" s="30" t="s">
+      <c r="H2" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
       <c r="L2" s="10"/>
-      <c r="M2" s="30" t="s">
+      <c r="M2" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
-      <c r="Q2" s="30"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
       <c r="R2" s="9"/>
-      <c r="S2" s="30" t="s">
+      <c r="S2" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="T2" s="30"/>
-      <c r="U2" s="30"/>
-      <c r="V2" s="30"/>
-      <c r="W2" s="30"/>
+      <c r="T2" s="32"/>
+      <c r="U2" s="32"/>
+      <c r="V2" s="32"/>
+      <c r="W2" s="32"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="30"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
       <c r="L3" s="10"/>
-      <c r="M3" s="30" t="s">
+      <c r="M3" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="N3" s="30"/>
-      <c r="O3" s="30"/>
-      <c r="P3" s="30"/>
-      <c r="Q3" s="30"/>
-      <c r="R3" s="30"/>
-      <c r="S3" s="30"/>
-      <c r="T3" s="30"/>
-      <c r="U3" s="30"/>
-      <c r="V3" s="30"/>
-      <c r="W3" s="30"/>
+      <c r="N3" s="32"/>
+      <c r="O3" s="32"/>
+      <c r="P3" s="32"/>
+      <c r="Q3" s="32"/>
+      <c r="R3" s="32"/>
+      <c r="S3" s="32"/>
+      <c r="T3" s="32"/>
+      <c r="U3" s="32"/>
+      <c r="V3" s="32"/>
+      <c r="W3" s="32"/>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" s="12"/>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="26"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="28"/>
       <c r="F4" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="G4" s="27" t="s">
+      <c r="G4" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="29"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="31"/>
       <c r="K4" s="12"/>
       <c r="L4" s="10"/>
       <c r="M4" s="12"/>
-      <c r="N4" s="27" t="s">
+      <c r="N4" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="O4" s="28"/>
-      <c r="P4" s="28"/>
-      <c r="Q4" s="29"/>
+      <c r="O4" s="30"/>
+      <c r="P4" s="30"/>
+      <c r="Q4" s="31"/>
       <c r="R4" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="S4" s="27" t="s">
+      <c r="S4" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="T4" s="28"/>
-      <c r="U4" s="28"/>
-      <c r="V4" s="29"/>
+      <c r="T4" s="30"/>
+      <c r="U4" s="30"/>
+      <c r="V4" s="31"/>
       <c r="W4" s="12"/>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.2">
@@ -1889,7 +1897,7 @@
         <v>40</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>204</v>
+        <v>46</v>
       </c>
       <c r="E5" s="14" t="s">
         <v>45</v>
@@ -1902,7 +1910,7 @@
         <v>40</v>
       </c>
       <c r="I5" s="18" t="s">
-        <v>204</v>
+        <v>46</v>
       </c>
       <c r="J5" s="14" t="s">
         <v>45</v>
@@ -1917,7 +1925,7 @@
         <v>40</v>
       </c>
       <c r="P5" s="18" t="s">
-        <v>204</v>
+        <v>46</v>
       </c>
       <c r="Q5" s="14" t="s">
         <v>45</v>
@@ -1930,7 +1938,7 @@
         <v>40</v>
       </c>
       <c r="U5" s="18" t="s">
-        <v>204</v>
+        <v>46</v>
       </c>
       <c r="V5" s="14" t="s">
         <v>45</v>
@@ -1944,13 +1952,13 @@
         <v>41</v>
       </c>
       <c r="C6" s="15">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>208</v>
+        <v>50</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>112</v>
+        <v>289</v>
       </c>
       <c r="F6" s="12"/>
       <c r="G6" s="15">
@@ -1958,13 +1966,13 @@
         <v>83</v>
       </c>
       <c r="H6" s="15">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="I6" s="20" t="s">
-        <v>247</v>
-      </c>
-      <c r="J6" s="15" t="s">
-        <v>71</v>
+        <v>89</v>
+      </c>
+      <c r="J6" s="37" t="s">
+        <v>217</v>
       </c>
       <c r="K6" s="12"/>
       <c r="L6" s="10"/>
@@ -1974,13 +1982,13 @@
         <v>125</v>
       </c>
       <c r="O6" s="15">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="P6" s="20" t="s">
-        <v>289</v>
+        <v>131</v>
       </c>
       <c r="Q6" s="15" t="s">
-        <v>123</v>
+        <v>290</v>
       </c>
       <c r="R6" s="17"/>
       <c r="S6" s="15">
@@ -1988,13 +1996,13 @@
         <v>167</v>
       </c>
       <c r="T6" s="15">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="U6" s="20" t="s">
-        <v>331</v>
+        <v>173</v>
       </c>
       <c r="V6" s="15" t="s">
-        <v>177</v>
+        <v>372</v>
       </c>
       <c r="W6" s="12"/>
     </row>
@@ -2005,13 +2013,13 @@
         <v>40</v>
       </c>
       <c r="C7" s="15">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>209</v>
+        <v>51</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>99</v>
+        <v>275</v>
       </c>
       <c r="F7" s="12"/>
       <c r="G7" s="15">
@@ -2019,13 +2027,13 @@
         <v>82</v>
       </c>
       <c r="H7" s="15">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="I7" s="20" t="s">
-        <v>248</v>
-      </c>
-      <c r="J7" s="15" t="s">
-        <v>85</v>
+        <v>90</v>
+      </c>
+      <c r="J7" s="37" t="s">
+        <v>218</v>
       </c>
       <c r="K7" s="12"/>
       <c r="L7" s="10"/>
@@ -2035,13 +2043,13 @@
         <v>124</v>
       </c>
       <c r="O7" s="15">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="P7" s="20" t="s">
-        <v>290</v>
+        <v>132</v>
       </c>
       <c r="Q7" s="15" t="s">
-        <v>110</v>
+        <v>276</v>
       </c>
       <c r="R7" s="17"/>
       <c r="S7" s="15">
@@ -2049,13 +2057,13 @@
         <v>166</v>
       </c>
       <c r="T7" s="15">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="U7" s="20" t="s">
-        <v>332</v>
+        <v>174</v>
       </c>
       <c r="V7" s="15" t="s">
-        <v>190</v>
+        <v>359</v>
       </c>
       <c r="W7" s="12"/>
     </row>
@@ -2066,13 +2074,13 @@
         <v>39</v>
       </c>
       <c r="C8" s="15">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>210</v>
+        <v>52</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>72</v>
+        <v>261</v>
       </c>
       <c r="F8" s="12"/>
       <c r="G8" s="15">
@@ -2080,13 +2088,13 @@
         <v>81</v>
       </c>
       <c r="H8" s="15">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="I8" s="20" t="s">
-        <v>249</v>
-      </c>
-      <c r="J8" s="15" t="s">
-        <v>58</v>
+        <v>91</v>
+      </c>
+      <c r="J8" s="37" t="s">
+        <v>219</v>
       </c>
       <c r="K8" s="12"/>
       <c r="L8" s="10"/>
@@ -2096,13 +2104,13 @@
         <v>123</v>
       </c>
       <c r="O8" s="15">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="P8" s="20" t="s">
-        <v>291</v>
+        <v>133</v>
       </c>
       <c r="Q8" s="15" t="s">
-        <v>83</v>
+        <v>262</v>
       </c>
       <c r="R8" s="17"/>
       <c r="S8" s="15">
@@ -2110,13 +2118,13 @@
         <v>165</v>
       </c>
       <c r="T8" s="15">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="U8" s="20" t="s">
-        <v>333</v>
+        <v>175</v>
       </c>
       <c r="V8" s="15" t="s">
-        <v>164</v>
+        <v>346</v>
       </c>
       <c r="W8" s="12"/>
     </row>
@@ -2127,13 +2135,13 @@
         <v>38</v>
       </c>
       <c r="C9" s="15">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>211</v>
+        <v>53</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>86</v>
+        <v>247</v>
       </c>
       <c r="F9" s="12"/>
       <c r="G9" s="15">
@@ -2141,13 +2149,13 @@
         <v>80</v>
       </c>
       <c r="H9" s="15">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="I9" s="20" t="s">
-        <v>250</v>
-      </c>
-      <c r="J9" s="15" t="s">
-        <v>46</v>
+        <v>92</v>
+      </c>
+      <c r="J9" s="37" t="s">
+        <v>220</v>
       </c>
       <c r="K9" s="12"/>
       <c r="L9" s="10"/>
@@ -2157,13 +2165,13 @@
         <v>122</v>
       </c>
       <c r="O9" s="15">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="P9" s="20" t="s">
-        <v>292</v>
+        <v>134</v>
       </c>
       <c r="Q9" s="15" t="s">
-        <v>97</v>
+        <v>248</v>
       </c>
       <c r="R9" s="17"/>
       <c r="S9" s="15">
@@ -2171,13 +2179,13 @@
         <v>164</v>
       </c>
       <c r="T9" s="15">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="U9" s="20" t="s">
-        <v>334</v>
+        <v>176</v>
       </c>
       <c r="V9" s="15" t="s">
-        <v>151</v>
+        <v>333</v>
       </c>
       <c r="W9" s="12"/>
     </row>
@@ -2188,13 +2196,13 @@
         <v>37</v>
       </c>
       <c r="C10" s="15">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>212</v>
+        <v>54</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>59</v>
+        <v>234</v>
       </c>
       <c r="F10" s="12"/>
       <c r="G10" s="15">
@@ -2202,13 +2210,13 @@
         <v>79</v>
       </c>
       <c r="H10" s="15">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="I10" s="20" t="s">
-        <v>251</v>
+        <v>93</v>
       </c>
       <c r="J10" s="15" t="s">
-        <v>178</v>
+        <v>373</v>
       </c>
       <c r="K10" s="12"/>
       <c r="L10" s="10"/>
@@ -2218,13 +2226,13 @@
         <v>121</v>
       </c>
       <c r="O10" s="15">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="P10" s="20" t="s">
-        <v>293</v>
+        <v>135</v>
       </c>
       <c r="Q10" s="15" t="s">
-        <v>69</v>
+        <v>235</v>
       </c>
       <c r="R10" s="17"/>
       <c r="S10" s="15">
@@ -2232,13 +2240,13 @@
         <v>163</v>
       </c>
       <c r="T10" s="15">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="U10" s="20" t="s">
-        <v>335</v>
+        <v>177</v>
       </c>
       <c r="V10" s="15" t="s">
-        <v>375</v>
+        <v>318</v>
       </c>
       <c r="W10" s="12"/>
     </row>
@@ -2249,13 +2257,13 @@
         <v>36</v>
       </c>
       <c r="C11" s="15">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>213</v>
+        <v>55</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>47</v>
+        <v>221</v>
       </c>
       <c r="F11" s="12"/>
       <c r="G11" s="15">
@@ -2263,13 +2271,13 @@
         <v>78</v>
       </c>
       <c r="H11" s="15">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="I11" s="20" t="s">
-        <v>252</v>
+        <v>94</v>
       </c>
       <c r="J11" s="15" t="s">
-        <v>191</v>
+        <v>360</v>
       </c>
       <c r="K11" s="12"/>
       <c r="L11" s="10"/>
@@ -2279,13 +2287,13 @@
         <v>120</v>
       </c>
       <c r="O11" s="15">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="P11" s="20" t="s">
-        <v>294</v>
+        <v>136</v>
       </c>
       <c r="Q11" s="15" t="s">
-        <v>57</v>
+        <v>222</v>
       </c>
       <c r="R11" s="17"/>
       <c r="S11" s="15">
@@ -2293,13 +2301,13 @@
         <v>162</v>
       </c>
       <c r="T11" s="15">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="U11" s="20" t="s">
-        <v>336</v>
+        <v>178</v>
       </c>
       <c r="V11" s="15" t="s">
-        <v>376</v>
+        <v>303</v>
       </c>
       <c r="W11" s="12"/>
     </row>
@@ -2310,13 +2318,13 @@
         <v>35</v>
       </c>
       <c r="C12" s="15">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>214</v>
+        <v>56</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>179</v>
+        <v>374</v>
       </c>
       <c r="F12" s="12"/>
       <c r="G12" s="15">
@@ -2324,13 +2332,13 @@
         <v>77</v>
       </c>
       <c r="H12" s="15">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="I12" s="20" t="s">
-        <v>253</v>
+        <v>95</v>
       </c>
       <c r="J12" s="15" t="s">
-        <v>165</v>
+        <v>347</v>
       </c>
       <c r="K12" s="12"/>
       <c r="L12" s="10"/>
@@ -2340,13 +2348,13 @@
         <v>119</v>
       </c>
       <c r="O12" s="15">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="P12" s="20" t="s">
-        <v>295</v>
+        <v>137</v>
       </c>
       <c r="Q12" s="15" t="s">
-        <v>137</v>
+        <v>319</v>
       </c>
       <c r="R12" s="17"/>
       <c r="S12" s="15">
@@ -2354,13 +2362,13 @@
         <v>161</v>
       </c>
       <c r="T12" s="15">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="U12" s="20" t="s">
-        <v>337</v>
+        <v>179</v>
       </c>
       <c r="V12" s="15" t="s">
-        <v>377</v>
+        <v>291</v>
       </c>
       <c r="W12" s="12"/>
     </row>
@@ -2371,13 +2379,13 @@
         <v>34</v>
       </c>
       <c r="C13" s="15">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>215</v>
+        <v>57</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>192</v>
+        <v>361</v>
       </c>
       <c r="F13" s="12"/>
       <c r="G13" s="15">
@@ -2385,13 +2393,13 @@
         <v>76</v>
       </c>
       <c r="H13" s="15">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="I13" s="20" t="s">
-        <v>254</v>
+        <v>96</v>
       </c>
       <c r="J13" s="15" t="s">
-        <v>152</v>
+        <v>334</v>
       </c>
       <c r="K13" s="12"/>
       <c r="L13" s="10"/>
@@ -2401,13 +2409,13 @@
         <v>118</v>
       </c>
       <c r="O13" s="15">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="P13" s="20" t="s">
-        <v>296</v>
+        <v>138</v>
       </c>
       <c r="Q13" s="15" t="s">
-        <v>150</v>
+        <v>304</v>
       </c>
       <c r="R13" s="17"/>
       <c r="S13" s="15">
@@ -2415,13 +2423,13 @@
         <v>160</v>
       </c>
       <c r="T13" s="15">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="U13" s="20" t="s">
-        <v>338</v>
+        <v>180</v>
       </c>
       <c r="V13" s="15" t="s">
-        <v>378</v>
+        <v>277</v>
       </c>
       <c r="W13" s="12"/>
     </row>
@@ -2432,13 +2440,13 @@
         <v>33</v>
       </c>
       <c r="C14" s="15">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>216</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>166</v>
+        <v>58</v>
+      </c>
+      <c r="E14" s="37" t="s">
+        <v>348</v>
       </c>
       <c r="F14" s="12"/>
       <c r="G14" s="15">
@@ -2446,13 +2454,13 @@
         <v>75</v>
       </c>
       <c r="H14" s="15">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="I14" s="20" t="s">
-        <v>255</v>
+        <v>97</v>
       </c>
       <c r="J14" s="15" t="s">
-        <v>127</v>
+        <v>320</v>
       </c>
       <c r="K14" s="12"/>
       <c r="L14" s="10"/>
@@ -2462,13 +2470,13 @@
         <v>117</v>
       </c>
       <c r="O14" s="15">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="P14" s="20" t="s">
-        <v>297</v>
+        <v>139</v>
       </c>
       <c r="Q14" s="15" t="s">
-        <v>113</v>
+        <v>292</v>
       </c>
       <c r="R14" s="17"/>
       <c r="S14" s="15">
@@ -2476,13 +2484,13 @@
         <v>159</v>
       </c>
       <c r="T14" s="15">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="U14" s="20" t="s">
-        <v>339</v>
+        <v>181</v>
       </c>
       <c r="V14" s="15" t="s">
-        <v>379</v>
+        <v>263</v>
       </c>
       <c r="W14" s="12"/>
     </row>
@@ -2493,13 +2501,13 @@
         <v>32</v>
       </c>
       <c r="C15" s="15">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>217</v>
+        <v>59</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>153</v>
+        <v>335</v>
       </c>
       <c r="F15" s="12"/>
       <c r="G15" s="15">
@@ -2507,13 +2515,13 @@
         <v>74</v>
       </c>
       <c r="H15" s="15">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="I15" s="20" t="s">
-        <v>256</v>
+        <v>98</v>
       </c>
       <c r="J15" s="15" t="s">
-        <v>140</v>
+        <v>305</v>
       </c>
       <c r="K15" s="12"/>
       <c r="L15" s="10"/>
@@ -2523,13 +2531,13 @@
         <v>116</v>
       </c>
       <c r="O15" s="15">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="P15" s="20" t="s">
-        <v>298</v>
+        <v>140</v>
       </c>
       <c r="Q15" s="15" t="s">
-        <v>100</v>
+        <v>278</v>
       </c>
       <c r="R15" s="17"/>
       <c r="S15" s="15">
@@ -2537,13 +2545,13 @@
         <v>158</v>
       </c>
       <c r="T15" s="15">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="U15" s="20" t="s">
-        <v>340</v>
+        <v>182</v>
       </c>
       <c r="V15" s="15" t="s">
-        <v>380</v>
+        <v>249</v>
       </c>
       <c r="W15" s="12"/>
     </row>
@@ -2554,13 +2562,13 @@
         <v>31</v>
       </c>
       <c r="C16" s="15">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>218</v>
+        <v>60</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>128</v>
+        <v>321</v>
       </c>
       <c r="F16" s="12"/>
       <c r="G16" s="15">
@@ -2568,13 +2576,13 @@
         <v>73</v>
       </c>
       <c r="H16" s="15">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="I16" s="20" t="s">
-        <v>257</v>
+        <v>99</v>
       </c>
       <c r="J16" s="15" t="s">
-        <v>116</v>
+        <v>293</v>
       </c>
       <c r="K16" s="12"/>
       <c r="L16" s="10"/>
@@ -2584,13 +2592,13 @@
         <v>115</v>
       </c>
       <c r="O16" s="15">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="P16" s="20" t="s">
-        <v>299</v>
+        <v>141</v>
       </c>
       <c r="Q16" s="15" t="s">
-        <v>73</v>
+        <v>264</v>
       </c>
       <c r="R16" s="17"/>
       <c r="S16" s="15">
@@ -2598,13 +2606,13 @@
         <v>157</v>
       </c>
       <c r="T16" s="15">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="U16" s="20" t="s">
-        <v>341</v>
+        <v>183</v>
       </c>
       <c r="V16" s="15" t="s">
-        <v>381</v>
+        <v>236</v>
       </c>
       <c r="W16" s="12"/>
     </row>
@@ -2615,13 +2623,13 @@
         <v>30</v>
       </c>
       <c r="C17" s="15">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>219</v>
+        <v>61</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>141</v>
+        <v>306</v>
       </c>
       <c r="F17" s="12"/>
       <c r="G17" s="15">
@@ -2629,13 +2637,13 @@
         <v>72</v>
       </c>
       <c r="H17" s="15">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="I17" s="20" t="s">
-        <v>258</v>
+        <v>100</v>
       </c>
       <c r="J17" s="15" t="s">
-        <v>103</v>
+        <v>279</v>
       </c>
       <c r="K17" s="12"/>
       <c r="L17" s="10"/>
@@ -2645,13 +2653,13 @@
         <v>114</v>
       </c>
       <c r="O17" s="15">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="P17" s="20" t="s">
-        <v>300</v>
+        <v>142</v>
       </c>
       <c r="Q17" s="15" t="s">
-        <v>87</v>
+        <v>250</v>
       </c>
       <c r="R17" s="17"/>
       <c r="S17" s="15">
@@ -2659,13 +2667,13 @@
         <v>156</v>
       </c>
       <c r="T17" s="15">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="U17" s="20" t="s">
-        <v>342</v>
+        <v>184</v>
       </c>
       <c r="V17" s="15" t="s">
-        <v>382</v>
+        <v>223</v>
       </c>
       <c r="W17" s="12"/>
     </row>
@@ -2676,13 +2684,13 @@
         <v>29</v>
       </c>
       <c r="C18" s="15">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>220</v>
+        <v>62</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>117</v>
+        <v>294</v>
       </c>
       <c r="F18" s="12"/>
       <c r="G18" s="15">
@@ -2690,13 +2698,13 @@
         <v>71</v>
       </c>
       <c r="H18" s="15">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="I18" s="20" t="s">
-        <v>259</v>
+        <v>101</v>
       </c>
       <c r="J18" s="15" t="s">
-        <v>76</v>
+        <v>265</v>
       </c>
       <c r="K18" s="12"/>
       <c r="L18" s="10"/>
@@ -2706,13 +2714,13 @@
         <v>113</v>
       </c>
       <c r="O18" s="15">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="P18" s="20" t="s">
-        <v>301</v>
+        <v>143</v>
       </c>
       <c r="Q18" s="15" t="s">
-        <v>60</v>
+        <v>237</v>
       </c>
       <c r="R18" s="17"/>
       <c r="S18" s="15">
@@ -2720,13 +2728,13 @@
         <v>155</v>
       </c>
       <c r="T18" s="15">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="U18" s="20" t="s">
-        <v>343</v>
+        <v>185</v>
       </c>
       <c r="V18" s="15" t="s">
-        <v>180</v>
+        <v>375</v>
       </c>
       <c r="W18" s="12"/>
     </row>
@@ -2737,13 +2745,13 @@
         <v>28</v>
       </c>
       <c r="C19" s="15">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="D19" s="20" t="s">
-        <v>221</v>
+        <v>63</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>104</v>
+        <v>280</v>
       </c>
       <c r="F19" s="12"/>
       <c r="G19" s="15">
@@ -2751,13 +2759,13 @@
         <v>70</v>
       </c>
       <c r="H19" s="15">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="I19" s="20" t="s">
-        <v>260</v>
+        <v>102</v>
       </c>
       <c r="J19" s="15" t="s">
-        <v>90</v>
+        <v>251</v>
       </c>
       <c r="K19" s="12"/>
       <c r="L19" s="10"/>
@@ -2767,13 +2775,13 @@
         <v>112</v>
       </c>
       <c r="O19" s="15">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="P19" s="20" t="s">
-        <v>302</v>
+        <v>144</v>
       </c>
       <c r="Q19" s="15" t="s">
-        <v>48</v>
+        <v>224</v>
       </c>
       <c r="R19" s="17"/>
       <c r="S19" s="15">
@@ -2781,13 +2789,13 @@
         <v>154</v>
       </c>
       <c r="T19" s="15">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="U19" s="20" t="s">
-        <v>344</v>
+        <v>186</v>
       </c>
       <c r="V19" s="15" t="s">
-        <v>193</v>
+        <v>362</v>
       </c>
       <c r="W19" s="12"/>
     </row>
@@ -2854,7 +2862,7 @@
         <v>40</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>204</v>
+        <v>46</v>
       </c>
       <c r="E22" s="14" t="s">
         <v>45</v>
@@ -2867,7 +2875,7 @@
         <v>40</v>
       </c>
       <c r="I22" s="18" t="s">
-        <v>204</v>
+        <v>46</v>
       </c>
       <c r="J22" s="14" t="s">
         <v>45</v>
@@ -2882,7 +2890,7 @@
         <v>40</v>
       </c>
       <c r="P22" s="18" t="s">
-        <v>204</v>
+        <v>46</v>
       </c>
       <c r="Q22" s="14" t="s">
         <v>45</v>
@@ -2895,7 +2903,7 @@
         <v>40</v>
       </c>
       <c r="U22" s="18" t="s">
-        <v>204</v>
+        <v>46</v>
       </c>
       <c r="V22" s="14" t="s">
         <v>45</v>
@@ -2909,13 +2917,13 @@
         <v>27</v>
       </c>
       <c r="C23" s="15">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>222</v>
+        <v>64</v>
       </c>
       <c r="E23" s="15" t="s">
-        <v>77</v>
+        <v>266</v>
       </c>
       <c r="F23" s="12"/>
       <c r="G23" s="15">
@@ -2923,13 +2931,13 @@
         <v>69</v>
       </c>
       <c r="H23" s="15">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="I23" s="20" t="s">
-        <v>261</v>
+        <v>103</v>
       </c>
       <c r="J23" s="15" t="s">
-        <v>63</v>
+        <v>238</v>
       </c>
       <c r="K23" s="12"/>
       <c r="L23" s="10"/>
@@ -2939,13 +2947,13 @@
         <v>111</v>
       </c>
       <c r="O23" s="15">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="P23" s="20" t="s">
-        <v>303</v>
+        <v>145</v>
       </c>
       <c r="Q23" s="15" t="s">
-        <v>181</v>
+        <v>376</v>
       </c>
       <c r="R23" s="17"/>
       <c r="S23" s="15">
@@ -2953,13 +2961,13 @@
         <v>153</v>
       </c>
       <c r="T23" s="15">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="U23" s="20" t="s">
-        <v>345</v>
+        <v>187</v>
       </c>
       <c r="V23" s="15" t="s">
-        <v>167</v>
+        <v>349</v>
       </c>
       <c r="W23" s="12"/>
     </row>
@@ -2970,13 +2978,13 @@
         <v>26</v>
       </c>
       <c r="C24" s="15">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>225</v>
+        <v>67</v>
       </c>
       <c r="E24" s="15" t="s">
-        <v>91</v>
+        <v>252</v>
       </c>
       <c r="F24" s="12"/>
       <c r="G24" s="15">
@@ -2984,13 +2992,13 @@
         <v>68</v>
       </c>
       <c r="H24" s="15">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="I24" s="20" t="s">
-        <v>262</v>
+        <v>104</v>
       </c>
       <c r="J24" s="15" t="s">
-        <v>51</v>
+        <v>225</v>
       </c>
       <c r="K24" s="12"/>
       <c r="L24" s="10"/>
@@ -3000,13 +3008,13 @@
         <v>110</v>
       </c>
       <c r="O24" s="15">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="P24" s="20" t="s">
-        <v>304</v>
+        <v>146</v>
       </c>
       <c r="Q24" s="15" t="s">
-        <v>194</v>
+        <v>363</v>
       </c>
       <c r="R24" s="17"/>
       <c r="S24" s="15">
@@ -3014,13 +3022,13 @@
         <v>152</v>
       </c>
       <c r="T24" s="15">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="U24" s="20" t="s">
-        <v>346</v>
+        <v>188</v>
       </c>
       <c r="V24" s="15" t="s">
-        <v>154</v>
+        <v>336</v>
       </c>
       <c r="W24" s="12"/>
     </row>
@@ -3031,13 +3039,13 @@
         <v>25</v>
       </c>
       <c r="C25" s="15">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="D25" s="20" t="s">
-        <v>224</v>
+        <v>66</v>
       </c>
       <c r="E25" s="15" t="s">
-        <v>64</v>
+        <v>239</v>
       </c>
       <c r="F25" s="12"/>
       <c r="G25" s="15">
@@ -3045,13 +3053,13 @@
         <v>67</v>
       </c>
       <c r="H25" s="15">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="I25" s="20" t="s">
-        <v>263</v>
+        <v>105</v>
       </c>
       <c r="J25" s="15" t="s">
-        <v>182</v>
+        <v>377</v>
       </c>
       <c r="K25" s="12"/>
       <c r="L25" s="10"/>
@@ -3061,13 +3069,13 @@
         <v>109</v>
       </c>
       <c r="O25" s="15">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="P25" s="20" t="s">
-        <v>305</v>
+        <v>147</v>
       </c>
       <c r="Q25" s="15" t="s">
-        <v>168</v>
+        <v>350</v>
       </c>
       <c r="R25" s="17"/>
       <c r="S25" s="15">
@@ -3075,13 +3083,13 @@
         <v>151</v>
       </c>
       <c r="T25" s="15">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="U25" s="20" t="s">
-        <v>347</v>
+        <v>189</v>
       </c>
       <c r="V25" s="15" t="s">
-        <v>125</v>
+        <v>322</v>
       </c>
       <c r="W25" s="12"/>
     </row>
@@ -3092,13 +3100,13 @@
         <v>24</v>
       </c>
       <c r="C26" s="15">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="D26" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="E26" s="15" t="s">
         <v>226</v>
-      </c>
-      <c r="E26" s="15" t="s">
-        <v>52</v>
       </c>
       <c r="F26" s="12"/>
       <c r="G26" s="15">
@@ -3106,13 +3114,13 @@
         <v>66</v>
       </c>
       <c r="H26" s="15">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="I26" s="20" t="s">
-        <v>264</v>
+        <v>106</v>
       </c>
       <c r="J26" s="15" t="s">
-        <v>195</v>
+        <v>364</v>
       </c>
       <c r="K26" s="12"/>
       <c r="L26" s="10"/>
@@ -3122,13 +3130,13 @@
         <v>108</v>
       </c>
       <c r="O26" s="15">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="P26" s="20" t="s">
-        <v>306</v>
+        <v>148</v>
       </c>
       <c r="Q26" s="15" t="s">
-        <v>155</v>
+        <v>337</v>
       </c>
       <c r="R26" s="17"/>
       <c r="S26" s="15">
@@ -3136,13 +3144,13 @@
         <v>150</v>
       </c>
       <c r="T26" s="15">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="U26" s="20" t="s">
-        <v>348</v>
+        <v>190</v>
       </c>
       <c r="V26" s="15" t="s">
-        <v>138</v>
+        <v>307</v>
       </c>
       <c r="W26" s="12"/>
     </row>
@@ -3153,13 +3161,13 @@
         <v>23</v>
       </c>
       <c r="C27" s="15">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>227</v>
+        <v>69</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>183</v>
+        <v>378</v>
       </c>
       <c r="F27" s="12"/>
       <c r="G27" s="15">
@@ -3167,13 +3175,13 @@
         <v>65</v>
       </c>
       <c r="H27" s="15">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="I27" s="20" t="s">
-        <v>265</v>
+        <v>107</v>
       </c>
       <c r="J27" s="15" t="s">
-        <v>169</v>
+        <v>351</v>
       </c>
       <c r="K27" s="12"/>
       <c r="L27" s="10"/>
@@ -3183,13 +3191,13 @@
         <v>107</v>
       </c>
       <c r="O27" s="15">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="P27" s="20" t="s">
-        <v>307</v>
+        <v>149</v>
       </c>
       <c r="Q27" s="15" t="s">
-        <v>126</v>
+        <v>323</v>
       </c>
       <c r="R27" s="17"/>
       <c r="S27" s="15">
@@ -3197,13 +3205,13 @@
         <v>149</v>
       </c>
       <c r="T27" s="15">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="U27" s="20" t="s">
-        <v>349</v>
+        <v>191</v>
       </c>
       <c r="V27" s="15" t="s">
-        <v>114</v>
+        <v>295</v>
       </c>
       <c r="W27" s="12"/>
     </row>
@@ -3214,13 +3222,13 @@
         <v>22</v>
       </c>
       <c r="C28" s="15">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>228</v>
+        <v>70</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>196</v>
+        <v>365</v>
       </c>
       <c r="F28" s="12"/>
       <c r="G28" s="15">
@@ -3228,13 +3236,13 @@
         <v>64</v>
       </c>
       <c r="H28" s="15">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="I28" s="20" t="s">
-        <v>266</v>
+        <v>108</v>
       </c>
       <c r="J28" s="15" t="s">
-        <v>156</v>
+        <v>338</v>
       </c>
       <c r="K28" s="12"/>
       <c r="L28" s="10"/>
@@ -3244,13 +3252,13 @@
         <v>106</v>
       </c>
       <c r="O28" s="15">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="P28" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q28" s="15" t="s">
         <v>308</v>
-      </c>
-      <c r="Q28" s="15" t="s">
-        <v>139</v>
       </c>
       <c r="R28" s="17"/>
       <c r="S28" s="15">
@@ -3258,13 +3266,13 @@
         <v>148</v>
       </c>
       <c r="T28" s="15">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="U28" s="20" t="s">
-        <v>350</v>
+        <v>192</v>
       </c>
       <c r="V28" s="15" t="s">
-        <v>101</v>
+        <v>281</v>
       </c>
       <c r="W28" s="12"/>
     </row>
@@ -3275,13 +3283,13 @@
         <v>21</v>
       </c>
       <c r="C29" s="15">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>229</v>
+        <v>71</v>
       </c>
       <c r="E29" s="15" t="s">
-        <v>170</v>
+        <v>352</v>
       </c>
       <c r="F29" s="12"/>
       <c r="G29" s="15">
@@ -3289,13 +3297,13 @@
         <v>63</v>
       </c>
       <c r="H29" s="15">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="I29" s="20" t="s">
-        <v>267</v>
+        <v>109</v>
       </c>
       <c r="J29" s="15" t="s">
-        <v>131</v>
+        <v>324</v>
       </c>
       <c r="K29" s="12"/>
       <c r="L29" s="10"/>
@@ -3305,13 +3313,13 @@
         <v>105</v>
       </c>
       <c r="O29" s="15">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="P29" s="20" t="s">
-        <v>309</v>
+        <v>151</v>
       </c>
       <c r="Q29" s="15" t="s">
-        <v>115</v>
+        <v>296</v>
       </c>
       <c r="R29" s="17"/>
       <c r="S29" s="15">
@@ -3319,13 +3327,13 @@
         <v>147</v>
       </c>
       <c r="T29" s="15">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="U29" s="20" t="s">
-        <v>351</v>
+        <v>193</v>
       </c>
       <c r="V29" s="15" t="s">
-        <v>74</v>
+        <v>267</v>
       </c>
       <c r="W29" s="12"/>
     </row>
@@ -3336,13 +3344,13 @@
         <v>20</v>
       </c>
       <c r="C30" s="15">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>230</v>
+        <v>72</v>
       </c>
       <c r="E30" s="15" t="s">
-        <v>157</v>
+        <v>339</v>
       </c>
       <c r="F30" s="12"/>
       <c r="G30" s="15">
@@ -3350,13 +3358,13 @@
         <v>62</v>
       </c>
       <c r="H30" s="15">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="I30" s="20" t="s">
-        <v>268</v>
+        <v>110</v>
       </c>
       <c r="J30" s="15" t="s">
-        <v>144</v>
+        <v>309</v>
       </c>
       <c r="K30" s="12"/>
       <c r="L30" s="10"/>
@@ -3366,13 +3374,13 @@
         <v>104</v>
       </c>
       <c r="O30" s="15">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="P30" s="20" t="s">
-        <v>310</v>
+        <v>152</v>
       </c>
       <c r="Q30" s="15" t="s">
-        <v>102</v>
+        <v>282</v>
       </c>
       <c r="R30" s="17"/>
       <c r="S30" s="15">
@@ -3380,13 +3388,13 @@
         <v>146</v>
       </c>
       <c r="T30" s="15">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="U30" s="20" t="s">
-        <v>352</v>
+        <v>194</v>
       </c>
       <c r="V30" s="15" t="s">
-        <v>88</v>
+        <v>253</v>
       </c>
       <c r="W30" s="12"/>
     </row>
@@ -3397,13 +3405,13 @@
         <v>19</v>
       </c>
       <c r="C31" s="15">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="D31" s="20" t="s">
-        <v>231</v>
+        <v>73</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>132</v>
+        <v>325</v>
       </c>
       <c r="F31" s="12"/>
       <c r="G31" s="15">
@@ -3411,13 +3419,13 @@
         <v>61</v>
       </c>
       <c r="H31" s="15">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="I31" s="20" t="s">
-        <v>269</v>
+        <v>111</v>
       </c>
       <c r="J31" s="15" t="s">
-        <v>120</v>
+        <v>297</v>
       </c>
       <c r="K31" s="12"/>
       <c r="L31" s="10"/>
@@ -3427,13 +3435,13 @@
         <v>103</v>
       </c>
       <c r="O31" s="15">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="P31" s="20" t="s">
-        <v>311</v>
+        <v>153</v>
       </c>
       <c r="Q31" s="15" t="s">
-        <v>75</v>
+        <v>268</v>
       </c>
       <c r="R31" s="17"/>
       <c r="S31" s="15">
@@ -3441,13 +3449,13 @@
         <v>145</v>
       </c>
       <c r="T31" s="15">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="U31" s="20" t="s">
-        <v>353</v>
+        <v>195</v>
       </c>
       <c r="V31" s="15" t="s">
-        <v>61</v>
+        <v>240</v>
       </c>
       <c r="W31" s="12"/>
     </row>
@@ -3458,13 +3466,13 @@
         <v>18</v>
       </c>
       <c r="C32" s="15">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="D32" s="20" t="s">
-        <v>232</v>
+        <v>74</v>
       </c>
       <c r="E32" s="15" t="s">
-        <v>145</v>
+        <v>310</v>
       </c>
       <c r="F32" s="12"/>
       <c r="G32" s="15">
@@ -3472,13 +3480,13 @@
         <v>60</v>
       </c>
       <c r="H32" s="15">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="I32" s="20" t="s">
-        <v>270</v>
+        <v>112</v>
       </c>
       <c r="J32" s="15" t="s">
-        <v>107</v>
+        <v>283</v>
       </c>
       <c r="K32" s="12"/>
       <c r="L32" s="10"/>
@@ -3488,13 +3496,13 @@
         <v>102</v>
       </c>
       <c r="O32" s="15">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="P32" s="20" t="s">
-        <v>312</v>
+        <v>154</v>
       </c>
       <c r="Q32" s="15" t="s">
-        <v>89</v>
+        <v>254</v>
       </c>
       <c r="R32" s="17"/>
       <c r="S32" s="15">
@@ -3502,13 +3510,13 @@
         <v>144</v>
       </c>
       <c r="T32" s="15">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="U32" s="20" t="s">
-        <v>354</v>
+        <v>196</v>
       </c>
       <c r="V32" s="15" t="s">
-        <v>49</v>
+        <v>227</v>
       </c>
       <c r="W32" s="12"/>
     </row>
@@ -3519,13 +3527,13 @@
         <v>17</v>
       </c>
       <c r="C33" s="15">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>233</v>
+        <v>75</v>
       </c>
       <c r="E33" s="15" t="s">
-        <v>121</v>
+        <v>298</v>
       </c>
       <c r="F33" s="12"/>
       <c r="G33" s="15">
@@ -3533,13 +3541,13 @@
         <v>59</v>
       </c>
       <c r="H33" s="15">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="I33" s="20" t="s">
-        <v>271</v>
+        <v>113</v>
       </c>
       <c r="J33" s="15" t="s">
-        <v>80</v>
+        <v>269</v>
       </c>
       <c r="K33" s="12"/>
       <c r="L33" s="10"/>
@@ -3549,13 +3557,13 @@
         <v>101</v>
       </c>
       <c r="O33" s="15">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="P33" s="20" t="s">
-        <v>313</v>
+        <v>155</v>
       </c>
       <c r="Q33" s="15" t="s">
-        <v>62</v>
+        <v>241</v>
       </c>
       <c r="R33" s="17"/>
       <c r="S33" s="15">
@@ -3563,13 +3571,13 @@
         <v>143</v>
       </c>
       <c r="T33" s="15">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="U33" s="20" t="s">
-        <v>355</v>
+        <v>197</v>
       </c>
       <c r="V33" s="15" t="s">
-        <v>184</v>
+        <v>379</v>
       </c>
       <c r="W33" s="12"/>
     </row>
@@ -3580,13 +3588,13 @@
         <v>16</v>
       </c>
       <c r="C34" s="15">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="D34" s="20" t="s">
-        <v>234</v>
+        <v>76</v>
       </c>
       <c r="E34" s="15" t="s">
-        <v>108</v>
+        <v>284</v>
       </c>
       <c r="F34" s="12"/>
       <c r="G34" s="15">
@@ -3594,13 +3602,13 @@
         <v>58</v>
       </c>
       <c r="H34" s="15">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="I34" s="20" t="s">
-        <v>272</v>
+        <v>114</v>
       </c>
       <c r="J34" s="15" t="s">
-        <v>94</v>
+        <v>255</v>
       </c>
       <c r="K34" s="12"/>
       <c r="L34" s="10"/>
@@ -3610,13 +3618,13 @@
         <v>100</v>
       </c>
       <c r="O34" s="15">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="P34" s="20" t="s">
-        <v>314</v>
+        <v>156</v>
       </c>
       <c r="Q34" s="15" t="s">
-        <v>50</v>
+        <v>228</v>
       </c>
       <c r="R34" s="17"/>
       <c r="S34" s="15">
@@ -3624,13 +3632,13 @@
         <v>142</v>
       </c>
       <c r="T34" s="15">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="U34" s="20" t="s">
-        <v>356</v>
+        <v>198</v>
       </c>
       <c r="V34" s="15" t="s">
-        <v>197</v>
+        <v>366</v>
       </c>
       <c r="W34" s="12"/>
     </row>
@@ -3641,13 +3649,13 @@
         <v>15</v>
       </c>
       <c r="C35" s="15">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="D35" s="20" t="s">
-        <v>235</v>
+        <v>77</v>
       </c>
       <c r="E35" s="15" t="s">
-        <v>81</v>
+        <v>270</v>
       </c>
       <c r="F35" s="12"/>
       <c r="G35" s="15">
@@ -3655,13 +3663,13 @@
         <v>57</v>
       </c>
       <c r="H35" s="15">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="I35" s="20" t="s">
-        <v>273</v>
+        <v>115</v>
       </c>
       <c r="J35" s="15" t="s">
-        <v>66</v>
+        <v>242</v>
       </c>
       <c r="K35" s="12"/>
       <c r="L35" s="10"/>
@@ -3671,13 +3679,13 @@
         <v>99</v>
       </c>
       <c r="O35" s="15">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="P35" s="20" t="s">
-        <v>315</v>
+        <v>157</v>
       </c>
       <c r="Q35" s="15" t="s">
-        <v>185</v>
+        <v>380</v>
       </c>
       <c r="R35" s="17"/>
       <c r="S35" s="15">
@@ -3685,13 +3693,13 @@
         <v>141</v>
       </c>
       <c r="T35" s="15">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="U35" s="20" t="s">
-        <v>357</v>
+        <v>199</v>
       </c>
       <c r="V35" s="15" t="s">
-        <v>171</v>
+        <v>353</v>
       </c>
       <c r="W35" s="12"/>
     </row>
@@ -3702,13 +3710,13 @@
         <v>14</v>
       </c>
       <c r="C36" s="15">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D36" s="20" t="s">
-        <v>236</v>
+        <v>78</v>
       </c>
       <c r="E36" s="15" t="s">
-        <v>95</v>
+        <v>256</v>
       </c>
       <c r="F36" s="12"/>
       <c r="G36" s="15">
@@ -3716,13 +3724,13 @@
         <v>56</v>
       </c>
       <c r="H36" s="15">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="I36" s="20" t="s">
-        <v>274</v>
+        <v>116</v>
       </c>
       <c r="J36" s="15" t="s">
-        <v>54</v>
+        <v>229</v>
       </c>
       <c r="K36" s="12"/>
       <c r="L36" s="10"/>
@@ -3732,13 +3740,13 @@
         <v>98</v>
       </c>
       <c r="O36" s="15">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="P36" s="20" t="s">
-        <v>316</v>
+        <v>158</v>
       </c>
       <c r="Q36" s="15" t="s">
-        <v>198</v>
+        <v>367</v>
       </c>
       <c r="R36" s="17"/>
       <c r="S36" s="15">
@@ -3746,13 +3754,13 @@
         <v>140</v>
       </c>
       <c r="T36" s="15">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="U36" s="20" t="s">
-        <v>358</v>
+        <v>200</v>
       </c>
       <c r="V36" s="15" t="s">
-        <v>158</v>
+        <v>340</v>
       </c>
       <c r="W36" s="12"/>
     </row>
@@ -3819,7 +3827,7 @@
         <v>40</v>
       </c>
       <c r="D39" s="18" t="s">
-        <v>204</v>
+        <v>46</v>
       </c>
       <c r="E39" s="14" t="s">
         <v>45</v>
@@ -3832,7 +3840,7 @@
         <v>40</v>
       </c>
       <c r="I39" s="18" t="s">
-        <v>204</v>
+        <v>46</v>
       </c>
       <c r="J39" s="14" t="s">
         <v>45</v>
@@ -3847,7 +3855,7 @@
         <v>40</v>
       </c>
       <c r="P39" s="18" t="s">
-        <v>204</v>
+        <v>46</v>
       </c>
       <c r="Q39" s="14" t="s">
         <v>45</v>
@@ -3860,7 +3868,7 @@
         <v>40</v>
       </c>
       <c r="U39" s="18" t="s">
-        <v>204</v>
+        <v>46</v>
       </c>
       <c r="V39" s="14" t="s">
         <v>45</v>
@@ -3877,10 +3885,10 @@
         <v>14</v>
       </c>
       <c r="D40" s="20" t="s">
-        <v>237</v>
+        <v>79</v>
       </c>
       <c r="E40" s="15" t="s">
-        <v>67</v>
+        <v>243</v>
       </c>
       <c r="F40" s="12"/>
       <c r="G40" s="15">
@@ -3891,10 +3899,10 @@
         <v>14</v>
       </c>
       <c r="I40" s="20" t="s">
-        <v>275</v>
+        <v>117</v>
       </c>
       <c r="J40" s="15" t="s">
-        <v>133</v>
+        <v>326</v>
       </c>
       <c r="K40" s="12"/>
       <c r="L40" s="10"/>
@@ -3907,10 +3915,10 @@
         <v>14</v>
       </c>
       <c r="P40" s="20" t="s">
-        <v>317</v>
+        <v>159</v>
       </c>
       <c r="Q40" s="15" t="s">
-        <v>172</v>
+        <v>354</v>
       </c>
       <c r="R40" s="12"/>
       <c r="S40" s="15">
@@ -3921,10 +3929,10 @@
         <v>14</v>
       </c>
       <c r="U40" s="20" t="s">
-        <v>359</v>
+        <v>201</v>
       </c>
       <c r="V40" s="15" t="s">
-        <v>129</v>
+        <v>327</v>
       </c>
       <c r="W40" s="12"/>
     </row>
@@ -3938,10 +3946,10 @@
         <v>13</v>
       </c>
       <c r="D41" s="20" t="s">
-        <v>238</v>
+        <v>80</v>
       </c>
       <c r="E41" s="15" t="s">
-        <v>55</v>
+        <v>230</v>
       </c>
       <c r="F41" s="12"/>
       <c r="G41" s="15">
@@ -3952,10 +3960,10 @@
         <v>13</v>
       </c>
       <c r="I41" s="20" t="s">
-        <v>276</v>
+        <v>118</v>
       </c>
       <c r="J41" s="15" t="s">
-        <v>146</v>
+        <v>311</v>
       </c>
       <c r="K41" s="12"/>
       <c r="L41" s="10"/>
@@ -3968,10 +3976,10 @@
         <v>13</v>
       </c>
       <c r="P41" s="20" t="s">
-        <v>318</v>
+        <v>160</v>
       </c>
       <c r="Q41" s="15" t="s">
-        <v>159</v>
+        <v>341</v>
       </c>
       <c r="R41" s="12"/>
       <c r="S41" s="15">
@@ -3982,10 +3990,10 @@
         <v>13</v>
       </c>
       <c r="U41" s="20" t="s">
-        <v>360</v>
+        <v>202</v>
       </c>
       <c r="V41" s="15" t="s">
-        <v>142</v>
+        <v>312</v>
       </c>
       <c r="W41" s="12"/>
     </row>
@@ -3999,10 +4007,10 @@
         <v>12</v>
       </c>
       <c r="D42" s="20" t="s">
-        <v>239</v>
+        <v>81</v>
       </c>
       <c r="E42" s="15" t="s">
-        <v>186</v>
+        <v>381</v>
       </c>
       <c r="F42" s="12"/>
       <c r="G42" s="15">
@@ -4013,10 +4021,10 @@
         <v>12</v>
       </c>
       <c r="I42" s="20" t="s">
-        <v>277</v>
+        <v>119</v>
       </c>
       <c r="J42" s="15" t="s">
-        <v>122</v>
+        <v>299</v>
       </c>
       <c r="K42" s="12"/>
       <c r="L42" s="10"/>
@@ -4029,10 +4037,10 @@
         <v>12</v>
       </c>
       <c r="P42" s="20" t="s">
-        <v>319</v>
+        <v>161</v>
       </c>
       <c r="Q42" s="15" t="s">
-        <v>130</v>
+        <v>328</v>
       </c>
       <c r="R42" s="12"/>
       <c r="S42" s="15">
@@ -4043,10 +4051,10 @@
         <v>12</v>
       </c>
       <c r="U42" s="20" t="s">
-        <v>361</v>
+        <v>203</v>
       </c>
       <c r="V42" s="15" t="s">
-        <v>118</v>
+        <v>300</v>
       </c>
       <c r="W42" s="12"/>
     </row>
@@ -4060,10 +4068,10 @@
         <v>11</v>
       </c>
       <c r="D43" s="20" t="s">
-        <v>240</v>
+        <v>82</v>
       </c>
       <c r="E43" s="15" t="s">
-        <v>199</v>
+        <v>368</v>
       </c>
       <c r="F43" s="12"/>
       <c r="G43" s="15">
@@ -4074,10 +4082,10 @@
         <v>11</v>
       </c>
       <c r="I43" s="20" t="s">
-        <v>278</v>
+        <v>120</v>
       </c>
       <c r="J43" s="15" t="s">
-        <v>109</v>
+        <v>285</v>
       </c>
       <c r="K43" s="12"/>
       <c r="L43" s="10"/>
@@ -4090,10 +4098,10 @@
         <v>11</v>
       </c>
       <c r="P43" s="20" t="s">
-        <v>320</v>
+        <v>162</v>
       </c>
       <c r="Q43" s="15" t="s">
-        <v>143</v>
+        <v>313</v>
       </c>
       <c r="R43" s="12"/>
       <c r="S43" s="15">
@@ -4104,10 +4112,10 @@
         <v>11</v>
       </c>
       <c r="U43" s="20" t="s">
-        <v>362</v>
+        <v>204</v>
       </c>
       <c r="V43" s="15" t="s">
-        <v>105</v>
+        <v>286</v>
       </c>
       <c r="W43" s="12"/>
     </row>
@@ -4121,10 +4129,10 @@
         <v>10</v>
       </c>
       <c r="D44" s="20" t="s">
-        <v>241</v>
+        <v>83</v>
       </c>
       <c r="E44" s="15" t="s">
-        <v>173</v>
+        <v>355</v>
       </c>
       <c r="F44" s="12"/>
       <c r="G44" s="15">
@@ -4135,10 +4143,10 @@
         <v>10</v>
       </c>
       <c r="I44" s="20" t="s">
-        <v>279</v>
+        <v>121</v>
       </c>
       <c r="J44" s="15" t="s">
-        <v>82</v>
+        <v>271</v>
       </c>
       <c r="K44" s="12"/>
       <c r="L44" s="10"/>
@@ -4151,10 +4159,10 @@
         <v>10</v>
       </c>
       <c r="P44" s="20" t="s">
-        <v>321</v>
+        <v>163</v>
       </c>
       <c r="Q44" s="15" t="s">
-        <v>119</v>
+        <v>301</v>
       </c>
       <c r="R44" s="12"/>
       <c r="S44" s="15">
@@ -4165,10 +4173,10 @@
         <v>10</v>
       </c>
       <c r="U44" s="20" t="s">
-        <v>363</v>
+        <v>205</v>
       </c>
       <c r="V44" s="15" t="s">
-        <v>78</v>
+        <v>272</v>
       </c>
       <c r="W44" s="12"/>
     </row>
@@ -4182,10 +4190,10 @@
         <v>9</v>
       </c>
       <c r="D45" s="20" t="s">
-        <v>242</v>
+        <v>84</v>
       </c>
       <c r="E45" s="15" t="s">
-        <v>160</v>
+        <v>342</v>
       </c>
       <c r="F45" s="12"/>
       <c r="G45" s="15">
@@ -4196,10 +4204,10 @@
         <v>9</v>
       </c>
       <c r="I45" s="20" t="s">
-        <v>280</v>
+        <v>122</v>
       </c>
       <c r="J45" s="15" t="s">
-        <v>96</v>
+        <v>257</v>
       </c>
       <c r="K45" s="12"/>
       <c r="L45" s="10"/>
@@ -4212,10 +4220,10 @@
         <v>9</v>
       </c>
       <c r="P45" s="20" t="s">
-        <v>322</v>
+        <v>164</v>
       </c>
       <c r="Q45" s="15" t="s">
-        <v>106</v>
+        <v>287</v>
       </c>
       <c r="R45" s="12"/>
       <c r="S45" s="15">
@@ -4226,10 +4234,10 @@
         <v>9</v>
       </c>
       <c r="U45" s="20" t="s">
-        <v>364</v>
+        <v>206</v>
       </c>
       <c r="V45" s="15" t="s">
-        <v>92</v>
+        <v>258</v>
       </c>
       <c r="W45" s="12"/>
     </row>
@@ -4243,10 +4251,10 @@
         <v>8</v>
       </c>
       <c r="D46" s="20" t="s">
-        <v>243</v>
+        <v>85</v>
       </c>
       <c r="E46" s="15" t="s">
-        <v>135</v>
+        <v>329</v>
       </c>
       <c r="F46" s="12"/>
       <c r="G46" s="15">
@@ -4257,10 +4265,10 @@
         <v>8</v>
       </c>
       <c r="I46" s="20" t="s">
-        <v>281</v>
+        <v>123</v>
       </c>
       <c r="J46" s="15" t="s">
-        <v>68</v>
+        <v>244</v>
       </c>
       <c r="K46" s="12"/>
       <c r="L46" s="10"/>
@@ -4273,10 +4281,10 @@
         <v>8</v>
       </c>
       <c r="P46" s="20" t="s">
-        <v>323</v>
+        <v>165</v>
       </c>
       <c r="Q46" s="15" t="s">
-        <v>79</v>
+        <v>273</v>
       </c>
       <c r="R46" s="12"/>
       <c r="S46" s="15">
@@ -4287,10 +4295,10 @@
         <v>8</v>
       </c>
       <c r="U46" s="20" t="s">
-        <v>365</v>
+        <v>207</v>
       </c>
       <c r="V46" s="15" t="s">
-        <v>65</v>
+        <v>245</v>
       </c>
       <c r="W46" s="12"/>
     </row>
@@ -4304,10 +4312,10 @@
         <v>7</v>
       </c>
       <c r="D47" s="20" t="s">
-        <v>223</v>
+        <v>65</v>
       </c>
       <c r="E47" s="15" t="s">
-        <v>148</v>
+        <v>314</v>
       </c>
       <c r="F47" s="12"/>
       <c r="G47" s="15">
@@ -4318,10 +4326,10 @@
         <v>7</v>
       </c>
       <c r="I47" s="20" t="s">
-        <v>282</v>
+        <v>124</v>
       </c>
       <c r="J47" s="15" t="s">
-        <v>56</v>
+        <v>231</v>
       </c>
       <c r="K47" s="12"/>
       <c r="L47" s="10"/>
@@ -4334,10 +4342,10 @@
         <v>7</v>
       </c>
       <c r="P47" s="20" t="s">
-        <v>324</v>
+        <v>166</v>
       </c>
       <c r="Q47" s="15" t="s">
-        <v>93</v>
+        <v>259</v>
       </c>
       <c r="R47" s="12"/>
       <c r="S47" s="15">
@@ -4348,10 +4356,10 @@
         <v>7</v>
       </c>
       <c r="U47" s="20" t="s">
-        <v>366</v>
+        <v>208</v>
       </c>
       <c r="V47" s="15" t="s">
-        <v>53</v>
+        <v>232</v>
       </c>
       <c r="W47" s="12"/>
     </row>
@@ -4365,10 +4373,10 @@
         <v>6</v>
       </c>
       <c r="D48" s="20" t="s">
-        <v>244</v>
+        <v>86</v>
       </c>
       <c r="E48" s="15" t="s">
-        <v>124</v>
+        <v>302</v>
       </c>
       <c r="F48" s="12"/>
       <c r="G48" s="15">
@@ -4379,10 +4387,10 @@
         <v>6</v>
       </c>
       <c r="I48" s="20" t="s">
-        <v>283</v>
+        <v>125</v>
       </c>
       <c r="J48" s="15" t="s">
-        <v>187</v>
+        <v>382</v>
       </c>
       <c r="K48" s="12"/>
       <c r="L48" s="10"/>
@@ -4395,10 +4403,10 @@
         <v>6</v>
       </c>
       <c r="P48" s="20" t="s">
-        <v>325</v>
-      </c>
-      <c r="Q48" s="38" t="s">
-        <v>384</v>
+        <v>167</v>
+      </c>
+      <c r="Q48" s="26" t="s">
+        <v>330</v>
       </c>
       <c r="R48" s="12"/>
       <c r="S48" s="15">
@@ -4409,10 +4417,10 @@
         <v>6</v>
       </c>
       <c r="U48" s="20" t="s">
-        <v>367</v>
+        <v>209</v>
       </c>
       <c r="V48" s="15" t="s">
-        <v>188</v>
+        <v>383</v>
       </c>
       <c r="W48" s="12"/>
     </row>
@@ -4426,10 +4434,10 @@
         <v>5</v>
       </c>
       <c r="D49" s="20" t="s">
-        <v>245</v>
+        <v>87</v>
       </c>
       <c r="E49" s="15" t="s">
-        <v>111</v>
+        <v>288</v>
       </c>
       <c r="F49" s="12"/>
       <c r="G49" s="15">
@@ -4440,10 +4448,10 @@
         <v>5</v>
       </c>
       <c r="I49" s="20" t="s">
-        <v>284</v>
+        <v>126</v>
       </c>
       <c r="J49" s="15" t="s">
-        <v>200</v>
+        <v>369</v>
       </c>
       <c r="K49" s="12"/>
       <c r="L49" s="10"/>
@@ -4456,10 +4464,10 @@
         <v>5</v>
       </c>
       <c r="P49" s="20" t="s">
-        <v>326</v>
-      </c>
-      <c r="Q49" s="38" t="s">
-        <v>383</v>
+        <v>168</v>
+      </c>
+      <c r="Q49" s="26" t="s">
+        <v>315</v>
       </c>
       <c r="R49" s="12"/>
       <c r="S49" s="15">
@@ -4470,10 +4478,10 @@
         <v>5</v>
       </c>
       <c r="U49" s="20" t="s">
-        <v>368</v>
+        <v>210</v>
       </c>
       <c r="V49" s="15" t="s">
-        <v>201</v>
+        <v>370</v>
       </c>
       <c r="W49" s="12"/>
     </row>
@@ -4487,10 +4495,10 @@
         <v>4</v>
       </c>
       <c r="D50" s="20" t="s">
-        <v>246</v>
+        <v>88</v>
       </c>
       <c r="E50" s="15" t="s">
-        <v>84</v>
+        <v>274</v>
       </c>
       <c r="F50" s="12"/>
       <c r="G50" s="15">
@@ -4501,10 +4509,10 @@
         <v>4</v>
       </c>
       <c r="I50" s="20" t="s">
-        <v>285</v>
+        <v>127</v>
       </c>
       <c r="J50" s="15" t="s">
-        <v>174</v>
+        <v>356</v>
       </c>
       <c r="K50" s="12"/>
       <c r="L50" s="10"/>
@@ -4517,10 +4525,10 @@
         <v>4</v>
       </c>
       <c r="P50" s="20" t="s">
-        <v>327</v>
+        <v>169</v>
       </c>
       <c r="Q50" s="15" t="s">
-        <v>189</v>
+        <v>384</v>
       </c>
       <c r="R50" s="12"/>
       <c r="S50" s="15">
@@ -4531,10 +4539,10 @@
         <v>4</v>
       </c>
       <c r="U50" s="20" t="s">
-        <v>369</v>
+        <v>211</v>
       </c>
       <c r="V50" s="15" t="s">
-        <v>175</v>
+        <v>357</v>
       </c>
       <c r="W50" s="12"/>
     </row>
@@ -4548,10 +4556,10 @@
         <v>3</v>
       </c>
       <c r="D51" s="20" t="s">
-        <v>207</v>
+        <v>49</v>
       </c>
       <c r="E51" s="15" t="s">
-        <v>98</v>
+        <v>260</v>
       </c>
       <c r="F51" s="12"/>
       <c r="G51" s="15">
@@ -4562,10 +4570,10 @@
         <v>3</v>
       </c>
       <c r="I51" s="20" t="s">
-        <v>286</v>
+        <v>128</v>
       </c>
       <c r="J51" s="15" t="s">
-        <v>161</v>
+        <v>343</v>
       </c>
       <c r="K51" s="12"/>
       <c r="L51" s="10"/>
@@ -4578,10 +4586,10 @@
         <v>3</v>
       </c>
       <c r="P51" s="20" t="s">
-        <v>328</v>
+        <v>170</v>
       </c>
       <c r="Q51" s="15" t="s">
-        <v>202</v>
+        <v>371</v>
       </c>
       <c r="R51" s="12"/>
       <c r="S51" s="15">
@@ -4592,10 +4600,10 @@
         <v>3</v>
       </c>
       <c r="U51" s="20" t="s">
-        <v>370</v>
+        <v>212</v>
       </c>
       <c r="V51" s="15" t="s">
-        <v>162</v>
+        <v>344</v>
       </c>
       <c r="W51" s="12"/>
     </row>
@@ -4609,10 +4617,10 @@
         <v>2</v>
       </c>
       <c r="D52" s="19" t="s">
-        <v>206</v>
+        <v>48</v>
       </c>
       <c r="E52" s="15" t="s">
-        <v>70</v>
+        <v>246</v>
       </c>
       <c r="F52" s="12"/>
       <c r="G52" s="15">
@@ -4623,10 +4631,10 @@
         <v>2</v>
       </c>
       <c r="I52" s="19" t="s">
-        <v>287</v>
+        <v>129</v>
       </c>
       <c r="J52" s="15" t="s">
-        <v>136</v>
+        <v>331</v>
       </c>
       <c r="K52" s="12"/>
       <c r="L52" s="10"/>
@@ -4639,10 +4647,10 @@
         <v>2</v>
       </c>
       <c r="P52" s="19" t="s">
-        <v>329</v>
+        <v>171</v>
       </c>
       <c r="Q52" s="15" t="s">
-        <v>176</v>
+        <v>358</v>
       </c>
       <c r="R52" s="12"/>
       <c r="S52" s="15">
@@ -4653,10 +4661,10 @@
         <v>2</v>
       </c>
       <c r="U52" s="19" t="s">
-        <v>371</v>
+        <v>213</v>
       </c>
       <c r="V52" s="15" t="s">
-        <v>134</v>
+        <v>332</v>
       </c>
       <c r="W52" s="12"/>
     </row>
@@ -4669,10 +4677,10 @@
         <v>1</v>
       </c>
       <c r="D53" s="19" t="s">
-        <v>205</v>
-      </c>
-      <c r="E53" s="15" t="s">
-        <v>203</v>
+        <v>47</v>
+      </c>
+      <c r="E53" s="37" t="s">
+        <v>233</v>
       </c>
       <c r="F53" s="12"/>
       <c r="G53" s="15">
@@ -4683,10 +4691,10 @@
         <v>1</v>
       </c>
       <c r="I53" s="19" t="s">
-        <v>288</v>
+        <v>130</v>
       </c>
       <c r="J53" s="15" t="s">
-        <v>149</v>
+        <v>316</v>
       </c>
       <c r="K53" s="12"/>
       <c r="L53" s="10"/>
@@ -4699,10 +4707,10 @@
         <v>1</v>
       </c>
       <c r="P53" s="19" t="s">
-        <v>330</v>
+        <v>172</v>
       </c>
       <c r="Q53" s="15" t="s">
-        <v>163</v>
+        <v>345</v>
       </c>
       <c r="R53" s="12"/>
       <c r="S53" s="15">
@@ -4713,10 +4721,10 @@
         <v>1</v>
       </c>
       <c r="U53" s="19" t="s">
-        <v>372</v>
+        <v>214</v>
       </c>
       <c r="V53" s="15" t="s">
-        <v>147</v>
+        <v>317</v>
       </c>
       <c r="W53" s="12"/>
     </row>
@@ -4781,30 +4789,30 @@
   <sheetData>
     <row r="1" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="32"/>
+      <c r="C1" s="34"/>
       <c r="D1" s="2"/>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="32"/>
+      <c r="F1" s="34"/>
       <c r="G1" s="2"/>
-      <c r="H1" s="31" t="s">
+      <c r="H1" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="32"/>
+      <c r="I1" s="34"/>
       <c r="J1" s="2"/>
-      <c r="K1" s="34" t="s">
+      <c r="K1" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="32"/>
+      <c r="L1" s="34"/>
       <c r="M1" s="2"/>
-      <c r="N1" s="31" t="s">
+      <c r="N1" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="O1" s="32"/>
+      <c r="O1" s="34"/>
       <c r="P1" s="2"/>
     </row>
     <row r="2" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5189,30 +5197,30 @@
     </row>
     <row r="12" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
-      <c r="B12" s="33" t="s">
+      <c r="B12" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="32"/>
+      <c r="C12" s="34"/>
       <c r="D12" s="2"/>
-      <c r="E12" s="31" t="s">
+      <c r="E12" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="32"/>
+      <c r="F12" s="34"/>
       <c r="G12" s="2"/>
-      <c r="H12" s="31" t="s">
+      <c r="H12" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="I12" s="32"/>
+      <c r="I12" s="34"/>
       <c r="J12" s="2"/>
-      <c r="K12" s="34" t="s">
+      <c r="K12" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="L12" s="32"/>
+      <c r="L12" s="34"/>
       <c r="M12" s="2"/>
-      <c r="N12" s="31" t="s">
+      <c r="N12" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="O12" s="32"/>
+      <c r="O12" s="34"/>
       <c r="P12" s="2"/>
       <c r="S12" s="22"/>
       <c r="U12" s="22"/>
@@ -5358,7 +5366,7 @@
         <v>13</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>374</v>
+        <v>216</v>
       </c>
       <c r="K16" s="5">
         <v>93</v>
@@ -5398,7 +5406,7 @@
         <v>14</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>374</v>
+        <v>216</v>
       </c>
       <c r="K17" s="5">
         <v>92</v>
@@ -5525,7 +5533,7 @@
         <v>17</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>374</v>
+        <v>216</v>
       </c>
       <c r="N20" s="5">
         <v>101</v>
@@ -5534,7 +5542,6 @@
         <v>17</v>
       </c>
       <c r="P20" s="2"/>
-      <c r="Q20" s="35"/>
       <c r="S20" s="22"/>
       <c r="U20" s="22"/>
     </row>
@@ -5566,7 +5573,7 @@
         <v>18</v>
       </c>
       <c r="M21" s="4" t="s">
-        <v>374</v>
+        <v>216</v>
       </c>
       <c r="N21" s="5">
         <v>100</v>
@@ -5575,7 +5582,6 @@
         <v>18</v>
       </c>
       <c r="P21" s="2"/>
-      <c r="Q21" s="35"/>
       <c r="S21" s="22"/>
       <c r="U21" s="22"/>
     </row>
@@ -5596,38 +5602,37 @@
       <c r="N22" s="4"/>
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
-      <c r="Q22" s="35"/>
       <c r="S22" s="22"/>
       <c r="U22" s="22"/>
     </row>
     <row r="23" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
-      <c r="B23" s="31" t="s">
+      <c r="B23" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="32"/>
+      <c r="C23" s="34"/>
       <c r="D23" s="2"/>
-      <c r="E23" s="31" t="s">
+      <c r="E23" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="F23" s="32"/>
+      <c r="F23" s="34"/>
       <c r="G23" s="2"/>
-      <c r="H23" s="34" t="s">
+      <c r="H23" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="I23" s="32"/>
+      <c r="I23" s="34"/>
       <c r="J23" s="2"/>
-      <c r="K23" s="31" t="s">
+      <c r="K23" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="L23" s="32"/>
+      <c r="L23" s="34"/>
       <c r="M23" s="2"/>
-      <c r="N23" s="31" t="s">
-        <v>373</v>
-      </c>
-      <c r="O23" s="32"/>
+      <c r="N23" s="33" t="s">
+        <v>215</v>
+      </c>
+      <c r="O23" s="34"/>
       <c r="P23" s="2"/>
-      <c r="Q23" s="36"/>
+      <c r="Q23" s="6"/>
       <c r="S23" s="22"/>
       <c r="U23" s="22"/>
     </row>
@@ -5668,7 +5673,7 @@
         <v>6</v>
       </c>
       <c r="P24" s="2"/>
-      <c r="Q24" s="36"/>
+      <c r="Q24" s="6"/>
       <c r="S24" s="22"/>
       <c r="U24" s="22"/>
     </row>
@@ -5709,7 +5714,7 @@
         <v>11</v>
       </c>
       <c r="P25" s="2"/>
-      <c r="Q25" s="36"/>
+      <c r="Q25" s="6"/>
       <c r="S25" s="22"/>
       <c r="U25" s="22"/>
     </row>
@@ -5751,7 +5756,7 @@
         <v>12</v>
       </c>
       <c r="P26" s="2"/>
-      <c r="Q26" s="36"/>
+      <c r="Q26" s="6"/>
       <c r="S26" s="22"/>
       <c r="U26" s="22"/>
     </row>
@@ -5793,7 +5798,7 @@
         <v>13</v>
       </c>
       <c r="P27" s="2"/>
-      <c r="Q27" s="36"/>
+      <c r="Q27" s="6"/>
       <c r="S27" s="22"/>
       <c r="U27" s="22"/>
     </row>
@@ -5835,7 +5840,7 @@
         <v>14</v>
       </c>
       <c r="P28" s="2"/>
-      <c r="Q28" s="36"/>
+      <c r="Q28" s="6"/>
       <c r="S28" s="22"/>
       <c r="U28" s="22"/>
     </row>
@@ -5877,7 +5882,7 @@
         <v>15</v>
       </c>
       <c r="P29" s="2"/>
-      <c r="Q29" s="36"/>
+      <c r="Q29" s="6"/>
       <c r="S29" s="22"/>
       <c r="U29" s="22"/>
     </row>
@@ -5919,7 +5924,7 @@
         <v>16</v>
       </c>
       <c r="P30" s="2"/>
-      <c r="Q30" s="36"/>
+      <c r="Q30" s="6"/>
       <c r="S30" s="22"/>
       <c r="U30" s="22"/>
     </row>
@@ -5961,7 +5966,7 @@
         <v>17</v>
       </c>
       <c r="P31" s="2"/>
-      <c r="Q31" s="36"/>
+      <c r="Q31" s="6"/>
       <c r="S31" s="22"/>
       <c r="U31" s="22"/>
     </row>
@@ -6003,7 +6008,7 @@
         <v>18</v>
       </c>
       <c r="P32" s="2"/>
-      <c r="Q32" s="36"/>
+      <c r="Q32" s="6"/>
       <c r="S32" s="22"/>
       <c r="U32" s="22"/>
     </row>
@@ -6024,7 +6029,7 @@
       <c r="N33" s="4"/>
       <c r="O33" s="4"/>
       <c r="P33" s="4"/>
-      <c r="Q33" s="37"/>
+      <c r="Q33" s="25"/>
       <c r="S33" s="22"/>
       <c r="U33" s="22"/>
     </row>
@@ -6045,7 +6050,7 @@
       <c r="N34" s="4"/>
       <c r="O34" s="4"/>
       <c r="P34" s="4"/>
-      <c r="Q34" s="37"/>
+      <c r="Q34" s="25"/>
       <c r="S34" s="22"/>
       <c r="U34" s="22"/>
     </row>
@@ -6110,30 +6115,30 @@
   <sheetData>
     <row r="1" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="32"/>
+      <c r="C1" s="34"/>
       <c r="D1" s="2"/>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="32"/>
+      <c r="F1" s="34"/>
       <c r="G1" s="2"/>
-      <c r="H1" s="31" t="s">
+      <c r="H1" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="32"/>
+      <c r="I1" s="34"/>
       <c r="J1" s="2"/>
-      <c r="K1" s="34" t="s">
+      <c r="K1" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="32"/>
+      <c r="L1" s="34"/>
       <c r="M1" s="2"/>
-      <c r="N1" s="31" t="s">
+      <c r="N1" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="O1" s="32"/>
+      <c r="O1" s="34"/>
       <c r="P1" s="2"/>
     </row>
     <row r="2" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6342,30 +6347,30 @@
     </row>
     <row r="8" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="32"/>
+      <c r="C8" s="34"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="31" t="s">
+      <c r="E8" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="32"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="2"/>
-      <c r="H8" s="31" t="s">
+      <c r="H8" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="32"/>
+      <c r="I8" s="34"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="34" t="s">
+      <c r="K8" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="L8" s="32"/>
+      <c r="L8" s="34"/>
       <c r="M8" s="2"/>
-      <c r="N8" s="31" t="s">
+      <c r="N8" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="O8" s="32"/>
+      <c r="O8" s="34"/>
       <c r="P8" s="2"/>
       <c r="S8" s="22"/>
       <c r="U8" s="22"/>
@@ -6587,38 +6592,37 @@
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
-      <c r="Q14" s="35"/>
       <c r="S14" s="22"/>
       <c r="U14" s="22"/>
     </row>
     <row r="15" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
-      <c r="B15" s="31" t="s">
+      <c r="B15" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="32"/>
+      <c r="C15" s="34"/>
       <c r="D15" s="2"/>
-      <c r="E15" s="31" t="s">
+      <c r="E15" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="F15" s="32"/>
+      <c r="F15" s="34"/>
       <c r="G15" s="2"/>
-      <c r="H15" s="34" t="s">
+      <c r="H15" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="I15" s="32"/>
+      <c r="I15" s="34"/>
       <c r="J15" s="2"/>
-      <c r="K15" s="31" t="s">
+      <c r="K15" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="L15" s="32"/>
+      <c r="L15" s="34"/>
       <c r="M15" s="2"/>
-      <c r="N15" s="31" t="s">
+      <c r="N15" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="O15" s="32"/>
+      <c r="O15" s="34"/>
       <c r="P15" s="2"/>
-      <c r="Q15" s="36"/>
+      <c r="Q15" s="6"/>
       <c r="S15" s="22"/>
       <c r="U15" s="22"/>
     </row>
@@ -6659,7 +6663,7 @@
         <v>6</v>
       </c>
       <c r="P16" s="2"/>
-      <c r="Q16" s="36"/>
+      <c r="Q16" s="6"/>
       <c r="S16" s="22"/>
       <c r="U16" s="22"/>
     </row>
@@ -6696,7 +6700,7 @@
         <v>7</v>
       </c>
       <c r="P17" s="2"/>
-      <c r="Q17" s="36"/>
+      <c r="Q17" s="6"/>
       <c r="S17" s="22"/>
       <c r="U17" s="22"/>
     </row>
@@ -6734,7 +6738,7 @@
         <v>8</v>
       </c>
       <c r="P18" s="2"/>
-      <c r="Q18" s="36"/>
+      <c r="Q18" s="6"/>
       <c r="S18" s="23"/>
       <c r="U18" s="23"/>
     </row>
@@ -6772,7 +6776,7 @@
         <v>9</v>
       </c>
       <c r="P19" s="2"/>
-      <c r="Q19" s="36"/>
+      <c r="Q19" s="6"/>
       <c r="S19" s="24"/>
       <c r="U19" s="24"/>
     </row>
@@ -6810,7 +6814,7 @@
         <v>10</v>
       </c>
       <c r="P20" s="2"/>
-      <c r="Q20" s="36"/>
+      <c r="Q20" s="6"/>
       <c r="S20" s="21"/>
       <c r="U20" s="21"/>
     </row>
@@ -6831,7 +6835,7 @@
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
       <c r="P21" s="4"/>
-      <c r="Q21" s="37"/>
+      <c r="Q21" s="25"/>
       <c r="S21" s="22"/>
       <c r="U21" s="22"/>
     </row>
@@ -6857,21 +6861,21 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="N1:O1"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="E15:F15"/>
     <mergeCell ref="H15:I15"/>
     <mergeCell ref="K15:L15"/>
     <mergeCell ref="N15:O15"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="N8:O8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
updated cable maps and map for unused pixels
</commit_message>
<xml_diff>
--- a/Cables and Labels/CableMapping.xlsx
+++ b/Cables and Labels/CableMapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/spaubt/Desktop/CDet/Cables and Labels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9765643D-E4F5-164E-BEF4-AB0BC65C2A83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80BF483A-5399-884A-938E-5CF2C0E0FBA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-960" yWindow="800" windowWidth="26000" windowHeight="16680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16680" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cdet TDC Cable Map" sheetId="4" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="387">
   <si>
     <t>Slot 3</t>
   </si>
@@ -683,9 +683,6 @@
     <t>CDET_2R0</t>
   </si>
   <si>
-    <t>Slot 20</t>
-  </si>
-  <si>
     <t>&lt;- UNUSED</t>
   </si>
   <si>
@@ -707,9 +704,6 @@
     <t>17, 0-15</t>
   </si>
   <si>
-    <t>20, 0-15</t>
-  </si>
-  <si>
     <t>16, 0-15</t>
   </si>
   <si>
@@ -746,9 +740,6 @@
     <t>17, 16-31</t>
   </si>
   <si>
-    <t>20, 16-31</t>
-  </si>
-  <si>
     <t>16, 16-31</t>
   </si>
   <si>
@@ -785,9 +776,6 @@
     <t>17, 32-47</t>
   </si>
   <si>
-    <t>20, 32-47</t>
-  </si>
-  <si>
     <t>16, 32-47</t>
   </si>
   <si>
@@ -827,9 +815,6 @@
     <t>17, 48-63</t>
   </si>
   <si>
-    <t>20, 48-63</t>
-  </si>
-  <si>
     <t>16, 48-63</t>
   </si>
   <si>
@@ -869,9 +854,6 @@
     <t>17, 64-79</t>
   </si>
   <si>
-    <t>20, 64-79</t>
-  </si>
-  <si>
     <t>16, 64-79</t>
   </si>
   <si>
@@ -911,9 +893,6 @@
     <t>17, 80-95</t>
   </si>
   <si>
-    <t>20, 80-95</t>
-  </si>
-  <si>
     <t>16, 80-95</t>
   </si>
   <si>
@@ -947,9 +926,6 @@
     <t>3, 80-95</t>
   </si>
   <si>
-    <t>20, 96-111</t>
-  </si>
-  <si>
     <t>16, 96-111</t>
   </si>
   <si>
@@ -992,9 +968,6 @@
     <t>17, 96-111</t>
   </si>
   <si>
-    <t>20, 112-127</t>
-  </si>
-  <si>
     <t>16, 112-127</t>
   </si>
   <si>
@@ -1191,17 +1164,57 @@
   </si>
   <si>
     <t>10, 176-191</t>
+  </si>
+  <si>
+    <t>7 no back</t>
+  </si>
+  <si>
+    <t>15 no back</t>
+  </si>
+  <si>
+    <t>13 no front</t>
+  </si>
+  <si>
+    <t>13, 112-127</t>
+  </si>
+  <si>
+    <t>13, 96-111</t>
+  </si>
+  <si>
+    <t>13, 80-95</t>
+  </si>
+  <si>
+    <t>13, 64-79</t>
+  </si>
+  <si>
+    <t>13, 48-63</t>
+  </si>
+  <si>
+    <t>13, 32-47</t>
+  </si>
+  <si>
+    <t>13, 16-31</t>
+  </si>
+  <si>
+    <t>13, 0-15</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1282,6 +1295,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -1333,7 +1353,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -1441,104 +1461,123 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1759,8 +1798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C267A411-0DF7-B748-9579-92A194184DBE}">
   <dimension ref="A2:W54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H17" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="Q48" sqref="Q48"/>
+    <sheetView topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="V18" sqref="V18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1790,102 +1829,102 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
-      <c r="H2" s="32" t="s">
+      <c r="H2" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
       <c r="L2" s="10"/>
-      <c r="M2" s="32" t="s">
+      <c r="M2" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="N2" s="32"/>
-      <c r="O2" s="32"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="34"/>
+      <c r="P2" s="34"/>
+      <c r="Q2" s="34"/>
       <c r="R2" s="9"/>
-      <c r="S2" s="32" t="s">
+      <c r="S2" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="T2" s="32"/>
-      <c r="U2" s="32"/>
-      <c r="V2" s="32"/>
-      <c r="W2" s="32"/>
+      <c r="T2" s="34"/>
+      <c r="U2" s="34"/>
+      <c r="V2" s="34"/>
+      <c r="W2" s="34"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
       <c r="L3" s="10"/>
-      <c r="M3" s="32" t="s">
+      <c r="M3" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="N3" s="32"/>
-      <c r="O3" s="32"/>
-      <c r="P3" s="32"/>
-      <c r="Q3" s="32"/>
-      <c r="R3" s="32"/>
-      <c r="S3" s="32"/>
-      <c r="T3" s="32"/>
-      <c r="U3" s="32"/>
-      <c r="V3" s="32"/>
-      <c r="W3" s="32"/>
+      <c r="N3" s="34"/>
+      <c r="O3" s="34"/>
+      <c r="P3" s="34"/>
+      <c r="Q3" s="34"/>
+      <c r="R3" s="34"/>
+      <c r="S3" s="34"/>
+      <c r="T3" s="34"/>
+      <c r="U3" s="34"/>
+      <c r="V3" s="34"/>
+      <c r="W3" s="34"/>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" s="12"/>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="28"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="30"/>
       <c r="F4" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="G4" s="29" t="s">
+      <c r="G4" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="31"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="33"/>
       <c r="K4" s="12"/>
       <c r="L4" s="10"/>
       <c r="M4" s="12"/>
-      <c r="N4" s="29" t="s">
+      <c r="N4" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="O4" s="30"/>
-      <c r="P4" s="30"/>
-      <c r="Q4" s="31"/>
+      <c r="O4" s="32"/>
+      <c r="P4" s="32"/>
+      <c r="Q4" s="33"/>
       <c r="R4" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="S4" s="29" t="s">
+      <c r="S4" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="T4" s="30"/>
-      <c r="U4" s="30"/>
-      <c r="V4" s="31"/>
+      <c r="T4" s="32"/>
+      <c r="U4" s="32"/>
+      <c r="V4" s="33"/>
       <c r="W4" s="12"/>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.2">
@@ -1958,7 +1997,7 @@
         <v>50</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="F6" s="12"/>
       <c r="G6" s="15">
@@ -1971,8 +2010,8 @@
       <c r="I6" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="J6" s="37" t="s">
-        <v>217</v>
+      <c r="J6" s="27" t="s">
+        <v>216</v>
       </c>
       <c r="K6" s="12"/>
       <c r="L6" s="10"/>
@@ -1988,7 +2027,7 @@
         <v>131</v>
       </c>
       <c r="Q6" s="15" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="R6" s="17"/>
       <c r="S6" s="15">
@@ -2002,7 +2041,7 @@
         <v>173</v>
       </c>
       <c r="V6" s="15" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="W6" s="12"/>
     </row>
@@ -2019,7 +2058,7 @@
         <v>51</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="F7" s="12"/>
       <c r="G7" s="15">
@@ -2032,8 +2071,8 @@
       <c r="I7" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="J7" s="37" t="s">
-        <v>218</v>
+      <c r="J7" s="27" t="s">
+        <v>217</v>
       </c>
       <c r="K7" s="12"/>
       <c r="L7" s="10"/>
@@ -2049,7 +2088,7 @@
         <v>132</v>
       </c>
       <c r="Q7" s="15" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="R7" s="17"/>
       <c r="S7" s="15">
@@ -2063,7 +2102,7 @@
         <v>174</v>
       </c>
       <c r="V7" s="15" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
       <c r="W7" s="12"/>
     </row>
@@ -2080,7 +2119,7 @@
         <v>52</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="F8" s="12"/>
       <c r="G8" s="15">
@@ -2093,8 +2132,8 @@
       <c r="I8" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="J8" s="37" t="s">
-        <v>219</v>
+      <c r="J8" s="27" t="s">
+        <v>218</v>
       </c>
       <c r="K8" s="12"/>
       <c r="L8" s="10"/>
@@ -2110,7 +2149,7 @@
         <v>133</v>
       </c>
       <c r="Q8" s="15" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="R8" s="17"/>
       <c r="S8" s="15">
@@ -2124,7 +2163,7 @@
         <v>175</v>
       </c>
       <c r="V8" s="15" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
       <c r="W8" s="12"/>
     </row>
@@ -2141,7 +2180,7 @@
         <v>53</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="F9" s="12"/>
       <c r="G9" s="15">
@@ -2154,8 +2193,8 @@
       <c r="I9" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="J9" s="37" t="s">
-        <v>220</v>
+      <c r="J9" s="27" t="s">
+        <v>219</v>
       </c>
       <c r="K9" s="12"/>
       <c r="L9" s="10"/>
@@ -2171,7 +2210,7 @@
         <v>134</v>
       </c>
       <c r="Q9" s="15" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="R9" s="17"/>
       <c r="S9" s="15">
@@ -2185,7 +2224,7 @@
         <v>176</v>
       </c>
       <c r="V9" s="15" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="W9" s="12"/>
     </row>
@@ -2202,7 +2241,7 @@
         <v>54</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="F10" s="12"/>
       <c r="G10" s="15">
@@ -2216,7 +2255,7 @@
         <v>93</v>
       </c>
       <c r="J10" s="15" t="s">
-        <v>373</v>
+        <v>364</v>
       </c>
       <c r="K10" s="12"/>
       <c r="L10" s="10"/>
@@ -2232,7 +2271,7 @@
         <v>135</v>
       </c>
       <c r="Q10" s="15" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="R10" s="17"/>
       <c r="S10" s="15">
@@ -2245,8 +2284,8 @@
       <c r="U10" s="20" t="s">
         <v>177</v>
       </c>
-      <c r="V10" s="15" t="s">
-        <v>318</v>
+      <c r="V10" s="39" t="s">
+        <v>379</v>
       </c>
       <c r="W10" s="12"/>
     </row>
@@ -2263,7 +2302,7 @@
         <v>55</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F11" s="12"/>
       <c r="G11" s="15">
@@ -2277,7 +2316,7 @@
         <v>94</v>
       </c>
       <c r="J11" s="15" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
       <c r="K11" s="12"/>
       <c r="L11" s="10"/>
@@ -2293,7 +2332,7 @@
         <v>136</v>
       </c>
       <c r="Q11" s="15" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="R11" s="17"/>
       <c r="S11" s="15">
@@ -2306,8 +2345,8 @@
       <c r="U11" s="20" t="s">
         <v>178</v>
       </c>
-      <c r="V11" s="15" t="s">
-        <v>303</v>
+      <c r="V11" s="39" t="s">
+        <v>380</v>
       </c>
       <c r="W11" s="12"/>
     </row>
@@ -2324,7 +2363,7 @@
         <v>56</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>374</v>
+        <v>365</v>
       </c>
       <c r="F12" s="12"/>
       <c r="G12" s="15">
@@ -2338,7 +2377,7 @@
         <v>95</v>
       </c>
       <c r="J12" s="15" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
       <c r="K12" s="12"/>
       <c r="L12" s="10"/>
@@ -2354,7 +2393,7 @@
         <v>137</v>
       </c>
       <c r="Q12" s="15" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="R12" s="17"/>
       <c r="S12" s="15">
@@ -2367,8 +2406,8 @@
       <c r="U12" s="20" t="s">
         <v>179</v>
       </c>
-      <c r="V12" s="15" t="s">
-        <v>291</v>
+      <c r="V12" s="39" t="s">
+        <v>381</v>
       </c>
       <c r="W12" s="12"/>
     </row>
@@ -2385,7 +2424,7 @@
         <v>57</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>361</v>
+        <v>352</v>
       </c>
       <c r="F13" s="12"/>
       <c r="G13" s="15">
@@ -2399,7 +2438,7 @@
         <v>96</v>
       </c>
       <c r="J13" s="15" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
       <c r="K13" s="12"/>
       <c r="L13" s="10"/>
@@ -2415,7 +2454,7 @@
         <v>138</v>
       </c>
       <c r="Q13" s="15" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="R13" s="17"/>
       <c r="S13" s="15">
@@ -2428,8 +2467,8 @@
       <c r="U13" s="20" t="s">
         <v>180</v>
       </c>
-      <c r="V13" s="15" t="s">
-        <v>277</v>
+      <c r="V13" s="39" t="s">
+        <v>382</v>
       </c>
       <c r="W13" s="12"/>
     </row>
@@ -2445,8 +2484,8 @@
       <c r="D14" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="E14" s="37" t="s">
-        <v>348</v>
+      <c r="E14" s="27" t="s">
+        <v>339</v>
       </c>
       <c r="F14" s="12"/>
       <c r="G14" s="15">
@@ -2460,7 +2499,7 @@
         <v>97</v>
       </c>
       <c r="J14" s="15" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
       <c r="K14" s="12"/>
       <c r="L14" s="10"/>
@@ -2476,7 +2515,7 @@
         <v>139</v>
       </c>
       <c r="Q14" s="15" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="R14" s="17"/>
       <c r="S14" s="15">
@@ -2489,8 +2528,8 @@
       <c r="U14" s="20" t="s">
         <v>181</v>
       </c>
-      <c r="V14" s="15" t="s">
-        <v>263</v>
+      <c r="V14" s="39" t="s">
+        <v>383</v>
       </c>
       <c r="W14" s="12"/>
     </row>
@@ -2507,7 +2546,7 @@
         <v>59</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="F15" s="12"/>
       <c r="G15" s="15">
@@ -2521,7 +2560,7 @@
         <v>98</v>
       </c>
       <c r="J15" s="15" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="K15" s="12"/>
       <c r="L15" s="10"/>
@@ -2537,7 +2576,7 @@
         <v>140</v>
       </c>
       <c r="Q15" s="15" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="R15" s="17"/>
       <c r="S15" s="15">
@@ -2550,8 +2589,8 @@
       <c r="U15" s="20" t="s">
         <v>182</v>
       </c>
-      <c r="V15" s="15" t="s">
-        <v>249</v>
+      <c r="V15" s="39" t="s">
+        <v>384</v>
       </c>
       <c r="W15" s="12"/>
     </row>
@@ -2568,7 +2607,7 @@
         <v>60</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="F16" s="12"/>
       <c r="G16" s="15">
@@ -2582,7 +2621,7 @@
         <v>99</v>
       </c>
       <c r="J16" s="15" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="K16" s="12"/>
       <c r="L16" s="10"/>
@@ -2598,7 +2637,7 @@
         <v>141</v>
       </c>
       <c r="Q16" s="15" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="R16" s="17"/>
       <c r="S16" s="15">
@@ -2611,8 +2650,8 @@
       <c r="U16" s="20" t="s">
         <v>183</v>
       </c>
-      <c r="V16" s="15" t="s">
-        <v>236</v>
+      <c r="V16" s="39" t="s">
+        <v>385</v>
       </c>
       <c r="W16" s="12"/>
     </row>
@@ -2629,7 +2668,7 @@
         <v>61</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="F17" s="12"/>
       <c r="G17" s="15">
@@ -2643,7 +2682,7 @@
         <v>100</v>
       </c>
       <c r="J17" s="15" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="K17" s="12"/>
       <c r="L17" s="10"/>
@@ -2659,7 +2698,7 @@
         <v>142</v>
       </c>
       <c r="Q17" s="15" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="R17" s="17"/>
       <c r="S17" s="15">
@@ -2672,8 +2711,8 @@
       <c r="U17" s="20" t="s">
         <v>184</v>
       </c>
-      <c r="V17" s="15" t="s">
-        <v>223</v>
+      <c r="V17" s="39" t="s">
+        <v>386</v>
       </c>
       <c r="W17" s="12"/>
     </row>
@@ -2690,7 +2729,7 @@
         <v>62</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="F18" s="12"/>
       <c r="G18" s="15">
@@ -2704,7 +2743,7 @@
         <v>101</v>
       </c>
       <c r="J18" s="15" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="K18" s="12"/>
       <c r="L18" s="10"/>
@@ -2720,7 +2759,7 @@
         <v>143</v>
       </c>
       <c r="Q18" s="15" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="R18" s="17"/>
       <c r="S18" s="15">
@@ -2734,7 +2773,7 @@
         <v>185</v>
       </c>
       <c r="V18" s="15" t="s">
-        <v>375</v>
+        <v>366</v>
       </c>
       <c r="W18" s="12"/>
     </row>
@@ -2751,7 +2790,7 @@
         <v>63</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="F19" s="12"/>
       <c r="G19" s="15">
@@ -2765,7 +2804,7 @@
         <v>102</v>
       </c>
       <c r="J19" s="15" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="K19" s="12"/>
       <c r="L19" s="10"/>
@@ -2781,7 +2820,7 @@
         <v>144</v>
       </c>
       <c r="Q19" s="15" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="R19" s="17"/>
       <c r="S19" s="15">
@@ -2795,7 +2834,7 @@
         <v>186</v>
       </c>
       <c r="V19" s="15" t="s">
-        <v>362</v>
+        <v>353</v>
       </c>
       <c r="W19" s="12"/>
     </row>
@@ -2923,7 +2962,7 @@
         <v>64</v>
       </c>
       <c r="E23" s="15" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="F23" s="12"/>
       <c r="G23" s="15">
@@ -2937,7 +2976,7 @@
         <v>103</v>
       </c>
       <c r="J23" s="15" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="K23" s="12"/>
       <c r="L23" s="10"/>
@@ -2953,7 +2992,7 @@
         <v>145</v>
       </c>
       <c r="Q23" s="15" t="s">
-        <v>376</v>
+        <v>367</v>
       </c>
       <c r="R23" s="17"/>
       <c r="S23" s="15">
@@ -2967,7 +3006,7 @@
         <v>187</v>
       </c>
       <c r="V23" s="15" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
       <c r="W23" s="12"/>
     </row>
@@ -2984,7 +3023,7 @@
         <v>67</v>
       </c>
       <c r="E24" s="15" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="F24" s="12"/>
       <c r="G24" s="15">
@@ -2998,7 +3037,7 @@
         <v>104</v>
       </c>
       <c r="J24" s="15" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="K24" s="12"/>
       <c r="L24" s="10"/>
@@ -3014,7 +3053,7 @@
         <v>146</v>
       </c>
       <c r="Q24" s="15" t="s">
-        <v>363</v>
+        <v>354</v>
       </c>
       <c r="R24" s="17"/>
       <c r="S24" s="15">
@@ -3028,7 +3067,7 @@
         <v>188</v>
       </c>
       <c r="V24" s="15" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="W24" s="12"/>
     </row>
@@ -3045,7 +3084,7 @@
         <v>66</v>
       </c>
       <c r="E25" s="15" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="F25" s="12"/>
       <c r="G25" s="15">
@@ -3059,7 +3098,7 @@
         <v>105</v>
       </c>
       <c r="J25" s="15" t="s">
-        <v>377</v>
+        <v>368</v>
       </c>
       <c r="K25" s="12"/>
       <c r="L25" s="10"/>
@@ -3075,7 +3114,7 @@
         <v>147</v>
       </c>
       <c r="Q25" s="15" t="s">
-        <v>350</v>
+        <v>341</v>
       </c>
       <c r="R25" s="17"/>
       <c r="S25" s="15">
@@ -3089,7 +3128,7 @@
         <v>189</v>
       </c>
       <c r="V25" s="15" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
       <c r="W25" s="12"/>
     </row>
@@ -3106,7 +3145,7 @@
         <v>68</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F26" s="12"/>
       <c r="G26" s="15">
@@ -3120,7 +3159,7 @@
         <v>106</v>
       </c>
       <c r="J26" s="15" t="s">
-        <v>364</v>
+        <v>355</v>
       </c>
       <c r="K26" s="12"/>
       <c r="L26" s="10"/>
@@ -3136,7 +3175,7 @@
         <v>148</v>
       </c>
       <c r="Q26" s="15" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
       <c r="R26" s="17"/>
       <c r="S26" s="15">
@@ -3150,7 +3189,7 @@
         <v>190</v>
       </c>
       <c r="V26" s="15" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="W26" s="12"/>
     </row>
@@ -3167,7 +3206,7 @@
         <v>69</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="F27" s="12"/>
       <c r="G27" s="15">
@@ -3181,7 +3220,7 @@
         <v>107</v>
       </c>
       <c r="J27" s="15" t="s">
-        <v>351</v>
+        <v>342</v>
       </c>
       <c r="K27" s="12"/>
       <c r="L27" s="10"/>
@@ -3197,7 +3236,7 @@
         <v>149</v>
       </c>
       <c r="Q27" s="15" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="R27" s="17"/>
       <c r="S27" s="15">
@@ -3211,7 +3250,7 @@
         <v>191</v>
       </c>
       <c r="V27" s="15" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="W27" s="12"/>
     </row>
@@ -3228,7 +3267,7 @@
         <v>70</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>365</v>
+        <v>356</v>
       </c>
       <c r="F28" s="12"/>
       <c r="G28" s="15">
@@ -3242,7 +3281,7 @@
         <v>108</v>
       </c>
       <c r="J28" s="15" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
       <c r="K28" s="12"/>
       <c r="L28" s="10"/>
@@ -3258,7 +3297,7 @@
         <v>150</v>
       </c>
       <c r="Q28" s="15" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="R28" s="17"/>
       <c r="S28" s="15">
@@ -3272,7 +3311,7 @@
         <v>192</v>
       </c>
       <c r="V28" s="15" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="W28" s="12"/>
     </row>
@@ -3289,7 +3328,7 @@
         <v>71</v>
       </c>
       <c r="E29" s="15" t="s">
-        <v>352</v>
+        <v>343</v>
       </c>
       <c r="F29" s="12"/>
       <c r="G29" s="15">
@@ -3303,7 +3342,7 @@
         <v>109</v>
       </c>
       <c r="J29" s="15" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="K29" s="12"/>
       <c r="L29" s="10"/>
@@ -3319,7 +3358,7 @@
         <v>151</v>
       </c>
       <c r="Q29" s="15" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="R29" s="17"/>
       <c r="S29" s="15">
@@ -3333,7 +3372,7 @@
         <v>193</v>
       </c>
       <c r="V29" s="15" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="W29" s="12"/>
     </row>
@@ -3350,7 +3389,7 @@
         <v>72</v>
       </c>
       <c r="E30" s="15" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="F30" s="12"/>
       <c r="G30" s="15">
@@ -3364,7 +3403,7 @@
         <v>110</v>
       </c>
       <c r="J30" s="15" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="K30" s="12"/>
       <c r="L30" s="10"/>
@@ -3380,7 +3419,7 @@
         <v>152</v>
       </c>
       <c r="Q30" s="15" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="R30" s="17"/>
       <c r="S30" s="15">
@@ -3394,7 +3433,7 @@
         <v>194</v>
       </c>
       <c r="V30" s="15" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="W30" s="12"/>
     </row>
@@ -3411,7 +3450,7 @@
         <v>73</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
       <c r="F31" s="12"/>
       <c r="G31" s="15">
@@ -3425,7 +3464,7 @@
         <v>111</v>
       </c>
       <c r="J31" s="15" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="K31" s="12"/>
       <c r="L31" s="10"/>
@@ -3441,7 +3480,7 @@
         <v>153</v>
       </c>
       <c r="Q31" s="15" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="R31" s="17"/>
       <c r="S31" s="15">
@@ -3455,7 +3494,7 @@
         <v>195</v>
       </c>
       <c r="V31" s="15" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="W31" s="12"/>
     </row>
@@ -3472,7 +3511,7 @@
         <v>74</v>
       </c>
       <c r="E32" s="15" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="F32" s="12"/>
       <c r="G32" s="15">
@@ -3486,7 +3525,7 @@
         <v>112</v>
       </c>
       <c r="J32" s="15" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="K32" s="12"/>
       <c r="L32" s="10"/>
@@ -3502,7 +3541,7 @@
         <v>154</v>
       </c>
       <c r="Q32" s="15" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="R32" s="17"/>
       <c r="S32" s="15">
@@ -3516,7 +3555,7 @@
         <v>196</v>
       </c>
       <c r="V32" s="15" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="W32" s="12"/>
     </row>
@@ -3533,7 +3572,7 @@
         <v>75</v>
       </c>
       <c r="E33" s="15" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="F33" s="12"/>
       <c r="G33" s="15">
@@ -3547,7 +3586,7 @@
         <v>113</v>
       </c>
       <c r="J33" s="15" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="K33" s="12"/>
       <c r="L33" s="10"/>
@@ -3563,7 +3602,7 @@
         <v>155</v>
       </c>
       <c r="Q33" s="15" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="R33" s="17"/>
       <c r="S33" s="15">
@@ -3577,7 +3616,7 @@
         <v>197</v>
       </c>
       <c r="V33" s="15" t="s">
-        <v>379</v>
+        <v>370</v>
       </c>
       <c r="W33" s="12"/>
     </row>
@@ -3594,7 +3633,7 @@
         <v>76</v>
       </c>
       <c r="E34" s="15" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="F34" s="12"/>
       <c r="G34" s="15">
@@ -3608,7 +3647,7 @@
         <v>114</v>
       </c>
       <c r="J34" s="15" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="K34" s="12"/>
       <c r="L34" s="10"/>
@@ -3624,7 +3663,7 @@
         <v>156</v>
       </c>
       <c r="Q34" s="15" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="R34" s="17"/>
       <c r="S34" s="15">
@@ -3638,7 +3677,7 @@
         <v>198</v>
       </c>
       <c r="V34" s="15" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="W34" s="12"/>
     </row>
@@ -3655,7 +3694,7 @@
         <v>77</v>
       </c>
       <c r="E35" s="15" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="F35" s="12"/>
       <c r="G35" s="15">
@@ -3669,7 +3708,7 @@
         <v>115</v>
       </c>
       <c r="J35" s="15" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="K35" s="12"/>
       <c r="L35" s="10"/>
@@ -3685,7 +3724,7 @@
         <v>157</v>
       </c>
       <c r="Q35" s="15" t="s">
-        <v>380</v>
+        <v>371</v>
       </c>
       <c r="R35" s="17"/>
       <c r="S35" s="15">
@@ -3699,7 +3738,7 @@
         <v>199</v>
       </c>
       <c r="V35" s="15" t="s">
-        <v>353</v>
+        <v>344</v>
       </c>
       <c r="W35" s="12"/>
     </row>
@@ -3716,7 +3755,7 @@
         <v>78</v>
       </c>
       <c r="E36" s="15" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="F36" s="12"/>
       <c r="G36" s="15">
@@ -3730,7 +3769,7 @@
         <v>116</v>
       </c>
       <c r="J36" s="15" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="K36" s="12"/>
       <c r="L36" s="10"/>
@@ -3746,7 +3785,7 @@
         <v>158</v>
       </c>
       <c r="Q36" s="15" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
       <c r="R36" s="17"/>
       <c r="S36" s="15">
@@ -3760,7 +3799,7 @@
         <v>200</v>
       </c>
       <c r="V36" s="15" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="W36" s="12"/>
     </row>
@@ -3888,7 +3927,7 @@
         <v>79</v>
       </c>
       <c r="E40" s="15" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="F40" s="12"/>
       <c r="G40" s="15">
@@ -3902,7 +3941,7 @@
         <v>117</v>
       </c>
       <c r="J40" s="15" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="K40" s="12"/>
       <c r="L40" s="10"/>
@@ -3918,7 +3957,7 @@
         <v>159</v>
       </c>
       <c r="Q40" s="15" t="s">
-        <v>354</v>
+        <v>345</v>
       </c>
       <c r="R40" s="12"/>
       <c r="S40" s="15">
@@ -3932,7 +3971,7 @@
         <v>201</v>
       </c>
       <c r="V40" s="15" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="W40" s="12"/>
     </row>
@@ -3949,7 +3988,7 @@
         <v>80</v>
       </c>
       <c r="E41" s="15" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F41" s="12"/>
       <c r="G41" s="15">
@@ -3963,7 +4002,7 @@
         <v>118</v>
       </c>
       <c r="J41" s="15" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="K41" s="12"/>
       <c r="L41" s="10"/>
@@ -3979,7 +4018,7 @@
         <v>160</v>
       </c>
       <c r="Q41" s="15" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="R41" s="12"/>
       <c r="S41" s="15">
@@ -3993,7 +4032,7 @@
         <v>202</v>
       </c>
       <c r="V41" s="15" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="W41" s="12"/>
     </row>
@@ -4010,7 +4049,7 @@
         <v>81</v>
       </c>
       <c r="E42" s="15" t="s">
-        <v>381</v>
+        <v>372</v>
       </c>
       <c r="F42" s="12"/>
       <c r="G42" s="15">
@@ -4024,7 +4063,7 @@
         <v>119</v>
       </c>
       <c r="J42" s="15" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="K42" s="12"/>
       <c r="L42" s="10"/>
@@ -4040,7 +4079,7 @@
         <v>161</v>
       </c>
       <c r="Q42" s="15" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="R42" s="12"/>
       <c r="S42" s="15">
@@ -4054,7 +4093,7 @@
         <v>203</v>
       </c>
       <c r="V42" s="15" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="W42" s="12"/>
     </row>
@@ -4071,7 +4110,7 @@
         <v>82</v>
       </c>
       <c r="E43" s="15" t="s">
-        <v>368</v>
+        <v>359</v>
       </c>
       <c r="F43" s="12"/>
       <c r="G43" s="15">
@@ -4085,7 +4124,7 @@
         <v>120</v>
       </c>
       <c r="J43" s="15" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="K43" s="12"/>
       <c r="L43" s="10"/>
@@ -4101,7 +4140,7 @@
         <v>162</v>
       </c>
       <c r="Q43" s="15" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="R43" s="12"/>
       <c r="S43" s="15">
@@ -4115,7 +4154,7 @@
         <v>204</v>
       </c>
       <c r="V43" s="15" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="W43" s="12"/>
     </row>
@@ -4132,7 +4171,7 @@
         <v>83</v>
       </c>
       <c r="E44" s="15" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
       <c r="F44" s="12"/>
       <c r="G44" s="15">
@@ -4146,7 +4185,7 @@
         <v>121</v>
       </c>
       <c r="J44" s="15" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="K44" s="12"/>
       <c r="L44" s="10"/>
@@ -4162,7 +4201,7 @@
         <v>163</v>
       </c>
       <c r="Q44" s="15" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="R44" s="12"/>
       <c r="S44" s="15">
@@ -4176,7 +4215,7 @@
         <v>205</v>
       </c>
       <c r="V44" s="15" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="W44" s="12"/>
     </row>
@@ -4193,7 +4232,7 @@
         <v>84</v>
       </c>
       <c r="E45" s="15" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="F45" s="12"/>
       <c r="G45" s="15">
@@ -4207,7 +4246,7 @@
         <v>122</v>
       </c>
       <c r="J45" s="15" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="K45" s="12"/>
       <c r="L45" s="10"/>
@@ -4223,7 +4262,7 @@
         <v>164</v>
       </c>
       <c r="Q45" s="15" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="R45" s="12"/>
       <c r="S45" s="15">
@@ -4237,7 +4276,7 @@
         <v>206</v>
       </c>
       <c r="V45" s="15" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="W45" s="12"/>
     </row>
@@ -4254,7 +4293,7 @@
         <v>85</v>
       </c>
       <c r="E46" s="15" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="F46" s="12"/>
       <c r="G46" s="15">
@@ -4268,7 +4307,7 @@
         <v>123</v>
       </c>
       <c r="J46" s="15" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="K46" s="12"/>
       <c r="L46" s="10"/>
@@ -4284,7 +4323,7 @@
         <v>165</v>
       </c>
       <c r="Q46" s="15" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="R46" s="12"/>
       <c r="S46" s="15">
@@ -4298,7 +4337,7 @@
         <v>207</v>
       </c>
       <c r="V46" s="15" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="W46" s="12"/>
     </row>
@@ -4315,7 +4354,7 @@
         <v>65</v>
       </c>
       <c r="E47" s="15" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="F47" s="12"/>
       <c r="G47" s="15">
@@ -4329,7 +4368,7 @@
         <v>124</v>
       </c>
       <c r="J47" s="15" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="K47" s="12"/>
       <c r="L47" s="10"/>
@@ -4345,7 +4384,7 @@
         <v>166</v>
       </c>
       <c r="Q47" s="15" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="R47" s="12"/>
       <c r="S47" s="15">
@@ -4359,7 +4398,7 @@
         <v>208</v>
       </c>
       <c r="V47" s="15" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="W47" s="12"/>
     </row>
@@ -4376,7 +4415,7 @@
         <v>86</v>
       </c>
       <c r="E48" s="15" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="F48" s="12"/>
       <c r="G48" s="15">
@@ -4390,7 +4429,7 @@
         <v>125</v>
       </c>
       <c r="J48" s="15" t="s">
-        <v>382</v>
+        <v>373</v>
       </c>
       <c r="K48" s="12"/>
       <c r="L48" s="10"/>
@@ -4406,7 +4445,7 @@
         <v>167</v>
       </c>
       <c r="Q48" s="26" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="R48" s="12"/>
       <c r="S48" s="15">
@@ -4420,7 +4459,7 @@
         <v>209</v>
       </c>
       <c r="V48" s="15" t="s">
-        <v>383</v>
+        <v>374</v>
       </c>
       <c r="W48" s="12"/>
     </row>
@@ -4437,7 +4476,7 @@
         <v>87</v>
       </c>
       <c r="E49" s="15" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="F49" s="12"/>
       <c r="G49" s="15">
@@ -4451,7 +4490,7 @@
         <v>126</v>
       </c>
       <c r="J49" s="15" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="K49" s="12"/>
       <c r="L49" s="10"/>
@@ -4467,7 +4506,7 @@
         <v>168</v>
       </c>
       <c r="Q49" s="26" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="R49" s="12"/>
       <c r="S49" s="15">
@@ -4481,7 +4520,7 @@
         <v>210</v>
       </c>
       <c r="V49" s="15" t="s">
-        <v>370</v>
+        <v>361</v>
       </c>
       <c r="W49" s="12"/>
     </row>
@@ -4498,7 +4537,7 @@
         <v>88</v>
       </c>
       <c r="E50" s="15" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="F50" s="12"/>
       <c r="G50" s="15">
@@ -4512,7 +4551,7 @@
         <v>127</v>
       </c>
       <c r="J50" s="15" t="s">
-        <v>356</v>
+        <v>347</v>
       </c>
       <c r="K50" s="12"/>
       <c r="L50" s="10"/>
@@ -4528,7 +4567,7 @@
         <v>169</v>
       </c>
       <c r="Q50" s="15" t="s">
-        <v>384</v>
+        <v>375</v>
       </c>
       <c r="R50" s="12"/>
       <c r="S50" s="15">
@@ -4542,7 +4581,7 @@
         <v>211</v>
       </c>
       <c r="V50" s="15" t="s">
-        <v>357</v>
+        <v>348</v>
       </c>
       <c r="W50" s="12"/>
     </row>
@@ -4559,7 +4598,7 @@
         <v>49</v>
       </c>
       <c r="E51" s="15" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="F51" s="12"/>
       <c r="G51" s="15">
@@ -4573,7 +4612,7 @@
         <v>128</v>
       </c>
       <c r="J51" s="15" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="K51" s="12"/>
       <c r="L51" s="10"/>
@@ -4589,7 +4628,7 @@
         <v>170</v>
       </c>
       <c r="Q51" s="15" t="s">
-        <v>371</v>
+        <v>362</v>
       </c>
       <c r="R51" s="12"/>
       <c r="S51" s="15">
@@ -4603,7 +4642,7 @@
         <v>212</v>
       </c>
       <c r="V51" s="15" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="W51" s="12"/>
     </row>
@@ -4620,7 +4659,7 @@
         <v>48</v>
       </c>
       <c r="E52" s="15" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="F52" s="12"/>
       <c r="G52" s="15">
@@ -4634,7 +4673,7 @@
         <v>129</v>
       </c>
       <c r="J52" s="15" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="K52" s="12"/>
       <c r="L52" s="10"/>
@@ -4650,7 +4689,7 @@
         <v>171</v>
       </c>
       <c r="Q52" s="15" t="s">
-        <v>358</v>
+        <v>349</v>
       </c>
       <c r="R52" s="12"/>
       <c r="S52" s="15">
@@ -4664,7 +4703,7 @@
         <v>213</v>
       </c>
       <c r="V52" s="15" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="W52" s="12"/>
     </row>
@@ -4679,8 +4718,8 @@
       <c r="D53" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="E53" s="37" t="s">
-        <v>233</v>
+      <c r="E53" s="27" t="s">
+        <v>231</v>
       </c>
       <c r="F53" s="12"/>
       <c r="G53" s="15">
@@ -4694,7 +4733,7 @@
         <v>130</v>
       </c>
       <c r="J53" s="15" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="K53" s="12"/>
       <c r="L53" s="10"/>
@@ -4710,7 +4749,7 @@
         <v>172</v>
       </c>
       <c r="Q53" s="15" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
       <c r="R53" s="12"/>
       <c r="S53" s="15">
@@ -4724,7 +4763,7 @@
         <v>214</v>
       </c>
       <c r="V53" s="15" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="W53" s="12"/>
     </row>
@@ -4776,10 +4815,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:U39"/>
+  <dimension ref="A1:U40"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K38" sqref="K38"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4789,30 +4828,30 @@
   <sheetData>
     <row r="1" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="34"/>
+      <c r="C1" s="36"/>
       <c r="D1" s="2"/>
-      <c r="E1" s="33" t="s">
+      <c r="E1" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="34"/>
+      <c r="F1" s="36"/>
       <c r="G1" s="2"/>
-      <c r="H1" s="33" t="s">
+      <c r="H1" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="34"/>
+      <c r="I1" s="36"/>
       <c r="J1" s="2"/>
-      <c r="K1" s="36" t="s">
+      <c r="K1" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="34"/>
+      <c r="L1" s="36"/>
       <c r="M1" s="2"/>
-      <c r="N1" s="33" t="s">
+      <c r="N1" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="O1" s="34"/>
+      <c r="O1" s="36"/>
       <c r="P1" s="2"/>
     </row>
     <row r="2" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5093,7 +5132,6 @@
       </c>
       <c r="P8" s="2"/>
       <c r="S8" s="22"/>
-      <c r="U8" s="22"/>
     </row>
     <row r="9" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
@@ -5133,7 +5171,6 @@
       </c>
       <c r="P9" s="2"/>
       <c r="S9" s="22"/>
-      <c r="U9" s="22"/>
     </row>
     <row r="10" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
@@ -5173,7 +5210,6 @@
       </c>
       <c r="P10" s="2"/>
       <c r="S10" s="22"/>
-      <c r="U10" s="22"/>
     </row>
     <row r="11" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
@@ -5193,37 +5229,35 @@
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
       <c r="S11" s="22"/>
-      <c r="U11" s="22"/>
     </row>
     <row r="12" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
-      <c r="B12" s="35" t="s">
+      <c r="B12" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="34"/>
+      <c r="C12" s="36"/>
       <c r="D12" s="2"/>
-      <c r="E12" s="33" t="s">
+      <c r="E12" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="34"/>
+      <c r="F12" s="36"/>
       <c r="G12" s="2"/>
-      <c r="H12" s="33" t="s">
+      <c r="H12" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="I12" s="34"/>
+      <c r="I12" s="36"/>
       <c r="J12" s="2"/>
-      <c r="K12" s="36" t="s">
+      <c r="K12" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="L12" s="36"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="L12" s="34"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="33" t="s">
-        <v>24</v>
-      </c>
-      <c r="O12" s="34"/>
+      <c r="O12" s="36"/>
       <c r="P12" s="2"/>
       <c r="S12" s="22"/>
-      <c r="U12" s="22"/>
     </row>
     <row r="13" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
@@ -5261,9 +5295,8 @@
       <c r="O13" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="P13" s="2"/>
+      <c r="P13" s="4"/>
       <c r="S13" s="23"/>
-      <c r="U13" s="23"/>
     </row>
     <row r="14" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
@@ -5289,21 +5322,20 @@
       </c>
       <c r="J14" s="4"/>
       <c r="K14" s="5">
-        <v>95</v>
+        <v>163</v>
       </c>
       <c r="L14" s="5" t="s">
         <v>11</v>
       </c>
       <c r="M14" s="4"/>
       <c r="N14" s="5">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="O14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="P14" s="2"/>
+      <c r="P14" s="4"/>
       <c r="S14" s="22"/>
-      <c r="U14" s="22"/>
     </row>
     <row r="15" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
@@ -5329,21 +5361,21 @@
       </c>
       <c r="J15" s="4"/>
       <c r="K15" s="5">
-        <v>94</v>
+        <f t="shared" ref="K15:K21" si="0">K14-1</f>
+        <v>162</v>
       </c>
       <c r="L15" s="5" t="s">
         <v>12</v>
       </c>
       <c r="M15" s="4"/>
       <c r="N15" s="5">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="O15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="P15" s="2"/>
+      <c r="P15" s="4"/>
       <c r="S15" s="22"/>
-      <c r="U15" s="22"/>
     </row>
     <row r="16" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
@@ -5366,24 +5398,24 @@
         <v>13</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="K16" s="5">
-        <v>93</v>
+        <f t="shared" si="0"/>
+        <v>161</v>
       </c>
       <c r="L16" s="5" t="s">
         <v>13</v>
       </c>
       <c r="M16" s="4"/>
       <c r="N16" s="5">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="O16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="P16" s="2"/>
+      <c r="P16" s="4"/>
       <c r="S16" s="22"/>
-      <c r="U16" s="22"/>
     </row>
     <row r="17" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
@@ -5406,24 +5438,24 @@
         <v>14</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="K17" s="5">
-        <v>92</v>
+        <f t="shared" si="0"/>
+        <v>160</v>
       </c>
       <c r="L17" s="5" t="s">
         <v>14</v>
       </c>
       <c r="M17" s="4"/>
       <c r="N17" s="5">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="O17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="P17" s="2"/>
+      <c r="P17" s="4"/>
       <c r="S17" s="22"/>
-      <c r="U17" s="22"/>
     </row>
     <row r="18" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
@@ -5449,19 +5481,20 @@
       </c>
       <c r="J18" s="4"/>
       <c r="K18" s="5">
-        <v>91</v>
+        <f t="shared" si="0"/>
+        <v>159</v>
       </c>
       <c r="L18" s="5" t="s">
         <v>15</v>
       </c>
       <c r="M18" s="4"/>
       <c r="N18" s="5">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="O18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="P18" s="2"/>
+      <c r="P18" s="4"/>
       <c r="S18" s="22"/>
       <c r="U18" s="22"/>
     </row>
@@ -5489,19 +5522,20 @@
       </c>
       <c r="J19" s="4"/>
       <c r="K19" s="5">
-        <v>90</v>
+        <f t="shared" si="0"/>
+        <v>158</v>
       </c>
       <c r="L19" s="5" t="s">
         <v>16</v>
       </c>
       <c r="M19" s="4"/>
       <c r="N19" s="5">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="O19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="P19" s="2"/>
+      <c r="P19" s="4"/>
       <c r="S19" s="22"/>
       <c r="U19" s="22"/>
     </row>
@@ -5528,20 +5562,21 @@
         <v>17</v>
       </c>
       <c r="J20" s="4"/>
-      <c r="K20" s="5"/>
+      <c r="K20" s="5">
+        <f t="shared" si="0"/>
+        <v>157</v>
+      </c>
       <c r="L20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="M20" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="N20" s="5">
-        <v>101</v>
-      </c>
+      <c r="M20" s="4"/>
+      <c r="N20" s="5"/>
       <c r="O20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="P20" s="2"/>
+      <c r="P20" s="4" t="s">
+        <v>215</v>
+      </c>
       <c r="S20" s="22"/>
       <c r="U20" s="22"/>
     </row>
@@ -5568,20 +5603,21 @@
         <v>18</v>
       </c>
       <c r="J21" s="4"/>
-      <c r="K21" s="5"/>
+      <c r="K21" s="5">
+        <f t="shared" si="0"/>
+        <v>156</v>
+      </c>
       <c r="L21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="M21" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="N21" s="5">
-        <v>100</v>
-      </c>
+      <c r="M21" s="4"/>
+      <c r="N21" s="5"/>
       <c r="O21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="P21" s="2"/>
+      <c r="P21" s="4" t="s">
+        <v>215</v>
+      </c>
       <c r="S21" s="22"/>
       <c r="U21" s="22"/>
     </row>
@@ -5607,30 +5643,30 @@
     </row>
     <row r="23" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
-      <c r="B23" s="33" t="s">
+      <c r="B23" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="36"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="34"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="33" t="s">
+      <c r="F23" s="36"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="F23" s="34"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="36" t="s">
+      <c r="I23" s="40"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="I23" s="34"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="33" t="s">
+      <c r="L23" s="41"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="L23" s="34"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="33" t="s">
-        <v>215</v>
-      </c>
-      <c r="O23" s="34"/>
+      <c r="O23" s="40"/>
       <c r="P23" s="2"/>
       <c r="Q23" s="6"/>
       <c r="S23" s="22"/>
@@ -5680,35 +5716,35 @@
     <row r="25" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
       <c r="B25" s="5">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="5">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G25" s="4"/>
       <c r="H25" s="5">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="I25" s="5" t="s">
         <v>11</v>
       </c>
       <c r="J25" s="4"/>
       <c r="K25" s="5">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="L25" s="5" t="s">
         <v>11</v>
       </c>
       <c r="M25" s="4"/>
       <c r="N25" s="5">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="O25" s="5" t="s">
         <v>11</v>
@@ -5721,36 +5757,35 @@
     <row r="26" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4"/>
       <c r="B26" s="5">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="5">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>12</v>
       </c>
       <c r="G26" s="4"/>
       <c r="H26" s="5">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="I26" s="5" t="s">
         <v>12</v>
       </c>
       <c r="J26" s="4"/>
       <c r="K26" s="5">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="L26" s="5" t="s">
         <v>12</v>
       </c>
       <c r="M26" s="4"/>
       <c r="N26" s="5">
-        <f t="shared" ref="N26:N32" si="0">N25-1</f>
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="O26" s="5" t="s">
         <v>12</v>
@@ -5763,36 +5798,35 @@
     <row r="27" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4"/>
       <c r="B27" s="5">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="5">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>13</v>
       </c>
       <c r="G27" s="4"/>
       <c r="H27" s="5">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="I27" s="5" t="s">
         <v>13</v>
       </c>
       <c r="J27" s="4"/>
       <c r="K27" s="5">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="L27" s="5" t="s">
         <v>13</v>
       </c>
       <c r="M27" s="4"/>
       <c r="N27" s="5">
-        <f t="shared" si="0"/>
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="O27" s="5" t="s">
         <v>13</v>
@@ -5805,36 +5839,35 @@
     <row r="28" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
       <c r="B28" s="5">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D28" s="4"/>
       <c r="E28" s="5">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>14</v>
       </c>
       <c r="G28" s="4"/>
       <c r="H28" s="5">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="I28" s="5" t="s">
         <v>14</v>
       </c>
       <c r="J28" s="4"/>
       <c r="K28" s="5">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="L28" s="5" t="s">
         <v>14</v>
       </c>
       <c r="M28" s="4"/>
       <c r="N28" s="5">
-        <f t="shared" si="0"/>
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="O28" s="5" t="s">
         <v>14</v>
@@ -5847,36 +5880,35 @@
     <row r="29" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4"/>
       <c r="B29" s="5">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="5">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G29" s="4"/>
       <c r="H29" s="5">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="I29" s="5" t="s">
         <v>15</v>
       </c>
       <c r="J29" s="4"/>
       <c r="K29" s="5">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="L29" s="5" t="s">
         <v>15</v>
       </c>
       <c r="M29" s="4"/>
       <c r="N29" s="5">
-        <f t="shared" si="0"/>
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="O29" s="5" t="s">
         <v>15</v>
@@ -5889,36 +5921,35 @@
     <row r="30" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4"/>
       <c r="B30" s="5">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D30" s="4"/>
       <c r="E30" s="5">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>16</v>
       </c>
       <c r="G30" s="4"/>
       <c r="H30" s="5">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="I30" s="5" t="s">
         <v>16</v>
       </c>
       <c r="J30" s="4"/>
       <c r="K30" s="5">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="L30" s="5" t="s">
         <v>16</v>
       </c>
       <c r="M30" s="4"/>
       <c r="N30" s="5">
-        <f t="shared" si="0"/>
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="O30" s="5" t="s">
         <v>16</v>
@@ -5931,36 +5962,35 @@
     <row r="31" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="4"/>
       <c r="B31" s="5">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="5">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>17</v>
       </c>
       <c r="G31" s="4"/>
       <c r="H31" s="5">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="I31" s="5" t="s">
         <v>17</v>
       </c>
       <c r="J31" s="4"/>
       <c r="K31" s="5">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="L31" s="5" t="s">
         <v>17</v>
       </c>
       <c r="M31" s="4"/>
       <c r="N31" s="5">
-        <f t="shared" si="0"/>
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="O31" s="5" t="s">
         <v>17</v>
@@ -5973,36 +6003,35 @@
     <row r="32" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="4"/>
       <c r="B32" s="5">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="5">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>18</v>
       </c>
       <c r="G32" s="4"/>
       <c r="H32" s="5">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="I32" s="5" t="s">
         <v>18</v>
       </c>
       <c r="J32" s="4"/>
       <c r="K32" s="5">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="L32" s="5" t="s">
         <v>18</v>
       </c>
       <c r="M32" s="4"/>
       <c r="N32" s="5">
-        <f t="shared" si="0"/>
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="O32" s="5" t="s">
         <v>18</v>
@@ -6067,15 +6096,27 @@
       <c r="U37" s="21"/>
     </row>
     <row r="38" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K38" s="28" t="s">
+        <v>376</v>
+      </c>
       <c r="S38" s="21"/>
       <c r="U38" s="21"/>
     </row>
     <row r="39" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K39" s="28" t="s">
+        <v>377</v>
+      </c>
       <c r="S39" s="23"/>
       <c r="U39" s="23"/>
     </row>
+    <row r="40" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K40" s="28" t="s">
+        <v>378</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="K12:L12"/>
     <mergeCell ref="N23:O23"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="E1:F1"/>
@@ -6086,7 +6127,6 @@
     <mergeCell ref="E12:F12"/>
     <mergeCell ref="N12:O12"/>
     <mergeCell ref="H12:I12"/>
-    <mergeCell ref="K12:L12"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="E23:F23"/>
     <mergeCell ref="H23:I23"/>
@@ -6115,30 +6155,30 @@
   <sheetData>
     <row r="1" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="34"/>
+      <c r="C1" s="36"/>
       <c r="D1" s="2"/>
-      <c r="E1" s="33" t="s">
+      <c r="E1" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="34"/>
+      <c r="F1" s="36"/>
       <c r="G1" s="2"/>
-      <c r="H1" s="33" t="s">
+      <c r="H1" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="34"/>
+      <c r="I1" s="36"/>
       <c r="J1" s="2"/>
-      <c r="K1" s="36" t="s">
+      <c r="K1" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="34"/>
+      <c r="L1" s="36"/>
       <c r="M1" s="2"/>
-      <c r="N1" s="33" t="s">
+      <c r="N1" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="O1" s="34"/>
+      <c r="O1" s="36"/>
       <c r="P1" s="2"/>
     </row>
     <row r="2" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6347,30 +6387,30 @@
     </row>
     <row r="8" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="34"/>
+      <c r="C8" s="36"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="33" t="s">
+      <c r="E8" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="34"/>
+      <c r="F8" s="36"/>
       <c r="G8" s="2"/>
-      <c r="H8" s="33" t="s">
+      <c r="H8" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="34"/>
+      <c r="I8" s="36"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="36" t="s">
+      <c r="K8" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="L8" s="34"/>
+      <c r="L8" s="36"/>
       <c r="M8" s="2"/>
-      <c r="N8" s="33" t="s">
+      <c r="N8" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="O8" s="34"/>
+      <c r="O8" s="36"/>
       <c r="P8" s="2"/>
       <c r="S8" s="22"/>
       <c r="U8" s="22"/>
@@ -6597,30 +6637,30 @@
     </row>
     <row r="15" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
-      <c r="B15" s="33" t="s">
+      <c r="B15" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="34"/>
+      <c r="C15" s="36"/>
       <c r="D15" s="2"/>
-      <c r="E15" s="33" t="s">
+      <c r="E15" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="F15" s="34"/>
+      <c r="F15" s="36"/>
       <c r="G15" s="2"/>
-      <c r="H15" s="36" t="s">
+      <c r="H15" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="I15" s="34"/>
+      <c r="I15" s="36"/>
       <c r="J15" s="2"/>
-      <c r="K15" s="33" t="s">
+      <c r="K15" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="L15" s="34"/>
+      <c r="L15" s="36"/>
       <c r="M15" s="2"/>
-      <c r="N15" s="33" t="s">
+      <c r="N15" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="O15" s="34"/>
+      <c r="O15" s="36"/>
       <c r="P15" s="2"/>
       <c r="Q15" s="6"/>
       <c r="S15" s="22"/>
@@ -6861,21 +6901,21 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="N1:O1"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="K8:L8"/>
     <mergeCell ref="N8:O8"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="N15:O15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>